<commit_message>
recaqlculo de los resultados, cambios de LSPMW
</commit_message>
<xml_diff>
--- a/codigo_final_organizado/Simulaciones/ARIMA_D/resultados_TEST_DOBLE_MODALIDAD.xlsx
+++ b/codigo_final_organizado/Simulaciones/ARIMA_D/resultados_TEST_DOBLE_MODALIDAD.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pleal\Documents\Unal\Tesis\Codigo\Prediccion_Probabilistica\codigo_final_organizado\Simulaciones\ARIMA_D\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9982650C-9B79-4389-AE39-3D4B766C7B52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87836297-F3FB-495F-8100-99D4B9CEB6EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -79,7 +79,7 @@
     <t>Sieve Bootstrap</t>
   </si>
   <si>
-    <t>ARIMA(0,1,0)</t>
+    <t>ARMA_I(0,1,0)</t>
   </si>
   <si>
     <t>RW</t>
@@ -97,16 +97,16 @@
     <t>CON_DIFF</t>
   </si>
   <si>
-    <t>ARIMA(1,1,0)</t>
+    <t>ARMA_I(1,1,0)</t>
   </si>
   <si>
     <t>AR(1)</t>
   </si>
   <si>
-    <t>ARIMA(0,2,0)</t>
+    <t>ARMA_I(0,2,0)</t>
   </si>
   <si>
-    <t>ARIMA(1,2,0)</t>
+    <t>ARMA_I(1,2,0)</t>
   </si>
 </sst>
 </file>
@@ -472,12 +472,12 @@
   <dimension ref="A1:S105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="2.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.21875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
@@ -578,34 +578,34 @@
         <v>22</v>
       </c>
       <c r="J2">
-        <v>-9.9682370787663341</v>
+        <v>-17.091393172277499</v>
       </c>
       <c r="K2">
-        <v>0.87770555944050499</v>
+        <v>4.0644711692521209</v>
       </c>
       <c r="L2">
-        <v>1.6491829505042339</v>
+        <v>0.63082791979502029</v>
       </c>
       <c r="M2">
-        <v>1.397118171482284</v>
+        <v>4.3268387718076067</v>
       </c>
       <c r="N2">
-        <v>0.28952325706034748</v>
+        <v>0.47968034827952671</v>
       </c>
       <c r="O2">
-        <v>1.377051660941772</v>
+        <v>1.805407274092113</v>
       </c>
       <c r="P2">
-        <v>0.22198955595021569</v>
+        <v>1.714080700021142</v>
       </c>
       <c r="Q2">
-        <v>0.16333311743458259</v>
+        <v>1.392278421166169</v>
       </c>
       <c r="R2">
-        <v>1.4758291984429139</v>
+        <v>0.65328781895416244</v>
       </c>
       <c r="S2">
-        <v>0.23972459673173971</v>
+        <v>0.22856299323609691</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
@@ -637,34 +637,34 @@
         <v>22</v>
       </c>
       <c r="J3">
-        <v>-8.4967451057731775</v>
+        <v>-16.74983762133699</v>
       </c>
       <c r="K3">
-        <v>0.44300331193510362</v>
+        <v>3.7224744388399489</v>
       </c>
       <c r="L3">
-        <v>3.4807191190170812</v>
+        <v>0.58614433175771097</v>
       </c>
       <c r="M3">
-        <v>1.028120854682921</v>
+        <v>4.0589559810611764</v>
       </c>
       <c r="N3">
-        <v>0.97053100618691834</v>
+        <v>0.2259201772414913</v>
       </c>
       <c r="O3">
-        <v>1.5017302467994551</v>
+        <v>1.8067854346893759</v>
       </c>
       <c r="P3">
-        <v>1.115311727805218</v>
+        <v>0.28501261319695548</v>
       </c>
       <c r="Q3">
-        <v>1.203052352152763</v>
+        <v>1.0714796969234781</v>
       </c>
       <c r="R3">
-        <v>2.9468989516836999</v>
+        <v>0.69578332535689436</v>
       </c>
       <c r="S3">
-        <v>0.93720392953263965</v>
+        <v>0.47540171452657121</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
@@ -696,34 +696,34 @@
         <v>22</v>
       </c>
       <c r="J4">
-        <v>-11.063403546704469</v>
+        <v>-15.0211399769314</v>
       </c>
       <c r="K4">
-        <v>1.5982791264457381</v>
+        <v>2.201195948867936</v>
       </c>
       <c r="L4">
-        <v>1.539703257415779</v>
+        <v>0.8437361735022153</v>
       </c>
       <c r="M4">
-        <v>2.0621409833833511</v>
+        <v>2.484305073146293</v>
       </c>
       <c r="N4">
-        <v>1.917784926735137</v>
+        <v>0.96950670692268304</v>
       </c>
       <c r="O4">
-        <v>1.3193570214148389</v>
+        <v>1.9071841168620729</v>
       </c>
       <c r="P4">
-        <v>0.69737452000016376</v>
+        <v>1.843047240960358</v>
       </c>
       <c r="Q4">
-        <v>0.76612099382629761</v>
+        <v>0.35245929811379523</v>
       </c>
       <c r="R4">
-        <v>1.6088672616025499</v>
+        <v>1.1210966131535089</v>
       </c>
       <c r="S4">
-        <v>2.2225674427523869</v>
+        <v>1.090736144150612</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
@@ -755,34 +755,34 @@
         <v>22</v>
       </c>
       <c r="J5">
-        <v>-11.30025381121416</v>
+        <v>-16.007997055359631</v>
       </c>
       <c r="K5">
-        <v>1.7783882174129431</v>
+        <v>3.0247858990008769</v>
       </c>
       <c r="L5">
-        <v>0.77494389441899636</v>
+        <v>0.57760109999973408</v>
       </c>
       <c r="M5">
-        <v>2.308542010054353</v>
+        <v>3.278375365746927</v>
       </c>
       <c r="N5">
-        <v>0.27096619418420781</v>
+        <v>0.44270402389000157</v>
       </c>
       <c r="O5">
-        <v>1.3194889545223349</v>
+        <v>1.8346745639190249</v>
       </c>
       <c r="P5">
-        <v>2.501259917621399</v>
+        <v>0.3836221332171651</v>
       </c>
       <c r="Q5">
-        <v>2.6041058545524329</v>
+        <v>0.55627490573471416</v>
       </c>
       <c r="R5">
-        <v>0.90586521168655498</v>
+        <v>0.90141378262770555</v>
       </c>
       <c r="S5">
-        <v>0.38087326647863179</v>
+        <v>0.88943986372142858</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
@@ -814,34 +814,34 @@
         <v>22</v>
       </c>
       <c r="J6">
-        <v>-11.12374138984171</v>
+        <v>-16.25327490130174</v>
       </c>
       <c r="K6">
-        <v>1.6362729637304541</v>
+        <v>3.2207722739751752</v>
       </c>
       <c r="L6">
-        <v>0.85383093546347855</v>
+        <v>0.60006695712863212</v>
       </c>
       <c r="M6">
-        <v>2.0652352201116781</v>
+        <v>3.5423387271547919</v>
       </c>
       <c r="N6">
-        <v>0.32565049035971377</v>
+        <v>0.32077531642081819</v>
       </c>
       <c r="O6">
-        <v>1.3076481799530499</v>
+        <v>1.8382342354173851</v>
       </c>
       <c r="P6">
-        <v>0.26659566710129529</v>
+        <v>1.0445591585715459</v>
       </c>
       <c r="Q6">
-        <v>0.2478310380096215</v>
+        <v>0.69939671455248098</v>
       </c>
       <c r="R6">
-        <v>1.1810849534370851</v>
+        <v>0.77939812319899127</v>
       </c>
       <c r="S6">
-        <v>0.2167205772002011</v>
+        <v>0.2379054701036788</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
@@ -873,34 +873,34 @@
         <v>22</v>
       </c>
       <c r="J7">
-        <v>-10.82774740015461</v>
+        <v>-15.47593732524</v>
       </c>
       <c r="K7">
-        <v>1.406997151483897</v>
+        <v>2.518646935175235</v>
       </c>
       <c r="L7">
-        <v>0.62763883027671008</v>
+        <v>0.66106728546895521</v>
       </c>
       <c r="M7">
-        <v>1.9103231036612129</v>
+        <v>2.6392777541986741</v>
       </c>
       <c r="N7">
-        <v>0.30387223629357318</v>
+        <v>0.33328248522195542</v>
       </c>
       <c r="O7">
-        <v>1.316695137212031</v>
+        <v>1.8703018044682369</v>
       </c>
       <c r="P7">
-        <v>0.34593138464019119</v>
+        <v>0.43842615781397071</v>
       </c>
       <c r="Q7">
-        <v>0.34280819260424089</v>
+        <v>0.38612402822330499</v>
       </c>
       <c r="R7">
-        <v>0.83080129433800309</v>
+        <v>1.086544047166569</v>
       </c>
       <c r="S7">
-        <v>0.38106407378797869</v>
+        <v>0.60293816995952587</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
@@ -932,34 +932,34 @@
         <v>22</v>
       </c>
       <c r="J8">
-        <v>-11.1996619814759</v>
+        <v>-15.041171250773379</v>
       </c>
       <c r="K8">
-        <v>1.6775796903297739</v>
+        <v>2.1387088466036759</v>
       </c>
       <c r="L8">
-        <v>0.71858392215328615</v>
+        <v>0.74963164143948502</v>
       </c>
       <c r="M8">
-        <v>2.3121983778758239</v>
+        <v>2.6151180019633289</v>
       </c>
       <c r="N8">
-        <v>0.33585297004090292</v>
+        <v>0.31766470795069762</v>
       </c>
       <c r="O8">
-        <v>1.2957029404094551</v>
+        <v>1.9000327689862611</v>
       </c>
       <c r="P8">
-        <v>0.31499348791069509</v>
+        <v>0.87730896308539275</v>
       </c>
       <c r="Q8">
-        <v>0.3414506370858279</v>
+        <v>0.3516981097077988</v>
       </c>
       <c r="R8">
-        <v>0.35809628326551651</v>
+        <v>1.1752072433368881</v>
       </c>
       <c r="S8">
-        <v>0.21142032602707431</v>
+        <v>0.24460193280458661</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
@@ -991,34 +991,34 @@
         <v>22</v>
       </c>
       <c r="J9">
-        <v>-12.956383763954481</v>
+        <v>-15.41732732200348</v>
       </c>
       <c r="K9">
-        <v>3.23518003678711</v>
+        <v>2.436920591091837</v>
       </c>
       <c r="L9">
-        <v>0.51034322535850518</v>
+        <v>0.6509586129003917</v>
       </c>
       <c r="M9">
-        <v>3.5639837228729272</v>
+        <v>2.803966768783436</v>
       </c>
       <c r="N9">
-        <v>1.1736940499643911</v>
+        <v>0.23985344100708381</v>
       </c>
       <c r="O9">
-        <v>1.611646521547033</v>
+        <v>1.8842894455013059</v>
       </c>
       <c r="P9">
-        <v>1.5051683627619159</v>
+        <v>0.25003383140100832</v>
       </c>
       <c r="Q9">
-        <v>1.5304367372938159</v>
+        <v>0.37570316419466121</v>
       </c>
       <c r="R9">
-        <v>0.74429281563299932</v>
+        <v>1.089510830865223</v>
       </c>
       <c r="S9">
-        <v>1.1117021738713471</v>
+        <v>0.30823900241263619</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
@@ -1050,34 +1050,34 @@
         <v>22</v>
       </c>
       <c r="J10">
-        <v>-12.628388280240371</v>
+        <v>-15.551150286519521</v>
       </c>
       <c r="K10">
-        <v>2.9145956367529622</v>
+        <v>2.5301012612200831</v>
       </c>
       <c r="L10">
-        <v>0.26536407216189623</v>
+        <v>0.63519070435447067</v>
       </c>
       <c r="M10">
-        <v>3.254083007907226</v>
+        <v>2.6276460074128591</v>
       </c>
       <c r="N10">
-        <v>0.29109101023632827</v>
+        <v>0.2162577558260684</v>
       </c>
       <c r="O10">
-        <v>1.383924078839347</v>
+        <v>1.8929818871697579</v>
       </c>
       <c r="P10">
-        <v>1.075876564684584</v>
+        <v>0.36277219884649492</v>
       </c>
       <c r="Q10">
-        <v>1.1269671428484631</v>
+        <v>0.39996031160221163</v>
       </c>
       <c r="R10">
-        <v>0.55021278619329972</v>
+        <v>0.53415322835612544</v>
       </c>
       <c r="S10">
-        <v>0.20920384369094749</v>
+        <v>0.23235922232477099</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
@@ -1109,34 +1109,34 @@
         <v>22</v>
       </c>
       <c r="J11">
-        <v>-10.90103806607619</v>
+        <v>-16.9260460948895</v>
       </c>
       <c r="K11">
-        <v>1.4214080664332549</v>
+        <v>3.757987756934047</v>
       </c>
       <c r="L11">
-        <v>0.6168618529292994</v>
+        <v>0.53682353980350495</v>
       </c>
       <c r="M11">
-        <v>1.858809779536154</v>
+        <v>4.0587073172045756</v>
       </c>
       <c r="N11">
-        <v>0.9535654808760029</v>
+        <v>0.92293866378827016</v>
       </c>
       <c r="O11">
-        <v>1.3148394951956439</v>
+        <v>2.0987431157580612</v>
       </c>
       <c r="P11">
-        <v>1.634552954470275</v>
+        <v>0.91303243462886141</v>
       </c>
       <c r="Q11">
-        <v>1.787651815062707</v>
+        <v>1.226931343778175</v>
       </c>
       <c r="R11">
-        <v>0.78313493568650949</v>
+        <v>0.98364891909171992</v>
       </c>
       <c r="S11">
-        <v>1.275991454912176</v>
+        <v>0.86328008775913079</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
@@ -1168,34 +1168,34 @@
         <v>22</v>
       </c>
       <c r="J12">
-        <v>-12.434899470992329</v>
+        <v>-17.16421983886417</v>
       </c>
       <c r="K12">
-        <v>2.6994500699494148</v>
+        <v>3.9712790164161809</v>
       </c>
       <c r="L12">
-        <v>0.29141313693863963</v>
+        <v>0.79001629498462611</v>
       </c>
       <c r="M12">
-        <v>3.0243565083213579</v>
+        <v>4.2498213879976348</v>
       </c>
       <c r="N12">
-        <v>1.08983746285921</v>
+        <v>0.47363368754156232</v>
       </c>
       <c r="O12">
-        <v>1.2695873092919689</v>
+        <v>2.1903418385646081</v>
       </c>
       <c r="P12">
-        <v>0.21293015519051969</v>
+        <v>1.108920602481994</v>
       </c>
       <c r="Q12">
-        <v>0.16035204586139451</v>
+        <v>1.465105087752842</v>
       </c>
       <c r="R12">
-        <v>0.49780166273842769</v>
+        <v>0.69439534709269179</v>
       </c>
       <c r="S12">
-        <v>1.7840563030759959</v>
+        <v>0.24593301198944739</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
@@ -1227,34 +1227,34 @@
         <v>22</v>
       </c>
       <c r="J13">
-        <v>-11.57107145729414</v>
+        <v>-17.43060732887313</v>
       </c>
       <c r="K13">
-        <v>1.9193460849643791</v>
+        <v>4.1975514122447404</v>
       </c>
       <c r="L13">
-        <v>0.58758869859395713</v>
+        <v>0.82028882624882282</v>
       </c>
       <c r="M13">
-        <v>2.3113850619609559</v>
+        <v>4.2757563253521784</v>
       </c>
       <c r="N13">
-        <v>0.44039014875809301</v>
+        <v>0.46966636078938778</v>
       </c>
       <c r="O13">
-        <v>1.2591430027550039</v>
+        <v>2.274100065994932</v>
       </c>
       <c r="P13">
-        <v>0.64820977295103488</v>
+        <v>0.29835234760334861</v>
       </c>
       <c r="Q13">
-        <v>0.72147858600854442</v>
+        <v>1.731492577761798</v>
       </c>
       <c r="R13">
-        <v>0.32230088617093389</v>
+        <v>0.6449466408191209</v>
       </c>
       <c r="S13">
-        <v>0.9004703745484085</v>
+        <v>0.29316427559373859</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
@@ -1286,31 +1286,31 @@
         <v>22</v>
       </c>
       <c r="K14">
-        <v>1.800683826305461</v>
+        <v>3.148741295801821</v>
       </c>
       <c r="L14">
-        <v>0.99301449126932206</v>
+        <v>0.67352944894863087</v>
       </c>
       <c r="M14">
-        <v>2.2580247334875199</v>
+        <v>3.4134256234857898</v>
       </c>
       <c r="N14">
-        <v>0.69689660279623544</v>
+        <v>0.45099030623996211</v>
       </c>
       <c r="O14">
-        <v>1.3564012124068281</v>
+        <v>1.9419230459519281</v>
       </c>
       <c r="P14">
-        <v>0.87834950592395911</v>
+        <v>0.79326403181901994</v>
       </c>
       <c r="Q14">
-        <v>0.91629904272839091</v>
+        <v>0.83407530495928572</v>
       </c>
       <c r="R14">
-        <v>1.017098853406541</v>
+        <v>0.8632821600016336</v>
       </c>
       <c r="S14">
-        <v>0.8225831968841274</v>
+        <v>0.47604682404851872</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
@@ -1342,34 +1342,34 @@
         <v>24</v>
       </c>
       <c r="J15">
-        <v>-9.9682370787663341</v>
+        <v>-17.091393172277499</v>
       </c>
       <c r="K15">
-        <v>0.12737258198552001</v>
+        <v>0.24338968243583001</v>
       </c>
       <c r="L15">
-        <v>0.27961369132143749</v>
+        <v>0.35872684648159031</v>
       </c>
       <c r="M15">
-        <v>0.24916397083071001</v>
+        <v>0.26180292430423058</v>
       </c>
       <c r="N15">
-        <v>0.25157046693599577</v>
+        <v>0.21096771710810591</v>
       </c>
       <c r="O15">
-        <v>0.69964932977632155</v>
+        <v>0.62305244247810776</v>
       </c>
       <c r="P15">
-        <v>0.21793347486998929</v>
+        <v>0.41826683353449901</v>
       </c>
       <c r="Q15">
-        <v>0.16647133860505531</v>
+        <v>0.42191620104318761</v>
       </c>
       <c r="R15">
-        <v>0.20584984708619999</v>
+        <v>0.53407600234092567</v>
       </c>
       <c r="S15">
-        <v>0.29416186147731122</v>
+        <v>0.28530747043464177</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
@@ -1401,34 +1401,34 @@
         <v>24</v>
       </c>
       <c r="J16">
-        <v>-8.4967451057731775</v>
+        <v>-16.74983762133699</v>
       </c>
       <c r="K16">
-        <v>1.2064572659732109</v>
+        <v>0.35702678001805749</v>
       </c>
       <c r="L16">
-        <v>1.011988653367752</v>
+        <v>0.76655026212169564</v>
       </c>
       <c r="M16">
-        <v>1.054291671409699</v>
+        <v>0.33736976049079281</v>
       </c>
       <c r="N16">
-        <v>1.0880122938842129</v>
+        <v>0.34379022088298949</v>
       </c>
       <c r="O16">
-        <v>0.95931768310635113</v>
+        <v>0.73257243199364952</v>
       </c>
       <c r="P16">
-        <v>1.022057668456245</v>
+        <v>0.51101021071242936</v>
       </c>
       <c r="Q16">
-        <v>0.98832347821946398</v>
+        <v>0.37776206114242522</v>
       </c>
       <c r="R16">
-        <v>0.64069098820175019</v>
+        <v>0.67616828591696065</v>
       </c>
       <c r="S16">
-        <v>1.030934834068242</v>
+        <v>0.28743341026000319</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.3">
@@ -1460,34 +1460,34 @@
         <v>24</v>
       </c>
       <c r="J17">
-        <v>-11.063403546704469</v>
+        <v>-15.0211399769314</v>
       </c>
       <c r="K17">
-        <v>2.2955890822929059</v>
+        <v>1.378354885148638</v>
       </c>
       <c r="L17">
-        <v>2.31759346804877</v>
+        <v>1.793648287288228</v>
       </c>
       <c r="M17">
-        <v>1.967453065616005</v>
+        <v>1.2856051319906341</v>
       </c>
       <c r="N17">
-        <v>2.103631244062881</v>
+        <v>1.344831842542022</v>
       </c>
       <c r="O17">
-        <v>1.6153282330280101</v>
+        <v>1.079164952385113</v>
       </c>
       <c r="P17">
-        <v>1.971216356755394</v>
+        <v>1.6151568343251901</v>
       </c>
       <c r="Q17">
-        <v>2.1320727857476158</v>
+        <v>0.95896039809121036</v>
       </c>
       <c r="R17">
-        <v>1.7187242027257741</v>
+        <v>2.1220455378898508</v>
       </c>
       <c r="S17">
-        <v>2.0830440460474731</v>
+        <v>2.1079155193108869</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.3">
@@ -1519,34 +1519,34 @@
         <v>24</v>
       </c>
       <c r="J18">
-        <v>-11.30025381121416</v>
+        <v>-16.007997055359631</v>
       </c>
       <c r="K18">
-        <v>0.14754080137472439</v>
+        <v>0.45141978977359831</v>
       </c>
       <c r="L18">
-        <v>0.66786161622322293</v>
+        <v>0.24954803115398971</v>
       </c>
       <c r="M18">
-        <v>0.22264430367065211</v>
+        <v>0.53538596581985765</v>
       </c>
       <c r="N18">
-        <v>0.21166741747056231</v>
+        <v>0.64877025700755475</v>
       </c>
       <c r="O18">
-        <v>0.6400460006735873</v>
+        <v>0.55483138258385023</v>
       </c>
       <c r="P18">
-        <v>0.26988951417970558</v>
+        <v>0.47915230798456349</v>
       </c>
       <c r="Q18">
-        <v>0.31958836687856867</v>
+        <v>0.70762402492167598</v>
       </c>
       <c r="R18">
-        <v>0.18427103207055201</v>
+        <v>1.355647974322131</v>
       </c>
       <c r="S18">
-        <v>0.43140889315047071</v>
+        <v>0.4899573332227205</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.3">
@@ -1578,34 +1578,34 @@
         <v>24</v>
       </c>
       <c r="J19">
-        <v>-11.12374138984171</v>
+        <v>-16.25327490130174</v>
       </c>
       <c r="K19">
-        <v>0.1353553078371397</v>
+        <v>0.23991973637667061</v>
       </c>
       <c r="L19">
-        <v>0.17474652435557189</v>
+        <v>0.71576307966152675</v>
       </c>
       <c r="M19">
-        <v>0.25494483635355852</v>
+        <v>0.23039492448094909</v>
       </c>
       <c r="N19">
-        <v>0.27596794189466278</v>
+        <v>0.20251567228741671</v>
       </c>
       <c r="O19">
-        <v>0.70278375620991251</v>
+        <v>0.64267493488257432</v>
       </c>
       <c r="P19">
-        <v>0.36786522386968551</v>
+        <v>0.24393221420959429</v>
       </c>
       <c r="Q19">
-        <v>0.32750676888878411</v>
+        <v>0.39567188240539819</v>
       </c>
       <c r="R19">
-        <v>0.30271553164482362</v>
+        <v>0.27437094012248309</v>
       </c>
       <c r="S19">
-        <v>0.21655375399093821</v>
+        <v>0.32241654315202029</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.3">
@@ -1637,34 +1637,34 @@
         <v>24</v>
       </c>
       <c r="J20">
-        <v>-10.82774740015461</v>
+        <v>-15.47593732524</v>
       </c>
       <c r="K20">
-        <v>0.1939912430037429</v>
+        <v>0.5977701665244779</v>
       </c>
       <c r="L20">
-        <v>0.31731023613284232</v>
+        <v>0.90799228857627301</v>
       </c>
       <c r="M20">
-        <v>0.29733346196399169</v>
+        <v>0.55340197789048307</v>
       </c>
       <c r="N20">
-        <v>0.27236402265499282</v>
+        <v>0.58757074305949275</v>
       </c>
       <c r="O20">
-        <v>0.72103839072120368</v>
+        <v>0.80039254562365003</v>
       </c>
       <c r="P20">
-        <v>0.31880358338088027</v>
+        <v>0.64904836818385392</v>
       </c>
       <c r="Q20">
-        <v>0.26848181391871001</v>
+        <v>0.46794612256301249</v>
       </c>
       <c r="R20">
-        <v>0.43899031068427941</v>
+        <v>0.64571753806989973</v>
       </c>
       <c r="S20">
-        <v>0.32399088953379651</v>
+        <v>0.45802327715432628</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.3">
@@ -1696,34 +1696,34 @@
         <v>24</v>
       </c>
       <c r="J21">
-        <v>-11.1996619814759</v>
+        <v>-15.041171250773379</v>
       </c>
       <c r="K21">
-        <v>0.22273714838179659</v>
+        <v>0.40029349327211522</v>
       </c>
       <c r="L21">
-        <v>0.70372938890771264</v>
+        <v>0.65485371969187123</v>
       </c>
       <c r="M21">
-        <v>0.24449497925358249</v>
+        <v>0.37100793143607669</v>
       </c>
       <c r="N21">
-        <v>0.28768620454582222</v>
+        <v>0.34287281171110578</v>
       </c>
       <c r="O21">
-        <v>0.61888409450833448</v>
+        <v>0.74714058789395421</v>
       </c>
       <c r="P21">
-        <v>0.42887256454776812</v>
+        <v>0.4557190602333957</v>
       </c>
       <c r="Q21">
-        <v>0.54753228541018473</v>
+        <v>0.39025227129492462</v>
       </c>
       <c r="R21">
-        <v>0.33885589844530012</v>
+        <v>0.45989850780996272</v>
       </c>
       <c r="S21">
-        <v>0.20901019470889559</v>
+        <v>0.58788192923975036</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.3">
@@ -1755,34 +1755,34 @@
         <v>24</v>
       </c>
       <c r="J22">
-        <v>-12.956383763954481</v>
+        <v>-15.41732732200348</v>
       </c>
       <c r="K22">
-        <v>1.481740329227309</v>
+        <v>0.24568546483804299</v>
       </c>
       <c r="L22">
-        <v>0.82421936282965258</v>
+        <v>0.64267259985117486</v>
       </c>
       <c r="M22">
-        <v>1.1492284610191741</v>
+        <v>0.24645189727747491</v>
       </c>
       <c r="N22">
-        <v>1.103627670856842</v>
+        <v>0.25908163008009533</v>
       </c>
       <c r="O22">
-        <v>0.80062794328497899</v>
+        <v>0.62262443424785685</v>
       </c>
       <c r="P22">
-        <v>1.0757907229887671</v>
+        <v>0.31188766956860242</v>
       </c>
       <c r="Q22">
-        <v>1.21245844295335</v>
+        <v>0.42409856462919882</v>
       </c>
       <c r="R22">
-        <v>0.73829802325898786</v>
+        <v>0.43273407532102298</v>
       </c>
       <c r="S22">
-        <v>0.93138812460169884</v>
+        <v>0.42482658923493971</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.3">
@@ -1814,34 +1814,34 @@
         <v>24</v>
       </c>
       <c r="J23">
-        <v>-12.628388280240371</v>
+        <v>-15.551150286519521</v>
       </c>
       <c r="K23">
-        <v>0.21588957106762111</v>
+        <v>0.24618874826424431</v>
       </c>
       <c r="L23">
-        <v>0.27467640159413331</v>
+        <v>0.29885724984251788</v>
       </c>
       <c r="M23">
-        <v>0.29747872546108678</v>
+        <v>0.22656885565064699</v>
       </c>
       <c r="N23">
-        <v>0.42160584500021703</v>
+        <v>0.208159159576807</v>
       </c>
       <c r="O23">
-        <v>0.72482521768524666</v>
+        <v>0.6595703694362659</v>
       </c>
       <c r="P23">
-        <v>0.345132334319736</v>
+        <v>0.24338783003187051</v>
       </c>
       <c r="Q23">
-        <v>0.30071561195193452</v>
+        <v>0.377937111123125</v>
       </c>
       <c r="R23">
-        <v>0.4998060317674764</v>
+        <v>0.2824834565415103</v>
       </c>
       <c r="S23">
-        <v>0.21885654745791361</v>
+        <v>0.2352550837318419</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.3">
@@ -1873,34 +1873,34 @@
         <v>24</v>
       </c>
       <c r="J24">
-        <v>-10.90103806607619</v>
+        <v>-16.9260460948895</v>
       </c>
       <c r="K24">
-        <v>1.449021221721257</v>
+        <v>0.70966564581507618</v>
       </c>
       <c r="L24">
-        <v>1.596233774468796</v>
+        <v>1.310264464958852</v>
       </c>
       <c r="M24">
-        <v>1.336944175325776</v>
+        <v>0.80611313586564837</v>
       </c>
       <c r="N24">
-        <v>1.2926552558454669</v>
+        <v>0.80476002187431872</v>
       </c>
       <c r="O24">
-        <v>1.103441971666727</v>
+        <v>0.61570476507519811</v>
       </c>
       <c r="P24">
-        <v>1.1613248746724141</v>
+        <v>0.73103648944596222</v>
       </c>
       <c r="Q24">
-        <v>1.190372308341918</v>
+        <v>0.99442802928402541</v>
       </c>
       <c r="R24">
-        <v>1.9756556999116399</v>
+        <v>0.28467564820941049</v>
       </c>
       <c r="S24">
-        <v>1.4839722667527171</v>
+        <v>0.99423438015377363</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.3">
@@ -1932,34 +1932,34 @@
         <v>24</v>
       </c>
       <c r="J25">
-        <v>-12.434899470992329</v>
+        <v>-17.16421983886417</v>
       </c>
       <c r="K25">
-        <v>1.267237823590184</v>
+        <v>0.23864991151780651</v>
       </c>
       <c r="L25">
-        <v>0.79987451846088198</v>
+        <v>0.3292579867467309</v>
       </c>
       <c r="M25">
-        <v>0.91605450440661984</v>
+        <v>0.22599672012088801</v>
       </c>
       <c r="N25">
-        <v>1.179259587687042</v>
+        <v>0.19324733866681901</v>
       </c>
       <c r="O25">
-        <v>0.65580847175345847</v>
+        <v>0.64302786759637831</v>
       </c>
       <c r="P25">
-        <v>1.1446322923833421</v>
+        <v>0.2268643300186084</v>
       </c>
       <c r="Q25">
-        <v>1.1890600119954049</v>
+        <v>0.39433631123551782</v>
       </c>
       <c r="R25">
-        <v>0.70323787135465998</v>
+        <v>0.1213078038758978</v>
       </c>
       <c r="S25">
-        <v>1.8179311223225461</v>
+        <v>0.43013534988840291</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.3">
@@ -1991,34 +1991,34 @@
         <v>24</v>
       </c>
       <c r="J26">
-        <v>-11.57107145729414</v>
+        <v>-17.43060732887313</v>
       </c>
       <c r="K26">
-        <v>0.6188383327889504</v>
+        <v>0.23747295928493209</v>
       </c>
       <c r="L26">
-        <v>0.59767584626374759</v>
+        <v>0.4669224679507642</v>
       </c>
       <c r="M26">
-        <v>0.60638772285466114</v>
+        <v>0.23472634623119029</v>
       </c>
       <c r="N26">
-        <v>0.77878165108284136</v>
+        <v>0.2026874409179748</v>
       </c>
       <c r="O26">
-        <v>0.8098792670797863</v>
+        <v>0.63826614542020332</v>
       </c>
       <c r="P26">
-        <v>0.37418980764986159</v>
+        <v>0.231182968480205</v>
       </c>
       <c r="Q26">
-        <v>0.33885223735296688</v>
+        <v>0.39964049548996411</v>
       </c>
       <c r="R26">
-        <v>0.50029398935933667</v>
+        <v>0.20178036452061951</v>
       </c>
       <c r="S26">
-        <v>1.056967854440225</v>
+        <v>0.25748392714622859</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.3">
@@ -2050,31 +2050,31 @@
         <v>24</v>
       </c>
       <c r="K27">
-        <v>0.78014755910369704</v>
+        <v>0.44548643860579079</v>
       </c>
       <c r="L27">
-        <v>0.79712695683121015</v>
+        <v>0.70792144036043458</v>
       </c>
       <c r="M27">
-        <v>0.71636832318045973</v>
+        <v>0.44290213096323933</v>
       </c>
       <c r="N27">
-        <v>0.77223580016012827</v>
+        <v>0.44577123797622531</v>
       </c>
       <c r="O27">
-        <v>0.83763586329115991</v>
+        <v>0.69658523830140018</v>
       </c>
       <c r="P27">
-        <v>0.72480903483948234</v>
+        <v>0.50972042639406456</v>
       </c>
       <c r="Q27">
-        <v>0.74845295418866309</v>
+        <v>0.52588112276863874</v>
       </c>
       <c r="R27">
-        <v>0.68728245220923168</v>
+        <v>0.61590884457838968</v>
       </c>
       <c r="S27">
-        <v>0.84151836571268568</v>
+        <v>0.57340590107746137</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.3">
@@ -2106,34 +2106,34 @@
         <v>22</v>
       </c>
       <c r="J28">
-        <v>-13.94284661468012</v>
+        <v>-11.91852847718317</v>
       </c>
       <c r="K28">
-        <v>11.76352151068831</v>
+        <v>3.664029695360806</v>
       </c>
       <c r="L28">
-        <v>0.95168371028651766</v>
+        <v>0.89756189745248083</v>
       </c>
       <c r="M28">
-        <v>13.78233925995778</v>
+        <v>4.3439479295066921</v>
       </c>
       <c r="N28">
-        <v>0.80933669930612662</v>
+        <v>0.31274404746241852</v>
       </c>
       <c r="O28">
-        <v>4.0934539313223626</v>
+        <v>5.0087855541669377</v>
       </c>
       <c r="P28">
-        <v>1.353451958730149</v>
+        <v>0.30146340172605518</v>
       </c>
       <c r="Q28">
-        <v>1.2597793576627561</v>
+        <v>0.28114920883968142</v>
       </c>
       <c r="R28">
-        <v>0.8951893108706872</v>
+        <v>0.61368214353018713</v>
       </c>
       <c r="S28">
-        <v>0.27544012047084232</v>
+        <v>0.24575510771945189</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
@@ -2165,34 +2165,34 @@
         <v>22</v>
       </c>
       <c r="J29">
-        <v>-12.229594417622669</v>
+        <v>-10.454792830440351</v>
       </c>
       <c r="K29">
-        <v>13.36887332512439</v>
+        <v>4.124230904859675</v>
       </c>
       <c r="L29">
-        <v>2.6232785489604309</v>
+        <v>0.90237450444198286</v>
       </c>
       <c r="M29">
-        <v>15.63399397272452</v>
+        <v>4.9285141467084959</v>
       </c>
       <c r="N29">
-        <v>1.32995271235987</v>
+        <v>1.0640593639571121</v>
       </c>
       <c r="O29">
-        <v>4.494640149173823</v>
+        <v>5.0934623910893473</v>
       </c>
       <c r="P29">
-        <v>1.449864389848005</v>
+        <v>1.008519824216177</v>
       </c>
       <c r="Q29">
-        <v>1.325328160983356</v>
+        <v>0.67217211581446057</v>
       </c>
       <c r="R29">
-        <v>2.82891060576141</v>
+        <v>0.85137174466058241</v>
       </c>
       <c r="S29">
-        <v>0.71913659360578375</v>
+        <v>1.3023346352676279</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.3">
@@ -2224,34 +2224,34 @@
         <v>22</v>
       </c>
       <c r="J30">
-        <v>-11.96879591831858</v>
+        <v>-9.0340993265067748</v>
       </c>
       <c r="K30">
-        <v>13.51948372259381</v>
+        <v>4.7794342306467303</v>
       </c>
       <c r="L30">
-        <v>3.1624184913568851</v>
+        <v>1.192164634048795</v>
       </c>
       <c r="M30">
-        <v>14.851998466602151</v>
+        <v>4.998558114835272</v>
       </c>
       <c r="N30">
-        <v>0.72416800222268751</v>
+        <v>0.88447874981687036</v>
       </c>
       <c r="O30">
-        <v>4.2987997624501189</v>
+        <v>5.171748725235072</v>
       </c>
       <c r="P30">
-        <v>0.99282820186708765</v>
+        <v>2.6632950229102872</v>
       </c>
       <c r="Q30">
-        <v>0.87969424720360212</v>
+        <v>1.90785081888708</v>
       </c>
       <c r="R30">
-        <v>4.7802269546279881</v>
+        <v>1.1833637502841921</v>
       </c>
       <c r="S30">
-        <v>0.3082595263957989</v>
+        <v>0.49083955333893531</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.3">
@@ -2283,34 +2283,34 @@
         <v>22</v>
       </c>
       <c r="J31">
-        <v>-12.01575520722014</v>
+        <v>-7.7486971337838737</v>
       </c>
       <c r="K31">
-        <v>13.35957657091503</v>
+        <v>5.4723668398220866</v>
       </c>
       <c r="L31">
-        <v>3.4963764898820759</v>
+        <v>1.087451831169727</v>
       </c>
       <c r="M31">
-        <v>15.547237369658269</v>
+        <v>5.9571579398483356</v>
       </c>
       <c r="N31">
-        <v>0.65021793007539541</v>
+        <v>0.44563482685085409</v>
       </c>
       <c r="O31">
-        <v>4.0622644661356446</v>
+        <v>5.2384082795205718</v>
       </c>
       <c r="P31">
-        <v>0.42321269236565162</v>
+        <v>1.5609890250251199</v>
       </c>
       <c r="Q31">
-        <v>0.59929592470819437</v>
+        <v>3.1781651267781981</v>
       </c>
       <c r="R31">
-        <v>6.2239339583333253</v>
+        <v>1.299894817775253</v>
       </c>
       <c r="S31">
-        <v>0.25055998967539272</v>
+        <v>0.44327688259614551</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.3">
@@ -2342,34 +2342,34 @@
         <v>22</v>
       </c>
       <c r="J32">
-        <v>-11.42441525498085</v>
+        <v>-5.8801567633685314</v>
       </c>
       <c r="K32">
-        <v>13.82956451402306</v>
+        <v>6.7239960539071673</v>
       </c>
       <c r="L32">
-        <v>4.1123822703323993</v>
+        <v>0.58396736399767146</v>
       </c>
       <c r="M32">
-        <v>15.963972161655629</v>
+        <v>6.7655934217262823</v>
       </c>
       <c r="N32">
-        <v>0.87602624799491613</v>
+        <v>0.58482363320760189</v>
       </c>
       <c r="O32">
-        <v>4.0663970952985418</v>
+        <v>5.3373885202599034</v>
       </c>
       <c r="P32">
-        <v>0.2875049537014841</v>
+        <v>2.0160285788420129</v>
       </c>
       <c r="Q32">
-        <v>0.18786868667368389</v>
+        <v>5.0467054971935408</v>
       </c>
       <c r="R32">
-        <v>6.8447053336618913</v>
+        <v>0.35960124675214922</v>
       </c>
       <c r="S32">
-        <v>0.5796636263832311</v>
+        <v>0.8171961659808763</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.3">
@@ -2401,34 +2401,34 @@
         <v>22</v>
       </c>
       <c r="J33">
-        <v>-11.84964237561382</v>
+        <v>-2.8967513795164028</v>
       </c>
       <c r="K33">
-        <v>13.30012139470594</v>
+        <v>9.1926137155176235</v>
       </c>
       <c r="L33">
-        <v>3.8042353189628502</v>
+        <v>1.6331944323802059</v>
       </c>
       <c r="M33">
-        <v>15.489915553834241</v>
+        <v>7.9873774079902944</v>
       </c>
       <c r="N33">
-        <v>0.55151181944393279</v>
+        <v>1.4192440380791329</v>
       </c>
       <c r="O33">
-        <v>3.8579971736093759</v>
+        <v>5.5647234407068318</v>
       </c>
       <c r="P33">
-        <v>0.245002929403034</v>
+        <v>3.6515063117219921</v>
       </c>
       <c r="Q33">
-        <v>0.19662114084832541</v>
+        <v>8.0301108810456689</v>
       </c>
       <c r="R33">
-        <v>6.2225385280823646</v>
+        <v>3.1747586229917211</v>
       </c>
       <c r="S33">
-        <v>0.50099196630739073</v>
+        <v>1.5363631173006129</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.3">
@@ -2460,34 +2460,34 @@
         <v>22</v>
       </c>
       <c r="J34">
-        <v>-12.061379764322639</v>
+        <v>0.2915371216201037</v>
       </c>
       <c r="K34">
-        <v>12.985578617906191</v>
+        <v>12.142404081463891</v>
       </c>
       <c r="L34">
-        <v>3.513557452870252</v>
+        <v>0.75415815785036244</v>
       </c>
       <c r="M34">
-        <v>14.770115326604079</v>
+        <v>10.19110987074029</v>
       </c>
       <c r="N34">
-        <v>0.62309730740083724</v>
+        <v>1.641126212470321</v>
       </c>
       <c r="O34">
-        <v>3.7723607094456368</v>
+        <v>6.0513306696798166</v>
       </c>
       <c r="P34">
-        <v>0.55515303234216595</v>
+        <v>4.6254516647340216</v>
       </c>
       <c r="Q34">
-        <v>0.75669204597923723</v>
+        <v>11.218399382182181</v>
       </c>
       <c r="R34">
-        <v>5.954144200627896</v>
+        <v>1.886259857051249</v>
       </c>
       <c r="S34">
-        <v>0.2465239821741351</v>
+        <v>1.268599894937172</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.3">
@@ -2519,34 +2519,34 @@
         <v>22</v>
       </c>
       <c r="J35">
-        <v>-10.65342968052545</v>
+        <v>1.1494642247970821</v>
       </c>
       <c r="K35">
-        <v>14.22871659865597</v>
+        <v>12.932589749029519</v>
       </c>
       <c r="L35">
-        <v>4.8084053171563106</v>
+        <v>1.545332084198564</v>
       </c>
       <c r="M35">
-        <v>16.728669882144569</v>
+        <v>11.518000818354389</v>
       </c>
       <c r="N35">
-        <v>1.478209099293571</v>
+        <v>0.39939098369876641</v>
       </c>
       <c r="O35">
-        <v>3.979976585162754</v>
+        <v>6.0100639153999804</v>
       </c>
       <c r="P35">
-        <v>0.93440018807476366</v>
+        <v>1.92615689712698</v>
       </c>
       <c r="Q35">
-        <v>0.85131061420577714</v>
+        <v>12.076326485359161</v>
       </c>
       <c r="R35">
-        <v>7.365200905933019</v>
+        <v>0.6093497443684508</v>
       </c>
       <c r="S35">
-        <v>0.96730317206640615</v>
+        <v>0.36280922174670499</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.3">
@@ -2578,34 +2578,34 @@
         <v>22</v>
       </c>
       <c r="J36">
-        <v>-9.7029552386445914</v>
+        <v>2.1923500188855689</v>
       </c>
       <c r="K36">
-        <v>15.021307239918659</v>
+        <v>13.88403767889772</v>
       </c>
       <c r="L36">
-        <v>5.6064799979100703</v>
+        <v>0.75953033635287048</v>
       </c>
       <c r="M36">
-        <v>17.185449709927369</v>
+        <v>11.732729846721471</v>
       </c>
       <c r="N36">
-        <v>1.4711420864815259</v>
+        <v>0.39218727296425188</v>
       </c>
       <c r="O36">
-        <v>4.1688260412695843</v>
+        <v>5.9668081603552876</v>
       </c>
       <c r="P36">
-        <v>1.9721822491522649</v>
+        <v>0.26487004243358342</v>
       </c>
       <c r="Q36">
-        <v>1.9273713557154091</v>
+        <v>13.119212279447639</v>
       </c>
       <c r="R36">
-        <v>8.2858676331849068</v>
+        <v>0.36328848524904928</v>
       </c>
       <c r="S36">
-        <v>0.3903274296685233</v>
+        <v>0.37014464548096881</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.3">
@@ -2637,34 +2637,34 @@
         <v>22</v>
       </c>
       <c r="J37">
-        <v>-9.6021898684714291</v>
+        <v>3.5919187144270341</v>
       </c>
       <c r="K37">
-        <v>14.9944745762533</v>
+        <v>15.178152547041689</v>
       </c>
       <c r="L37">
-        <v>5.7142764352500981</v>
+        <v>0.80997954428947017</v>
       </c>
       <c r="M37">
-        <v>16.506057088707859</v>
+        <v>12.2840386638978</v>
       </c>
       <c r="N37">
-        <v>0.96186440044389387</v>
+        <v>0.56098643041530138</v>
       </c>
       <c r="O37">
-        <v>4.1019855217129244</v>
+        <v>5.9910806789303228</v>
       </c>
       <c r="P37">
-        <v>0.31714494266914323</v>
+        <v>1.3064299475217169</v>
       </c>
       <c r="Q37">
-        <v>0.2202011493846259</v>
+        <v>14.518780974989109</v>
       </c>
       <c r="R37">
-        <v>8.3949589612325326</v>
+        <v>0.34685705319642252</v>
       </c>
       <c r="S37">
-        <v>0.24650829664249471</v>
+        <v>0.47601129957563842</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.3">
@@ -2696,34 +2696,34 @@
         <v>22</v>
       </c>
       <c r="J38">
-        <v>-8.4123539485237355</v>
+        <v>5.3953533278732859</v>
       </c>
       <c r="K38">
-        <v>16.004570296286431</v>
+        <v>16.869167533617581</v>
       </c>
       <c r="L38">
-        <v>6.8746923633461554</v>
+        <v>0.74203859865720889</v>
       </c>
       <c r="M38">
-        <v>17.841931239269531</v>
+        <v>13.72413992709351</v>
       </c>
       <c r="N38">
-        <v>1.8167862648651429</v>
+        <v>0.98129964477271325</v>
       </c>
       <c r="O38">
-        <v>4.4308480973245858</v>
+        <v>6.1085679237738164</v>
       </c>
       <c r="P38">
-        <v>0.53207029478340939</v>
+        <v>1.8569643110692671</v>
       </c>
       <c r="Q38">
-        <v>0.41900838699786158</v>
+        <v>16.322215588435359</v>
       </c>
       <c r="R38">
-        <v>9.5388477240342215</v>
+        <v>0.54689933592387741</v>
       </c>
       <c r="S38">
-        <v>0.79321240187059872</v>
+        <v>0.72690400095241348</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.3">
@@ -2755,34 +2755,34 @@
         <v>22</v>
       </c>
       <c r="J39">
-        <v>-8.8344287080347428</v>
+        <v>6.3363129693044078</v>
       </c>
       <c r="K39">
-        <v>15.473087057577411</v>
+        <v>17.69275941348273</v>
       </c>
       <c r="L39">
-        <v>6.4641109641755206</v>
+        <v>0.35836932982187591</v>
       </c>
       <c r="M39">
-        <v>17.939244366067339</v>
+        <v>15.455592210598949</v>
       </c>
       <c r="N39">
-        <v>0.9858017586936374</v>
+        <v>0.75509886304134421</v>
       </c>
       <c r="O39">
-        <v>4.1325421314170736</v>
+        <v>6.0288083593013821</v>
       </c>
       <c r="P39">
-        <v>0.45805065565460429</v>
+        <v>1.4006408989628889</v>
       </c>
       <c r="Q39">
-        <v>0.37080852446282092</v>
+        <v>17.26317522986648</v>
       </c>
       <c r="R39">
-        <v>9.1501711427491212</v>
+        <v>0.50232631487617152</v>
       </c>
       <c r="S39">
-        <v>0.49816100338600272</v>
+        <v>0.25154096419138933</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.3">
@@ -2814,31 +2814,31 @@
         <v>22</v>
       </c>
       <c r="K40">
-        <v>13.987406285387371</v>
+        <v>10.221315203637269</v>
       </c>
       <c r="L40">
-        <v>4.2609914467074654</v>
+        <v>0.93884355955510135</v>
       </c>
       <c r="M40">
-        <v>16.020077033096111</v>
+        <v>9.1572300248351493</v>
       </c>
       <c r="N40">
-        <v>1.0231761940484609</v>
+        <v>0.78675617222805727</v>
       </c>
       <c r="O40">
-        <v>4.1216743053602034</v>
+        <v>5.6309313848682727</v>
       </c>
       <c r="P40">
-        <v>0.79340554071598035</v>
+        <v>1.8818596605241751</v>
       </c>
       <c r="Q40">
-        <v>0.74949829956880398</v>
+        <v>8.6361886324032131</v>
       </c>
       <c r="R40">
-        <v>6.3737246049249459</v>
+        <v>0.97813775972160866</v>
       </c>
       <c r="S40">
-        <v>0.48134067572055012</v>
+        <v>0.69098129075732828</v>
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.3">
@@ -2870,34 +2870,34 @@
         <v>24</v>
       </c>
       <c r="J41">
-        <v>-13.94284661468012</v>
+        <v>-11.91852847718317</v>
       </c>
       <c r="K41">
-        <v>0.36985085427681069</v>
+        <v>0.29870287560184339</v>
       </c>
       <c r="L41">
-        <v>0.61844312706845783</v>
+        <v>0.24899677669613279</v>
       </c>
       <c r="M41">
-        <v>0.5587671487058905</v>
+        <v>0.33455106466458701</v>
       </c>
       <c r="N41">
-        <v>0.27317531696996877</v>
+        <v>0.292576340058192</v>
       </c>
       <c r="O41">
-        <v>1.0075031166926891</v>
+        <v>0.91417100274033714</v>
       </c>
       <c r="P41">
-        <v>0.3167711830179214</v>
+        <v>0.25846405429268549</v>
       </c>
       <c r="Q41">
-        <v>0.23930450690779689</v>
+        <v>0.26248969419536772</v>
       </c>
       <c r="R41">
-        <v>0.55732360396223857</v>
+        <v>0.21974517685150519</v>
       </c>
       <c r="S41">
-        <v>0.28459131898327011</v>
+        <v>0.25629304038625</v>
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.3">
@@ -2929,34 +2929,34 @@
         <v>24</v>
       </c>
       <c r="J42">
-        <v>-12.229594417622669</v>
+        <v>-10.454792830440351</v>
       </c>
       <c r="K42">
-        <v>0.92553976736062671</v>
+        <v>1.110985499751975</v>
       </c>
       <c r="L42">
-        <v>0.31566268258512631</v>
+        <v>1.0456773317141741</v>
       </c>
       <c r="M42">
-        <v>1.1230131347246519</v>
+        <v>0.92663580384509703</v>
       </c>
       <c r="N42">
-        <v>0.71699542155900997</v>
+        <v>1.2542196793454179</v>
       </c>
       <c r="O42">
-        <v>1.092317117876165</v>
+        <v>1.1767666796447149</v>
       </c>
       <c r="P42">
-        <v>0.5793714135353154</v>
+        <v>1.320758657097632</v>
       </c>
       <c r="Q42">
-        <v>0.50532410255595472</v>
+        <v>1.3706045054808911</v>
       </c>
       <c r="R42">
-        <v>0.38742663715759068</v>
+        <v>1.577663561858065</v>
       </c>
       <c r="S42">
-        <v>0.58808561519653679</v>
+        <v>1.2752859625606801</v>
       </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.3">
@@ -2988,34 +2988,34 @@
         <v>24</v>
       </c>
       <c r="J43">
-        <v>-11.96879591831858</v>
+        <v>-9.0340993265067748</v>
       </c>
       <c r="K43">
-        <v>0.16307847902678249</v>
+        <v>1.0741061336779401</v>
       </c>
       <c r="L43">
-        <v>0.56040885362278581</v>
+        <v>1.3222558786163241</v>
       </c>
       <c r="M43">
-        <v>0.29638767351973028</v>
+        <v>0.93737950610971277</v>
       </c>
       <c r="N43">
-        <v>0.3604836135327002</v>
+        <v>0.73341206327284136</v>
       </c>
       <c r="O43">
-        <v>0.96791802484287581</v>
+        <v>1.1192611935974379</v>
       </c>
       <c r="P43">
-        <v>0.29215985266607952</v>
+        <v>1.2089042558536269</v>
       </c>
       <c r="Q43">
-        <v>0.32034937850860989</v>
+        <v>1.332813504094378</v>
       </c>
       <c r="R43">
-        <v>0.49008497557702929</v>
+        <v>0.21277882991191599</v>
       </c>
       <c r="S43">
-        <v>0.26096353034236142</v>
+        <v>0.4852208761829071</v>
       </c>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.3">
@@ -3047,34 +3047,34 @@
         <v>24</v>
       </c>
       <c r="J44">
-        <v>-12.01575520722014</v>
+        <v>-7.7486971337838737</v>
       </c>
       <c r="K44">
-        <v>0.25234631241193278</v>
+        <v>0.95157951890667247</v>
       </c>
       <c r="L44">
-        <v>0.32589337616289948</v>
+        <v>0.54849822104069768</v>
       </c>
       <c r="M44">
-        <v>0.29120177533045621</v>
+        <v>0.75987792272870969</v>
       </c>
       <c r="N44">
-        <v>0.27437233949830581</v>
+        <v>0.48309737451852208</v>
       </c>
       <c r="O44">
-        <v>0.95386283159003038</v>
+        <v>1.0507003837188189</v>
       </c>
       <c r="P44">
-        <v>0.64304206553658294</v>
+        <v>0.42592136166841482</v>
       </c>
       <c r="Q44">
-        <v>0.84689466246455058</v>
+        <v>1.2145193355698889</v>
       </c>
       <c r="R44">
-        <v>0.12758371145121811</v>
+        <v>0.5464297579107571</v>
       </c>
       <c r="S44">
-        <v>0.2811663601793627</v>
+        <v>0.41845051802690031</v>
       </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.3">
@@ -3106,34 +3106,34 @@
         <v>24</v>
       </c>
       <c r="J45">
-        <v>-11.42441525498085</v>
+        <v>-5.8801567633685314</v>
       </c>
       <c r="K45">
-        <v>0.21028016778174161</v>
+        <v>1.4960179146076611</v>
       </c>
       <c r="L45">
-        <v>0.27686711863497709</v>
+        <v>1.011675086835599</v>
       </c>
       <c r="M45">
-        <v>0.37158914988978847</v>
+        <v>1.2773160411118749</v>
       </c>
       <c r="N45">
-        <v>0.3285959006939756</v>
+        <v>0.81628041543389629</v>
       </c>
       <c r="O45">
-        <v>0.99734752385299053</v>
+        <v>1.2051823513935529</v>
       </c>
       <c r="P45">
-        <v>0.27579776663731642</v>
+        <v>0.80032601533116976</v>
       </c>
       <c r="Q45">
-        <v>0.1949777333508898</v>
+        <v>1.7311101413870531</v>
       </c>
       <c r="R45">
-        <v>0.59774036186106938</v>
+        <v>0.44186236571705312</v>
       </c>
       <c r="S45">
-        <v>0.50138300518161383</v>
+        <v>0.76452289205544832</v>
       </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.3">
@@ -3165,34 +3165,34 @@
         <v>24</v>
       </c>
       <c r="J46">
-        <v>-11.84964237561382</v>
+        <v>-2.8967513795164028</v>
       </c>
       <c r="K46">
-        <v>0.49535557545270559</v>
+        <v>2.6054414470193268</v>
       </c>
       <c r="L46">
-        <v>1.2617103840621779</v>
+        <v>1.108865839604624</v>
       </c>
       <c r="M46">
-        <v>0.34501727491293172</v>
+        <v>2.3361774796436969</v>
       </c>
       <c r="N46">
-        <v>0.50555716914755799</v>
+        <v>1.8620412904001451</v>
       </c>
       <c r="O46">
-        <v>0.93987377862113619</v>
+        <v>1.976020973626238</v>
       </c>
       <c r="P46">
-        <v>0.36722899650360091</v>
+        <v>1.72874964017111</v>
       </c>
       <c r="Q46">
-        <v>0.40182467313326792</v>
+        <v>2.821544030188976</v>
       </c>
       <c r="R46">
-        <v>1.075241014638282</v>
+        <v>2.184851143833582</v>
       </c>
       <c r="S46">
-        <v>0.6130284640203193</v>
+        <v>1.529307944595403</v>
       </c>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.3">
@@ -3224,34 +3224,34 @@
         <v>24</v>
       </c>
       <c r="J47">
-        <v>-12.061379764322639</v>
+        <v>0.2915371216201037</v>
       </c>
       <c r="K47">
-        <v>0.34242303414463582</v>
+        <v>2.8076459064374788</v>
       </c>
       <c r="L47">
-        <v>0.22810997028502081</v>
+        <v>1.4715672534095521</v>
       </c>
       <c r="M47">
-        <v>0.3055440672698676</v>
+        <v>2.5558721263335968</v>
       </c>
       <c r="N47">
-        <v>0.25219597212464551</v>
+        <v>1.9539881570584361</v>
       </c>
       <c r="O47">
-        <v>0.95631522131050728</v>
+        <v>1.995345541376039</v>
       </c>
       <c r="P47">
-        <v>0.38256598722021162</v>
+        <v>1.6276414812708671</v>
       </c>
       <c r="Q47">
-        <v>0.44073091650874258</v>
+        <v>3.0264271474733562</v>
       </c>
       <c r="R47">
-        <v>0.47288651744230359</v>
+        <v>1.8976106535324131</v>
       </c>
       <c r="S47">
-        <v>0.24241289971217961</v>
+        <v>1.0970028377365939</v>
       </c>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.3">
@@ -3283,34 +3283,34 @@
         <v>24</v>
       </c>
       <c r="J48">
-        <v>-10.65342968052545</v>
+        <v>1.1494642247970821</v>
       </c>
       <c r="K48">
-        <v>0.6775415884175523</v>
+        <v>0.59534425490650034</v>
       </c>
       <c r="L48">
-        <v>0.9578768512612329</v>
+        <v>0.22449032181973411</v>
       </c>
       <c r="M48">
-        <v>0.8296587274624615</v>
+        <v>0.53492140964925494</v>
       </c>
       <c r="N48">
-        <v>0.86179915914426697</v>
+        <v>0.20353569689202411</v>
       </c>
       <c r="O48">
-        <v>1.0765867385781971</v>
+        <v>0.99119698086870955</v>
       </c>
       <c r="P48">
-        <v>1.017013355098549</v>
+        <v>0.47580981011717199</v>
       </c>
       <c r="Q48">
-        <v>1.017786049096697</v>
+        <v>0.84921695424810539</v>
       </c>
       <c r="R48">
-        <v>1.434049838364053</v>
+        <v>0.26336180220947408</v>
       </c>
       <c r="S48">
-        <v>1.0055769192194011</v>
+        <v>0.48534142686095649</v>
       </c>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.3">
@@ -3342,34 +3342,34 @@
         <v>24</v>
       </c>
       <c r="J49">
-        <v>-9.7029552386445914</v>
+        <v>2.1923500188855689</v>
       </c>
       <c r="K49">
-        <v>0.37005080044385069</v>
+        <v>0.72160634899671361</v>
       </c>
       <c r="L49">
-        <v>0.20241815412312739</v>
+        <v>0.44781578087011648</v>
       </c>
       <c r="M49">
-        <v>0.51168954564074842</v>
+        <v>0.58491000109146296</v>
       </c>
       <c r="N49">
-        <v>0.26644610658947182</v>
+        <v>0.31375145614252342</v>
       </c>
       <c r="O49">
-        <v>1.02822037501621</v>
+        <v>1.007419614054202</v>
       </c>
       <c r="P49">
-        <v>0.6373339802407525</v>
+        <v>0.4801024660548634</v>
       </c>
       <c r="Q49">
-        <v>0.61872489369920269</v>
+        <v>1.004972892728462</v>
       </c>
       <c r="R49">
-        <v>0.1158025694616361</v>
+        <v>0.20640298522982409</v>
       </c>
       <c r="S49">
-        <v>0.32045519702017577</v>
+        <v>0.30761292583327587</v>
       </c>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.3">
@@ -3401,34 +3401,34 @@
         <v>24</v>
       </c>
       <c r="J50">
-        <v>-9.6021898684714291</v>
+        <v>3.5919187144270341</v>
       </c>
       <c r="K50">
-        <v>0.19321517149540399</v>
+        <v>1.02667411906887</v>
       </c>
       <c r="L50">
-        <v>0.5379869363522527</v>
+        <v>0.50590450974454304</v>
       </c>
       <c r="M50">
-        <v>0.27945502875021488</v>
+        <v>0.83420857624117994</v>
       </c>
       <c r="N50">
-        <v>0.31643158067884652</v>
+        <v>0.5390454030770665</v>
       </c>
       <c r="O50">
-        <v>0.97338290829751761</v>
+        <v>1.0387303936143191</v>
       </c>
       <c r="P50">
-        <v>0.38620214094486038</v>
+        <v>0.43091547215668158</v>
       </c>
       <c r="Q50">
-        <v>0.4377473764495794</v>
+        <v>1.3142659223261051</v>
       </c>
       <c r="R50">
-        <v>0.49225957418544558</v>
+        <v>0.54799378020614942</v>
       </c>
       <c r="S50">
-        <v>0.24378876458223961</v>
+        <v>0.39306119439831139</v>
       </c>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.3">
@@ -3460,34 +3460,34 @@
         <v>24</v>
       </c>
       <c r="J51">
-        <v>-8.4123539485237355</v>
+        <v>5.3953533278732859</v>
       </c>
       <c r="K51">
-        <v>0.51637403188321007</v>
+        <v>1.407997075417031</v>
       </c>
       <c r="L51">
-        <v>1.5522374352398169</v>
+        <v>1.1040833692596479</v>
       </c>
       <c r="M51">
-        <v>0.65348790129103063</v>
+        <v>1.211969780431986</v>
       </c>
       <c r="N51">
-        <v>0.61040694049068689</v>
+        <v>0.85029029581024018</v>
       </c>
       <c r="O51">
-        <v>1.045210824665719</v>
+        <v>1.0906124275505349</v>
       </c>
       <c r="P51">
-        <v>0.40394029537905601</v>
+        <v>0.55560508713053602</v>
       </c>
       <c r="Q51">
-        <v>0.34416771874022639</v>
+        <v>1.670395414398967</v>
       </c>
       <c r="R51">
-        <v>1.330353955645539</v>
+        <v>0.52028326805581215</v>
       </c>
       <c r="S51">
-        <v>0.66721391465753155</v>
+        <v>0.54058466697765228</v>
       </c>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.3">
@@ -3519,34 +3519,34 @@
         <v>24</v>
       </c>
       <c r="J52">
-        <v>-8.8344287080347428</v>
+        <v>6.3363129693044078</v>
       </c>
       <c r="K52">
-        <v>0.49423034560876528</v>
+        <v>0.64403368330863575</v>
       </c>
       <c r="L52">
-        <v>0.1584789691946619</v>
+        <v>0.37707383133448802</v>
       </c>
       <c r="M52">
-        <v>0.37468036696835838</v>
+        <v>0.53116575401630639</v>
       </c>
       <c r="N52">
-        <v>0.62383412300598484</v>
+        <v>0.31350729008780043</v>
       </c>
       <c r="O52">
-        <v>0.93959842340631794</v>
+        <v>1.0178902107800141</v>
       </c>
       <c r="P52">
-        <v>0.35389031157210088</v>
+        <v>0.26152907945451132</v>
       </c>
       <c r="Q52">
-        <v>0.37529044001384543</v>
+        <v>0.91830002607555405</v>
       </c>
       <c r="R52">
-        <v>0.1364596114383532</v>
+        <v>0.94944559848580545</v>
       </c>
       <c r="S52">
-        <v>0.44983344446415618</v>
+        <v>0.25572812859930433</v>
       </c>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.3">
@@ -3578,31 +3578,31 @@
         <v>24</v>
       </c>
       <c r="K53">
-        <v>0.41752384402533482</v>
+        <v>1.2283445648083871</v>
       </c>
       <c r="L53">
-        <v>0.58300782154937814</v>
+        <v>0.78474201674546951</v>
       </c>
       <c r="M53">
-        <v>0.49504098287217763</v>
+        <v>1.0687487888222891</v>
       </c>
       <c r="N53">
-        <v>0.44919113695295171</v>
+        <v>0.80131212184142531</v>
       </c>
       <c r="O53">
-        <v>0.99817807372919642</v>
+        <v>1.2152748127470769</v>
       </c>
       <c r="P53">
-        <v>0.47127644569602889</v>
+        <v>0.79789394838327254</v>
       </c>
       <c r="Q53">
-        <v>0.47859353761911372</v>
+        <v>1.459721630680592</v>
       </c>
       <c r="R53">
-        <v>0.60143436426539665</v>
+        <v>0.79736907698352966</v>
       </c>
       <c r="S53">
-        <v>0.45487495279659562</v>
+        <v>0.65070103451780681</v>
       </c>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.3">
@@ -3634,34 +3634,34 @@
         <v>22</v>
       </c>
       <c r="J54">
-        <v>3480.4738739055051</v>
+        <v>913.34959263109363</v>
       </c>
       <c r="K54">
-        <v>1270.9760094578371</v>
+        <v>525.77483581175602</v>
       </c>
       <c r="L54">
-        <v>138.4410458558591</v>
+        <v>95.164362857710685</v>
       </c>
       <c r="M54">
-        <v>1396.3563006964989</v>
+        <v>567.04915647130599</v>
       </c>
       <c r="N54">
-        <v>758.85955119700839</v>
+        <v>415.54762719758321</v>
       </c>
       <c r="O54">
-        <v>126.93114124223909</v>
+        <v>126.88294238574829</v>
       </c>
       <c r="P54">
-        <v>18.92877594832785</v>
+        <v>11.248678291248449</v>
       </c>
       <c r="Q54">
-        <v>19.133037712452658</v>
+        <v>11.309480628835731</v>
       </c>
       <c r="R54">
-        <v>341.44770567062261</v>
+        <v>172.28384435441501</v>
       </c>
       <c r="S54">
-        <v>0.29991219549740861</v>
+        <v>1.354697542123388</v>
       </c>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.3">
@@ -3693,34 +3693,34 @@
         <v>22</v>
       </c>
       <c r="J55">
-        <v>3497.0458965335511</v>
+        <v>923.47008174948451</v>
       </c>
       <c r="K55">
-        <v>1276.4239163614659</v>
+        <v>530.39498076673465</v>
       </c>
       <c r="L55">
-        <v>152.5240228058457</v>
+        <v>104.1114186586487</v>
       </c>
       <c r="M55">
-        <v>1371.542853797629</v>
+        <v>550.23941533539937</v>
       </c>
       <c r="N55">
-        <v>775.04155783870146</v>
+        <v>415.64622008909458</v>
       </c>
       <c r="O55">
-        <v>128.5444904089178</v>
+        <v>128.02834717712139</v>
       </c>
       <c r="P55">
-        <v>16.11956997646039</v>
+        <v>11.5312785838275</v>
       </c>
       <c r="Q55">
-        <v>16.200574400188469</v>
+        <v>21.429969747226622</v>
       </c>
       <c r="R55">
-        <v>350.15179421878207</v>
+        <v>178.7183924781082</v>
       </c>
       <c r="S55">
-        <v>0.58447475535304227</v>
+        <v>1.3948694235097521</v>
       </c>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.3">
@@ -3752,34 +3752,34 @@
         <v>22</v>
       </c>
       <c r="J56">
-        <v>3512.4692885124559</v>
+        <v>932.93217907338601</v>
       </c>
       <c r="K56">
-        <v>1280.711433013144</v>
+        <v>534.31887934588428</v>
       </c>
       <c r="L56">
-        <v>163.4559987260017</v>
+        <v>106.7536998309597</v>
       </c>
       <c r="M56">
-        <v>1329.8033691187391</v>
+        <v>549.67637861970775</v>
       </c>
       <c r="N56">
-        <v>790.0846132794195</v>
+        <v>433.61947116807329</v>
       </c>
       <c r="O56">
-        <v>130.0352347231952</v>
+        <v>129.1366376262155</v>
       </c>
       <c r="P56">
-        <v>13.83029722893308</v>
+        <v>6.9998200604408831</v>
       </c>
       <c r="Q56">
-        <v>13.910250470594161</v>
+        <v>30.8920670711281</v>
       </c>
       <c r="R56">
-        <v>346.10026017603252</v>
+        <v>178.8823955911204</v>
       </c>
       <c r="S56">
-        <v>1.3880855253798401</v>
+        <v>0.58116060540211723</v>
       </c>
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.3">
@@ -3811,34 +3811,34 @@
         <v>22</v>
       </c>
       <c r="J57">
-        <v>3528.689130869896</v>
+        <v>942.41783946817861</v>
       </c>
       <c r="K57">
-        <v>1285.759736456921</v>
+        <v>538.23054312863974</v>
       </c>
       <c r="L57">
-        <v>186.88140131191739</v>
+        <v>126.3482192672712</v>
       </c>
       <c r="M57">
-        <v>1373.988066270701</v>
+        <v>572.63336091045062</v>
       </c>
       <c r="N57">
-        <v>807.6458620597665</v>
+        <v>439.90924573663551</v>
       </c>
       <c r="O57">
-        <v>131.86775819921351</v>
+        <v>130.34611636484681</v>
       </c>
       <c r="P57">
-        <v>14.213138481400151</v>
+        <v>7.7244273513934356</v>
       </c>
       <c r="Q57">
-        <v>14.333393132096489</v>
+        <v>40.377727465920707</v>
       </c>
       <c r="R57">
-        <v>389.80470806804158</v>
+        <v>201.7676204851615</v>
       </c>
       <c r="S57">
-        <v>0.28730444038247732</v>
+        <v>0.28420388671861418</v>
       </c>
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.3">
@@ -3870,34 +3870,34 @@
         <v>22</v>
       </c>
       <c r="J58">
-        <v>3545.5983680934978</v>
+        <v>952.53824666183857</v>
       </c>
       <c r="K58">
-        <v>1291.42084387109</v>
+        <v>542.73920560250633</v>
       </c>
       <c r="L58">
-        <v>202.74808185372649</v>
+        <v>132.637085175805</v>
       </c>
       <c r="M58">
-        <v>1394.225373241499</v>
+        <v>591.33019459551713</v>
       </c>
       <c r="N58">
-        <v>816.70197652799118</v>
+        <v>444.35094039410211</v>
       </c>
       <c r="O58">
-        <v>134.09990319517391</v>
+        <v>131.87031376455641</v>
       </c>
       <c r="P58">
-        <v>16.70723281592462</v>
+        <v>9.5236980715077166</v>
       </c>
       <c r="Q58">
-        <v>16.860619365521941</v>
+        <v>50.498134659580657</v>
       </c>
       <c r="R58">
-        <v>403.97533492918171</v>
+        <v>210.55561928677179</v>
       </c>
       <c r="S58">
-        <v>0.38726859279735271</v>
+        <v>0.36556661352306052</v>
       </c>
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.3">
@@ -3929,34 +3929,34 @@
         <v>22</v>
       </c>
       <c r="J59">
-        <v>3563.3094852628678</v>
+        <v>962.52654558995187</v>
       </c>
       <c r="K59">
-        <v>1297.80820904179</v>
+        <v>547.07304921741502</v>
       </c>
       <c r="L59">
-        <v>224.42480086494999</v>
+        <v>148.70993746104949</v>
       </c>
       <c r="M59">
-        <v>1388.7493208076839</v>
+        <v>585.05241930926104</v>
       </c>
       <c r="N59">
-        <v>847.99491937673372</v>
+        <v>455.58228156098193</v>
       </c>
       <c r="O59">
-        <v>136.77368239632531</v>
+        <v>133.49752024367999</v>
       </c>
       <c r="P59">
-        <v>17.61043008183259</v>
+        <v>9.920709781475189</v>
       </c>
       <c r="Q59">
-        <v>17.7500905820654</v>
+        <v>60.486433587693952</v>
       </c>
       <c r="R59">
-        <v>438.41969482408541</v>
+        <v>228.30851231062991</v>
       </c>
       <c r="S59">
-        <v>0.58757044717377849</v>
+        <v>0.25630087134942309</v>
       </c>
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.3">
@@ -3988,34 +3988,34 @@
         <v>22</v>
       </c>
       <c r="J60">
-        <v>3579.6969785113151</v>
+        <v>972.92707663137855</v>
       </c>
       <c r="K60">
-        <v>1302.904236868359</v>
+        <v>551.76967371831267</v>
       </c>
       <c r="L60">
-        <v>239.78685049510341</v>
+        <v>157.48953708600999</v>
       </c>
       <c r="M60">
-        <v>1307.1184917880059</v>
+        <v>552.45417146069326</v>
       </c>
       <c r="N60">
-        <v>858.56591393775216</v>
+        <v>472.08912492650848</v>
       </c>
       <c r="O60">
-        <v>139.39812731114901</v>
+        <v>135.42736818664841</v>
       </c>
       <c r="P60">
-        <v>16.374388423770551</v>
+        <v>9.5581167286098783</v>
       </c>
       <c r="Q60">
-        <v>16.497457989856311</v>
+        <v>70.886964629120669</v>
       </c>
       <c r="R60">
-        <v>450.34280518399419</v>
+        <v>236.62037629358349</v>
       </c>
       <c r="S60">
-        <v>0.94896418802770799</v>
+        <v>0.2559552181388941</v>
       </c>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.3">
@@ -4047,34 +4047,34 @@
         <v>22</v>
       </c>
       <c r="J61">
-        <v>3596.2043638047498</v>
+        <v>982.27160489533685</v>
       </c>
       <c r="K61">
-        <v>1308.057341899914</v>
+        <v>555.39254390902011</v>
       </c>
       <c r="L61">
-        <v>251.28427822310181</v>
+        <v>160.78714559634631</v>
       </c>
       <c r="M61">
-        <v>1482.4332002154781</v>
+        <v>605.96602329899054</v>
       </c>
       <c r="N61">
-        <v>871.65724386079125</v>
+        <v>490.14859527085707</v>
       </c>
       <c r="O61">
-        <v>142.33174293633371</v>
+        <v>137.1908751175236</v>
       </c>
       <c r="P61">
-        <v>14.456712693991911</v>
+        <v>8.9511403645114047</v>
       </c>
       <c r="Q61">
-        <v>14.56577833723891</v>
+        <v>80.231492893078965</v>
       </c>
       <c r="R61">
-        <v>448.15489455325161</v>
+        <v>237.02088127349529</v>
       </c>
       <c r="S61">
-        <v>0.28272814968484722</v>
+        <v>0.96886603294053253</v>
       </c>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.3">
@@ -4106,34 +4106,34 @@
         <v>22</v>
       </c>
       <c r="J62">
-        <v>3612.4731196298608</v>
+        <v>992.37274911489692</v>
       </c>
       <c r="K62">
-        <v>1312.92208977786</v>
+        <v>559.73945657237346</v>
       </c>
       <c r="L62">
-        <v>270.51109807994578</v>
+        <v>177.42087869640179</v>
       </c>
       <c r="M62">
-        <v>1335.6014956592501</v>
+        <v>554.81513147249188</v>
       </c>
       <c r="N62">
-        <v>879.30233753800405</v>
+        <v>477.95941008561329</v>
       </c>
       <c r="O62">
-        <v>145.46100263881809</v>
+        <v>139.41919258579401</v>
       </c>
       <c r="P62">
-        <v>15.43215835292332</v>
+        <v>8.3540186114544603</v>
       </c>
       <c r="Q62">
-        <v>15.573084279231191</v>
+        <v>90.33263711263902</v>
       </c>
       <c r="R62">
-        <v>474.72296551818448</v>
+        <v>252.48199620708999</v>
       </c>
       <c r="S62">
-        <v>0.30325178602742547</v>
+        <v>0.35537133738265009</v>
       </c>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.3">
@@ -4165,34 +4165,34 @@
         <v>22</v>
       </c>
       <c r="J63">
-        <v>3629.1725180851231</v>
+        <v>1003.513100491997</v>
       </c>
       <c r="K63">
-        <v>1318.2077892522741</v>
+        <v>565.05986934443217</v>
       </c>
       <c r="L63">
-        <v>285.60463802635201</v>
+        <v>184.37887530116799</v>
       </c>
       <c r="M63">
-        <v>1434.779915673251</v>
+        <v>600.1448662458763</v>
       </c>
       <c r="N63">
-        <v>897.61297828233216</v>
+        <v>488.65285246492323</v>
       </c>
       <c r="O63">
-        <v>149.02701395407939</v>
+        <v>142.26632458669411</v>
       </c>
       <c r="P63">
-        <v>15.670160546082471</v>
+        <v>11.04615304879481</v>
       </c>
       <c r="Q63">
-        <v>15.82719803024305</v>
+        <v>101.4729884897386</v>
       </c>
       <c r="R63">
-        <v>485.17425465501378</v>
+        <v>259.97549790948312</v>
       </c>
       <c r="S63">
-        <v>0.2606930534313795</v>
+        <v>0.72483797094529112</v>
       </c>
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.3">
@@ -4224,34 +4224,34 @@
         <v>22</v>
       </c>
       <c r="J64">
-        <v>3644.2246446667609</v>
+        <v>1013.530086128269</v>
       </c>
       <c r="K64">
-        <v>1321.852759647853</v>
+        <v>569.25446495967651</v>
       </c>
       <c r="L64">
-        <v>298.24108648548321</v>
+        <v>191.2262458122969</v>
       </c>
       <c r="M64">
-        <v>1441.016391069508</v>
+        <v>601.1657727226044</v>
       </c>
       <c r="N64">
-        <v>922.62647279870566</v>
+        <v>497.79861409474063</v>
       </c>
       <c r="O64">
-        <v>152.2805466761379</v>
+        <v>144.88246101011919</v>
       </c>
       <c r="P64">
-        <v>14.563566457892771</v>
+        <v>10.47551557963955</v>
       </c>
       <c r="Q64">
-        <v>14.73618836495451</v>
+        <v>111.4899741260114</v>
       </c>
       <c r="R64">
-        <v>490.8854266504722</v>
+        <v>266.08785485108001</v>
       </c>
       <c r="S64">
-        <v>1.6959519338763021</v>
+        <v>0.78737602662896222</v>
       </c>
     </row>
     <row r="65" spans="1:19" x14ac:dyDescent="0.3">
@@ -4283,34 +4283,34 @@
         <v>22</v>
       </c>
       <c r="J65">
-        <v>3659.8603334637251</v>
+        <v>1022.738895276989</v>
       </c>
       <c r="K65">
-        <v>1326.0145965362501</v>
+        <v>572.62720325500095</v>
       </c>
       <c r="L65">
-        <v>317.93333270379833</v>
+        <v>204.94648995575449</v>
       </c>
       <c r="M65">
-        <v>1456.0713790561449</v>
+        <v>616.4565812139881</v>
       </c>
       <c r="N65">
-        <v>943.6019139375569</v>
+        <v>517.99553350243514</v>
       </c>
       <c r="O65">
-        <v>156.1551584324545</v>
+        <v>147.3235770415358</v>
       </c>
       <c r="P65">
-        <v>13.267455940564041</v>
+        <v>7.3448539070513634</v>
       </c>
       <c r="Q65">
-        <v>13.44283052662426</v>
+        <v>120.6987832747306</v>
       </c>
       <c r="R65">
-        <v>524.05181129455332</v>
+        <v>282.99697032791812</v>
       </c>
       <c r="S65">
-        <v>0.40660112041337798</v>
+        <v>0.7258059392128261</v>
       </c>
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.3">
@@ -4342,31 +4342,31 @@
         <v>22</v>
       </c>
       <c r="K66">
-        <v>1299.4215801820631</v>
+        <v>549.364558802646</v>
       </c>
       <c r="L66">
-        <v>227.65305295267379</v>
+        <v>149.16449130828519</v>
       </c>
       <c r="M66">
-        <v>1392.6405131161989</v>
+        <v>578.91528930469065</v>
       </c>
       <c r="N66">
-        <v>847.47461171956365</v>
+        <v>462.44165970762901</v>
       </c>
       <c r="O66">
-        <v>139.40881684283639</v>
+        <v>135.52263967420691</v>
       </c>
       <c r="P66">
-        <v>15.59782391234198</v>
+        <v>9.3898675316628868</v>
       </c>
       <c r="Q66">
-        <v>15.73587526592228</v>
+        <v>65.842221140475417</v>
       </c>
       <c r="R66">
-        <v>428.60263797851798</v>
+        <v>225.47499678073811</v>
       </c>
       <c r="S66">
-        <v>0.61940051567041154</v>
+        <v>0.67125095565629256</v>
       </c>
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.3">
@@ -4398,34 +4398,34 @@
         <v>24</v>
       </c>
       <c r="J67">
-        <v>3480.4738739055051</v>
+        <v>913.34959263109363</v>
       </c>
       <c r="K67">
-        <v>1.018199302807727</v>
+        <v>4.0843217553848854</v>
       </c>
       <c r="L67">
-        <v>0.28279423044976332</v>
+        <v>1.082888501095832</v>
       </c>
       <c r="M67">
-        <v>1.78577705561433</v>
+        <v>4.268641154653352</v>
       </c>
       <c r="N67">
-        <v>0.26938636996420018</v>
+        <v>2.0503766558459828</v>
       </c>
       <c r="O67">
-        <v>3.5632973829977259</v>
+        <v>3.0889573311480669</v>
       </c>
       <c r="P67">
-        <v>2.1793485449469192</v>
+        <v>1.533104954661231</v>
       </c>
       <c r="Q67">
-        <v>2.255712315834026</v>
+        <v>1.4769580709476231</v>
       </c>
       <c r="R67">
-        <v>0.37502910570001291</v>
+        <v>1.3362063421952199</v>
       </c>
       <c r="S67">
-        <v>0.35739482867444211</v>
+        <v>1.231089023776619</v>
       </c>
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.3">
@@ -4457,34 +4457,34 @@
         <v>24</v>
       </c>
       <c r="J68">
-        <v>3497.0458965335511</v>
+        <v>923.47008174948451</v>
       </c>
       <c r="K68">
-        <v>0.78921583084383085</v>
+        <v>2.5403931851265318</v>
       </c>
       <c r="L68">
-        <v>0.46311617223861351</v>
+        <v>0.26591266829629462</v>
       </c>
       <c r="M68">
-        <v>1.752483776000866</v>
+        <v>3.2326592170178579</v>
       </c>
       <c r="N68">
-        <v>0.6235794822967935</v>
+        <v>0.54592400431948329</v>
       </c>
       <c r="O68">
-        <v>3.335116572844282</v>
+        <v>2.795069600589442</v>
       </c>
       <c r="P68">
-        <v>0.31162278177702618</v>
+        <v>0.31514698770620009</v>
       </c>
       <c r="Q68">
-        <v>0.33265155643454342</v>
+        <v>0.27931351359816869</v>
       </c>
       <c r="R68">
-        <v>0.34925151456498088</v>
+        <v>0.32082720201351028</v>
       </c>
       <c r="S68">
-        <v>0.46029109222459491</v>
+        <v>1.6104626704390339</v>
       </c>
     </row>
     <row r="69" spans="1:19" x14ac:dyDescent="0.3">
@@ -4516,34 +4516,34 @@
         <v>24</v>
       </c>
       <c r="J69">
-        <v>3512.4692885124559</v>
+        <v>932.93217907338601</v>
       </c>
       <c r="K69">
-        <v>0.63936835479703213</v>
+        <v>2.1412389397458669</v>
       </c>
       <c r="L69">
-        <v>1.163804502542567</v>
+        <v>0.67135241922828581</v>
       </c>
       <c r="M69">
-        <v>1.43625719112498</v>
+        <v>2.754778804889026</v>
       </c>
       <c r="N69">
-        <v>1.052353554523036</v>
+        <v>0.3712450327991067</v>
       </c>
       <c r="O69">
-        <v>3.1446447232745691</v>
+        <v>2.7430585098590541</v>
       </c>
       <c r="P69">
-        <v>1.1973037367795669</v>
+        <v>1.658009711097483</v>
       </c>
       <c r="Q69">
-        <v>1.1794558919371489</v>
+        <v>0.37407824136858348</v>
       </c>
       <c r="R69">
-        <v>1.217002197854016</v>
+        <v>0.60527059213119228</v>
       </c>
       <c r="S69">
-        <v>1.009556325002483</v>
+        <v>0.30769222621495301</v>
       </c>
     </row>
     <row r="70" spans="1:19" x14ac:dyDescent="0.3">
@@ -4575,34 +4575,34 @@
         <v>24</v>
       </c>
       <c r="J70">
-        <v>3528.689130869896</v>
+        <v>942.41783946817861</v>
       </c>
       <c r="K70">
-        <v>0.70214643826360512</v>
+        <v>2.1332622930502669</v>
       </c>
       <c r="L70">
-        <v>0.25464066498836863</v>
+        <v>0.37648356312296061</v>
       </c>
       <c r="M70">
-        <v>1.6953929139129129</v>
+        <v>2.650408525315624</v>
       </c>
       <c r="N70">
-        <v>0.30904591971674122</v>
+        <v>0.39868516196686421</v>
       </c>
       <c r="O70">
-        <v>3.216671286761847</v>
+        <v>2.74545407287507</v>
       </c>
       <c r="P70">
-        <v>0.34688497848536132</v>
+        <v>0.53780808014309656</v>
       </c>
       <c r="Q70">
-        <v>0.33376280329150509</v>
+        <v>0.36655565248712491</v>
       </c>
       <c r="R70">
-        <v>0.32126617661831308</v>
+        <v>0.59908129161591017</v>
       </c>
       <c r="S70">
-        <v>0.26145134274958609</v>
+        <v>0.33548168887083751</v>
       </c>
     </row>
     <row r="71" spans="1:19" x14ac:dyDescent="0.3">
@@ -4634,34 +4634,34 @@
         <v>24</v>
       </c>
       <c r="J71">
-        <v>3545.5983680934978</v>
+        <v>952.53824666183857</v>
       </c>
       <c r="K71">
-        <v>0.87132412685975047</v>
+        <v>2.4685332003037321</v>
       </c>
       <c r="L71">
-        <v>0.2713655381010498</v>
+        <v>0.13239267501767141</v>
       </c>
       <c r="M71">
-        <v>1.581381054689132</v>
+        <v>3.015813509146906</v>
       </c>
       <c r="N71">
-        <v>0.3657299394711343</v>
+        <v>0.80836996937207406</v>
       </c>
       <c r="O71">
-        <v>3.2941306003563859</v>
+        <v>2.80114008898108</v>
       </c>
       <c r="P71">
-        <v>0.82987957358778641</v>
+        <v>0.49390386099238409</v>
       </c>
       <c r="Q71">
-        <v>0.91187032582522842</v>
+        <v>0.27930663192074279</v>
       </c>
       <c r="R71">
-        <v>0.4054248004142228</v>
+        <v>0.14559595095002251</v>
       </c>
       <c r="S71">
-        <v>0.50981385244910793</v>
+        <v>0.61422421919551018</v>
       </c>
     </row>
     <row r="72" spans="1:19" x14ac:dyDescent="0.3">
@@ -4693,34 +4693,34 @@
         <v>24</v>
       </c>
       <c r="J72">
-        <v>3563.3094852628678</v>
+        <v>962.52654558995187</v>
       </c>
       <c r="K72">
-        <v>1.2276829353831451</v>
+        <v>2.3667747770216732</v>
       </c>
       <c r="L72">
-        <v>0.39033683019742249</v>
+        <v>0.12846447929312119</v>
       </c>
       <c r="M72">
-        <v>1.9715654218828369</v>
+        <v>2.887066026617398</v>
       </c>
       <c r="N72">
-        <v>0.36678793016547312</v>
+        <v>0.33651925945074512</v>
       </c>
       <c r="O72">
-        <v>3.419701527392331</v>
+        <v>2.7915154012141201</v>
       </c>
       <c r="P72">
-        <v>1.0754656563783309</v>
+        <v>0.37854080495991721</v>
       </c>
       <c r="Q72">
-        <v>1.1099525618064321</v>
+        <v>0.2721538634271502</v>
       </c>
       <c r="R72">
-        <v>0.35165146149392079</v>
+        <v>0.18534944678309781</v>
       </c>
       <c r="S72">
-        <v>0.65487003884000172</v>
+        <v>0.34234366947487449</v>
       </c>
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.3">
@@ -4752,34 +4752,34 @@
         <v>24</v>
       </c>
       <c r="J73">
-        <v>3579.6969785113151</v>
+        <v>972.92707663137855</v>
       </c>
       <c r="K73">
-        <v>0.71795163956895891</v>
+        <v>2.6195226751012108</v>
       </c>
       <c r="L73">
-        <v>0.64378194340481842</v>
+        <v>0.2386178400042763</v>
       </c>
       <c r="M73">
-        <v>1.502918946431254</v>
+        <v>3.1718648161867868</v>
       </c>
       <c r="N73">
-        <v>1.007349163184629</v>
+        <v>0.43813771606587132</v>
       </c>
       <c r="O73">
-        <v>3.178859885073162</v>
+        <v>2.8356856886373212</v>
       </c>
       <c r="P73">
-        <v>0.36016032818368487</v>
+        <v>0.32081465609076409</v>
       </c>
       <c r="Q73">
-        <v>0.35930709819360679</v>
+        <v>0.318479266627122</v>
       </c>
       <c r="R73">
-        <v>1.002112126254793</v>
+        <v>0.14425835967411341</v>
       </c>
       <c r="S73">
-        <v>0.79116582084284348</v>
+        <v>0.58633472880337756</v>
       </c>
     </row>
     <row r="74" spans="1:19" x14ac:dyDescent="0.3">
@@ -4811,34 +4811,34 @@
         <v>24</v>
       </c>
       <c r="J74">
-        <v>3596.2043638047498</v>
+        <v>982.27160489533685</v>
       </c>
       <c r="K74">
-        <v>0.74016604919254103</v>
+        <v>1.9879937848269329</v>
       </c>
       <c r="L74">
-        <v>0.40953988368696248</v>
+        <v>0.81317786890872501</v>
       </c>
       <c r="M74">
-        <v>1.4751171347453831</v>
+        <v>2.527550385730577</v>
       </c>
       <c r="N74">
-        <v>0.26550685276551511</v>
+        <v>0.39412451499457068</v>
       </c>
       <c r="O74">
-        <v>3.1869334985214191</v>
+        <v>2.741263193940179</v>
       </c>
       <c r="P74">
-        <v>0.6358891610881815</v>
+        <v>0.41286089047519953</v>
       </c>
       <c r="Q74">
-        <v>0.66127283953944949</v>
+        <v>0.41380141153672179</v>
       </c>
       <c r="R74">
-        <v>0.81974825485286473</v>
+        <v>0.83451751747710468</v>
       </c>
       <c r="S74">
-        <v>0.26220739889047479</v>
+        <v>0.71040892916927567</v>
       </c>
     </row>
     <row r="75" spans="1:19" x14ac:dyDescent="0.3">
@@ -4870,34 +4870,34 @@
         <v>24</v>
       </c>
       <c r="J75">
-        <v>3612.4731196298608</v>
+        <v>992.37274911489692</v>
       </c>
       <c r="K75">
-        <v>0.68604965005958762</v>
+        <v>2.36875724539183</v>
       </c>
       <c r="L75">
-        <v>0.68241403317487159</v>
+        <v>0.12829921674573891</v>
       </c>
       <c r="M75">
-        <v>1.5295992183372009</v>
+        <v>3.106991362322379</v>
       </c>
       <c r="N75">
-        <v>0.32862377922896269</v>
+        <v>0.60294481088179519</v>
       </c>
       <c r="O75">
-        <v>3.1689456579173059</v>
+        <v>2.8083714150710528</v>
       </c>
       <c r="P75">
-        <v>0.30160478590141221</v>
+        <v>0.28801494616204909</v>
       </c>
       <c r="Q75">
-        <v>0.32729198691618161</v>
+        <v>0.27768854209633781</v>
       </c>
       <c r="R75">
-        <v>0.46816541067993478</v>
+        <v>0.1612063510250718</v>
       </c>
       <c r="S75">
-        <v>0.27210566860861862</v>
+        <v>0.46049131463642462</v>
       </c>
     </row>
     <row r="76" spans="1:19" x14ac:dyDescent="0.3">
@@ -4929,34 +4929,34 @@
         <v>24</v>
       </c>
       <c r="J76">
-        <v>3629.1725180851231</v>
+        <v>1003.513100491997</v>
       </c>
       <c r="K76">
-        <v>0.78032882396428138</v>
+        <v>3.1530767891422729</v>
       </c>
       <c r="L76">
-        <v>0.41122701386409399</v>
+        <v>0.66882490561975516</v>
       </c>
       <c r="M76">
-        <v>1.526702558294242</v>
+        <v>3.414420022548037</v>
       </c>
       <c r="N76">
-        <v>0.26696840279957229</v>
+        <v>1.1244219677708009</v>
       </c>
       <c r="O76">
-        <v>3.221277329756024</v>
+        <v>2.9513878599190648</v>
       </c>
       <c r="P76">
-        <v>0.29535388141212221</v>
+        <v>1.1401163430164629</v>
       </c>
       <c r="Q76">
-        <v>0.3087335700445718</v>
+        <v>0.72908183916375557</v>
       </c>
       <c r="R76">
-        <v>0.31388674325850902</v>
+        <v>0.527859544283656</v>
       </c>
       <c r="S76">
-        <v>0.30471441663267668</v>
+        <v>0.7021818645378578</v>
       </c>
     </row>
     <row r="77" spans="1:19" x14ac:dyDescent="0.3">
@@ -4988,34 +4988,34 @@
         <v>24</v>
       </c>
       <c r="J77">
-        <v>3644.2246446667609</v>
+        <v>1013.530086128269</v>
       </c>
       <c r="K77">
-        <v>0.68368342114591729</v>
+        <v>2.27560252923131</v>
       </c>
       <c r="L77">
-        <v>1.8291637150966551</v>
+        <v>0.30677140076956783</v>
       </c>
       <c r="M77">
-        <v>1.480658987756196</v>
+        <v>3.080400606520131</v>
       </c>
       <c r="N77">
-        <v>1.2992126681603939</v>
+        <v>0.39277921129612442</v>
       </c>
       <c r="O77">
-        <v>3.093941619873859</v>
+        <v>2.800072378942625</v>
       </c>
       <c r="P77">
-        <v>0.77457063172652663</v>
+        <v>0.27378901749736018</v>
       </c>
       <c r="Q77">
-        <v>0.74874720882416923</v>
+        <v>0.2721718280435369</v>
       </c>
       <c r="R77">
-        <v>1.694989427823373</v>
+        <v>0.37481915785190939</v>
       </c>
       <c r="S77">
-        <v>1.3607695013703931</v>
+        <v>0.84104782423408353</v>
       </c>
     </row>
     <row r="78" spans="1:19" x14ac:dyDescent="0.3">
@@ -5047,34 +5047,34 @@
         <v>24</v>
       </c>
       <c r="J78">
-        <v>3659.8603334637251</v>
+        <v>1022.738895276989</v>
       </c>
       <c r="K78">
-        <v>0.62597243321539242</v>
+        <v>1.8612574029609019</v>
       </c>
       <c r="L78">
-        <v>0.31906016407373189</v>
+        <v>0.77105844612363739</v>
       </c>
       <c r="M78">
-        <v>1.393569429132423</v>
+        <v>2.3557804079046818</v>
       </c>
       <c r="N78">
-        <v>0.2461479543154905</v>
+        <v>0.45174434144927472</v>
       </c>
       <c r="O78">
-        <v>3.1477504699253829</v>
+        <v>2.7331541998694409</v>
       </c>
       <c r="P78">
-        <v>0.55403105853230283</v>
+        <v>1.2704305630053809</v>
       </c>
       <c r="Q78">
-        <v>0.56023306540226958</v>
+        <v>0.46261884891987493</v>
       </c>
       <c r="R78">
-        <v>0.34799346687040411</v>
+        <v>0.86641149280045382</v>
       </c>
       <c r="S78">
-        <v>0.52350523457580278</v>
+        <v>0.4368730608759267</v>
       </c>
     </row>
     <row r="79" spans="1:19" x14ac:dyDescent="0.3">
@@ -5106,31 +5106,31 @@
         <v>24</v>
       </c>
       <c r="K79">
-        <v>0.79017408384181387</v>
+        <v>2.5000612147739512</v>
       </c>
       <c r="L79">
-        <v>0.59343705765157651</v>
+        <v>0.46535366535215572</v>
       </c>
       <c r="M79">
-        <v>1.5942853073268131</v>
+        <v>3.0388645699043959</v>
       </c>
       <c r="N79">
-        <v>0.53339100138266182</v>
+        <v>0.65960605385105786</v>
       </c>
       <c r="O79">
-        <v>3.2476058795578582</v>
+        <v>2.8195941450872102</v>
       </c>
       <c r="P79">
-        <v>0.73850959323326837</v>
+        <v>0.71854506798396078</v>
       </c>
       <c r="Q79">
-        <v>0.75741593533742757</v>
+        <v>0.46018397584472848</v>
       </c>
       <c r="R79">
-        <v>0.63887672386544536</v>
+        <v>0.50845027073343863</v>
       </c>
       <c r="S79">
-        <v>0.56398712673841878</v>
+        <v>0.68155260168573106</v>
       </c>
     </row>
     <row r="80" spans="1:19" x14ac:dyDescent="0.3">
@@ -5162,34 +5162,34 @@
         <v>22</v>
       </c>
       <c r="J80">
-        <v>-3271.4163406127</v>
+        <v>2000.469666259582</v>
       </c>
       <c r="K80">
-        <v>230.11292845159909</v>
+        <v>1226.803706113026</v>
       </c>
       <c r="L80">
-        <v>37.89663792399422</v>
+        <v>136.28382918312909</v>
       </c>
       <c r="M80">
-        <v>337.47619576331221</v>
+        <v>1260.582295814565</v>
       </c>
       <c r="N80">
-        <v>62.778631673286817</v>
+        <v>1090.2654932941521</v>
       </c>
       <c r="O80">
-        <v>157.6776786374264</v>
+        <v>190.10795278427341</v>
       </c>
       <c r="P80">
-        <v>2.472509702699627</v>
+        <v>21.942095253256859</v>
       </c>
       <c r="Q80">
-        <v>2.5544362010277109</v>
+        <v>21.904449880061879</v>
       </c>
       <c r="R80">
-        <v>17.27959354358703</v>
+        <v>371.89229203108778</v>
       </c>
       <c r="S80">
-        <v>0.23350488626771271</v>
+        <v>0.5869519170119275</v>
       </c>
     </row>
     <row r="81" spans="1:19" x14ac:dyDescent="0.3">
@@ -5221,34 +5221,34 @@
         <v>22</v>
       </c>
       <c r="J81">
-        <v>-3273.1373129316598</v>
+        <v>2023.6219531813711</v>
       </c>
       <c r="K81">
-        <v>229.78919364817449</v>
+        <v>1236.870576372984</v>
       </c>
       <c r="L81">
-        <v>45.064107290419159</v>
+        <v>169.99444658188179</v>
       </c>
       <c r="M81">
-        <v>352.91178628079501</v>
+        <v>1289.672984094623</v>
       </c>
       <c r="N81">
-        <v>66.53960160397547</v>
+        <v>1099.962429194278</v>
       </c>
       <c r="O81">
-        <v>157.9669556566005</v>
+        <v>197.1562915791072</v>
       </c>
       <c r="P81">
-        <v>1.0167245373294731</v>
+        <v>21.54233444724662</v>
       </c>
       <c r="Q81">
-        <v>1.0187933445845669</v>
+        <v>45.056736801850022</v>
       </c>
       <c r="R81">
-        <v>20.73397302520393</v>
+        <v>417.0453470494848</v>
       </c>
       <c r="S81">
-        <v>0.46392349495176349</v>
+        <v>0.43789580638179082</v>
       </c>
     </row>
     <row r="82" spans="1:19" x14ac:dyDescent="0.3">
@@ -5280,34 +5280,34 @@
         <v>22</v>
       </c>
       <c r="J82">
-        <v>-3274.898425748504</v>
+        <v>2047.0823163542659</v>
       </c>
       <c r="K82">
-        <v>229.49919151143831</v>
+        <v>1247.1340935586841</v>
       </c>
       <c r="L82">
-        <v>42.234230827312757</v>
+        <v>181.26494115601449</v>
       </c>
       <c r="M82">
-        <v>350.49388678437731</v>
+        <v>1298.0061536638229</v>
       </c>
       <c r="N82">
-        <v>67.620354016183569</v>
+        <v>1088.804976505387</v>
       </c>
       <c r="O82">
-        <v>158.42515747586719</v>
+        <v>204.9898766760945</v>
       </c>
       <c r="P82">
-        <v>2.0197811204475169</v>
+        <v>23.65560826659933</v>
       </c>
       <c r="Q82">
-        <v>1.9521339069912109</v>
+        <v>68.517099974745761</v>
       </c>
       <c r="R82">
-        <v>19.280693674137542</v>
+        <v>422.25868670457987</v>
       </c>
       <c r="S82">
-        <v>0.35836471952664922</v>
+        <v>0.28294149253772682</v>
       </c>
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.3">
@@ -5339,34 +5339,34 @@
         <v>22</v>
       </c>
       <c r="J83">
-        <v>-3276.7062388454101</v>
+        <v>2070.49032564141</v>
       </c>
       <c r="K83">
-        <v>229.24808002984571</v>
+        <v>1257.241026207663</v>
       </c>
       <c r="L83">
-        <v>41.441087506917647</v>
+        <v>211.08279137462259</v>
       </c>
       <c r="M83">
-        <v>361.3732388938684</v>
+        <v>1330.3627474437619</v>
       </c>
       <c r="N83">
-        <v>72.545416188562115</v>
+        <v>1201.1581493912611</v>
       </c>
       <c r="O83">
-        <v>158.98566317537669</v>
+        <v>213.3932715616715</v>
       </c>
       <c r="P83">
-        <v>0.75394036249665897</v>
+        <v>23.235967526665981</v>
       </c>
       <c r="Q83">
-        <v>0.75993491731447715</v>
+        <v>91.925109261889801</v>
       </c>
       <c r="R83">
-        <v>21.44125472484269</v>
+        <v>441.02629052221192</v>
       </c>
       <c r="S83">
-        <v>0.23099785939229839</v>
+        <v>0.24232250559884411</v>
       </c>
     </row>
     <row r="84" spans="1:19" x14ac:dyDescent="0.3">
@@ -5398,34 +5398,34 @@
         <v>22</v>
       </c>
       <c r="J84">
-        <v>-3279.7499434251049</v>
+        <v>2091.0367914009498</v>
       </c>
       <c r="K84">
-        <v>230.12464708300541</v>
+        <v>1264.438634961808</v>
       </c>
       <c r="L84">
-        <v>43.410297683059831</v>
+        <v>221.78728903006419</v>
       </c>
       <c r="M84">
-        <v>355.87770132910788</v>
+        <v>1379.5212897099079</v>
       </c>
       <c r="N84">
-        <v>74.105346562865577</v>
+        <v>1133.619364962552</v>
       </c>
       <c r="O84">
-        <v>159.8991658934321</v>
+        <v>220.260549427623</v>
       </c>
       <c r="P84">
-        <v>2.5937309813308538</v>
+        <v>19.808405949773409</v>
       </c>
       <c r="Q84">
-        <v>2.5188419415148382</v>
+        <v>112.4715750214292</v>
       </c>
       <c r="R84">
-        <v>20.97711882160716</v>
+        <v>459.83664201586402</v>
       </c>
       <c r="S84">
-        <v>1.130553471697394</v>
+        <v>2.1600252886367519</v>
       </c>
     </row>
     <row r="85" spans="1:19" x14ac:dyDescent="0.3">
@@ -5457,34 +5457,34 @@
         <v>22</v>
       </c>
       <c r="J85">
-        <v>-3283.672906992756</v>
+        <v>2109.1149513201171</v>
       </c>
       <c r="K85">
-        <v>231.81989070883029</v>
+        <v>1269.1894399070179</v>
       </c>
       <c r="L85">
-        <v>49.840320682331722</v>
+        <v>252.00275833618889</v>
       </c>
       <c r="M85">
-        <v>335.62207986827281</v>
+        <v>1277.898859320261</v>
       </c>
       <c r="N85">
-        <v>75.493102767976737</v>
+        <v>1162.617678676155</v>
       </c>
       <c r="O85">
-        <v>161.06972144002231</v>
+        <v>225.83733903958279</v>
       </c>
       <c r="P85">
-        <v>4.6871295676454556</v>
+        <v>14.766948410040751</v>
       </c>
       <c r="Q85">
-        <v>4.6252226247372308</v>
+        <v>130.54973494059649</v>
       </c>
       <c r="R85">
-        <v>26.231549660263621</v>
+        <v>489.74353033336263</v>
       </c>
       <c r="S85">
-        <v>0.30134801170458558</v>
+        <v>0.56403631095575202</v>
       </c>
     </row>
     <row r="86" spans="1:19" x14ac:dyDescent="0.3">
@@ -5516,34 +5516,34 @@
         <v>22</v>
       </c>
       <c r="J86">
-        <v>-3288.3071835253731</v>
+        <v>2125.5339481833712</v>
       </c>
       <c r="K86">
-        <v>234.2984908387462</v>
+        <v>1272.2152132316801</v>
       </c>
       <c r="L86">
-        <v>51.417965967737352</v>
+        <v>257.85843988658161</v>
       </c>
       <c r="M86">
-        <v>326.17465696435102</v>
+        <v>1321.268741954666</v>
       </c>
       <c r="N86">
-        <v>78.789713437323513</v>
+        <v>1162.011295956733</v>
       </c>
       <c r="O86">
-        <v>162.44285175295769</v>
+        <v>230.61231320120129</v>
       </c>
       <c r="P86">
-        <v>4.3314758880724016</v>
+        <v>14.98222148786741</v>
       </c>
       <c r="Q86">
-        <v>4.2056407199346042</v>
+        <v>146.96873180385069</v>
       </c>
       <c r="R86">
-        <v>28.0105797030063</v>
+        <v>490.73383985178418</v>
       </c>
       <c r="S86">
-        <v>0.35467656570072731</v>
+        <v>0.29239414558160398</v>
       </c>
     </row>
     <row r="87" spans="1:19" x14ac:dyDescent="0.3">
@@ -5575,34 +5575,34 @@
         <v>22</v>
       </c>
       <c r="J87">
-        <v>-3293.6281020290339</v>
+        <v>2142.15747878305</v>
       </c>
       <c r="K87">
-        <v>237.56935461977619</v>
+        <v>1275.455886499743</v>
       </c>
       <c r="L87">
-        <v>57.475156040207203</v>
+        <v>274.22964834398789</v>
       </c>
       <c r="M87">
-        <v>334.60010851198513</v>
+        <v>1345.487553499104</v>
       </c>
       <c r="N87">
-        <v>82.667117436462547</v>
+        <v>1210.9222277823419</v>
       </c>
       <c r="O87">
-        <v>164.01188714404429</v>
+        <v>235.95503003496631</v>
       </c>
       <c r="P87">
-        <v>5.0895865196324346</v>
+        <v>15.77621863132223</v>
       </c>
       <c r="Q87">
-        <v>4.9746879902899286</v>
+        <v>163.59226240352939</v>
       </c>
       <c r="R87">
-        <v>34.258664647005631</v>
+        <v>504.93220105426332</v>
       </c>
       <c r="S87">
-        <v>0.2263294209444621</v>
+        <v>0.5636275907439513</v>
       </c>
     </row>
     <row r="88" spans="1:19" x14ac:dyDescent="0.3">
@@ -5634,34 +5634,34 @@
         <v>22</v>
       </c>
       <c r="J88">
-        <v>-3299.5217098105691</v>
+        <v>2159.339960104227</v>
       </c>
       <c r="K88">
-        <v>241.51746552848431</v>
+        <v>1279.1633512376329</v>
       </c>
       <c r="L88">
-        <v>64.398831274177155</v>
+        <v>285.4370851772415</v>
       </c>
       <c r="M88">
-        <v>346.74864293059642</v>
+        <v>1315.1929805937491</v>
       </c>
       <c r="N88">
-        <v>85.112493302526048</v>
+        <v>1204.5342278968351</v>
       </c>
       <c r="O88">
-        <v>165.6885692752241</v>
+        <v>242.2106180278933</v>
       </c>
       <c r="P88">
-        <v>5.7918429540454888</v>
+        <v>17.73198928688694</v>
       </c>
       <c r="Q88">
-        <v>5.6835450408993884</v>
+        <v>180.77474372470601</v>
       </c>
       <c r="R88">
-        <v>39.130884068623352</v>
+        <v>525.79134553680342</v>
       </c>
       <c r="S88">
-        <v>0.25066334355565739</v>
+        <v>0.33087698497859402</v>
       </c>
     </row>
     <row r="89" spans="1:19" x14ac:dyDescent="0.3">
@@ -5693,34 +5693,34 @@
         <v>22</v>
       </c>
       <c r="J89">
-        <v>-3305.585779628595</v>
+        <v>2178.6097199489618</v>
       </c>
       <c r="K89">
-        <v>245.62208499212269</v>
+        <v>1284.845118089961</v>
       </c>
       <c r="L89">
-        <v>68.195949587022653</v>
+        <v>310.08772910974352</v>
       </c>
       <c r="M89">
-        <v>376.22017361930961</v>
+        <v>1339.080129811703</v>
       </c>
       <c r="N89">
-        <v>90.291762613542147</v>
+        <v>1237.6705515050789</v>
       </c>
       <c r="O89">
-        <v>167.3435348037377</v>
+        <v>250.64933372570701</v>
       </c>
       <c r="P89">
-        <v>5.8360570438979318</v>
+        <v>19.2051340695051</v>
       </c>
       <c r="Q89">
-        <v>5.7281812598174859</v>
+        <v>200.04450356944159</v>
       </c>
       <c r="R89">
-        <v>45.686744757938612</v>
+        <v>542.26871687678556</v>
       </c>
       <c r="S89">
-        <v>0.21917988318673931</v>
+        <v>1.327528304445792</v>
       </c>
     </row>
     <row r="90" spans="1:19" x14ac:dyDescent="0.3">
@@ -5752,34 +5752,34 @@
         <v>22</v>
       </c>
       <c r="J90">
-        <v>-3311.6486268320341</v>
+        <v>2196.985073320001</v>
       </c>
       <c r="K90">
-        <v>249.70379658247171</v>
+        <v>1289.6420725194471</v>
       </c>
       <c r="L90">
-        <v>76.230464226011009</v>
+        <v>544.94148681935985</v>
       </c>
       <c r="M90">
-        <v>354.06231154642188</v>
+        <v>1294.335951037878</v>
       </c>
       <c r="N90">
-        <v>94.18731451033716</v>
+        <v>1271.559885119894</v>
       </c>
       <c r="O90">
-        <v>168.87014273125169</v>
+        <v>258.95826197734459</v>
       </c>
       <c r="P90">
-        <v>5.5036181470860948</v>
+        <v>19.726985880599681</v>
       </c>
       <c r="Q90">
-        <v>5.4049117152348058</v>
+        <v>218.41985694048091</v>
       </c>
       <c r="R90">
-        <v>52.630112084522068</v>
+        <v>572.76169196426952</v>
       </c>
       <c r="S90">
-        <v>0.25773329098762238</v>
+        <v>1.2265826367996759</v>
       </c>
     </row>
     <row r="91" spans="1:19" x14ac:dyDescent="0.3">
@@ -5811,34 +5811,34 @@
         <v>22</v>
       </c>
       <c r="J91">
-        <v>-3317.8464358168758</v>
+        <v>2214.0317568714031</v>
       </c>
       <c r="K91">
-        <v>253.89324296280509</v>
+        <v>1293.0885761726281</v>
       </c>
       <c r="L91">
-        <v>83.158149750348059</v>
+        <v>549.14432335665265</v>
       </c>
       <c r="M91">
-        <v>358.37677915252351</v>
+        <v>1322.3448129624039</v>
       </c>
       <c r="N91">
-        <v>98.705971906180451</v>
+        <v>1279.6750114527799</v>
       </c>
       <c r="O91">
-        <v>170.31567412481459</v>
+        <v>266.61300005137178</v>
       </c>
       <c r="P91">
-        <v>5.6942120169215151</v>
+        <v>14.638572133875311</v>
       </c>
       <c r="Q91">
-        <v>5.6177903762025894</v>
+        <v>235.46654049188251</v>
       </c>
       <c r="R91">
-        <v>57.217982602866087</v>
+        <v>575.62012789035361</v>
       </c>
       <c r="S91">
-        <v>0.27445350722098039</v>
+        <v>0.46991267665552988</v>
       </c>
     </row>
     <row r="92" spans="1:19" x14ac:dyDescent="0.3">
@@ -5870,31 +5870,31 @@
         <v>22</v>
       </c>
       <c r="K92">
-        <v>236.93319724644161</v>
+        <v>1266.340641239356</v>
       </c>
       <c r="L92">
-        <v>55.063599896628233</v>
+        <v>282.84289736295568</v>
       </c>
       <c r="M92">
-        <v>349.16146347041013</v>
+        <v>1314.4795416588711</v>
       </c>
       <c r="N92">
-        <v>79.069735501601855</v>
+        <v>1178.5667743114541</v>
       </c>
       <c r="O92">
-        <v>162.7247501758963</v>
+        <v>228.06198650723641</v>
       </c>
       <c r="P92">
-        <v>3.8158840701337891</v>
+        <v>18.917706778636639</v>
       </c>
       <c r="Q92">
-        <v>3.75367666987907</v>
+        <v>134.64094540120541</v>
       </c>
       <c r="R92">
-        <v>31.90659594280034</v>
+        <v>484.4925593192375</v>
       </c>
       <c r="S92">
-        <v>0.35847737126138268</v>
+        <v>0.70709130502732842</v>
       </c>
     </row>
     <row r="93" spans="1:19" x14ac:dyDescent="0.3">
@@ -5926,34 +5926,34 @@
         <v>24</v>
       </c>
       <c r="J93">
-        <v>-3271.4163406127</v>
+        <v>2000.469666259582</v>
       </c>
       <c r="K93">
-        <v>5.1407466719098567</v>
+        <v>5.8877898764184273</v>
       </c>
       <c r="L93">
-        <v>1.5474164242424919</v>
+        <v>0.8629950081597263</v>
       </c>
       <c r="M93">
-        <v>6.0892483024815398</v>
+        <v>7.5594313600601986</v>
       </c>
       <c r="N93">
-        <v>1.9453648677020789</v>
+        <v>1.664432077421911</v>
       </c>
       <c r="O93">
-        <v>6.7672077991734918</v>
+        <v>6.0882474202800489</v>
       </c>
       <c r="P93">
-        <v>3.5740033024772622</v>
+        <v>1.605755637107694</v>
       </c>
       <c r="Q93">
-        <v>3.7827428754935659</v>
+        <v>1.715189408026687</v>
       </c>
       <c r="R93">
-        <v>0.96462555858181298</v>
+        <v>0.84703314128852292</v>
       </c>
       <c r="S93">
-        <v>0.2709755673805927</v>
+        <v>0.69496914608741789</v>
       </c>
     </row>
     <row r="94" spans="1:19" x14ac:dyDescent="0.3">
@@ -5985,34 +5985,34 @@
         <v>24</v>
       </c>
       <c r="J94">
-        <v>-3273.1373129316598</v>
+        <v>2023.6219531813711</v>
       </c>
       <c r="K94">
-        <v>4.3567232735436558</v>
+        <v>5.7974059026091798</v>
       </c>
       <c r="L94">
-        <v>2.015922679001021</v>
+        <v>0.95601379920317542</v>
       </c>
       <c r="M94">
-        <v>4.9457925086859502</v>
+        <v>6.3369089285224547</v>
       </c>
       <c r="N94">
-        <v>1.80671133611729</v>
+        <v>1.2782931018465209</v>
       </c>
       <c r="O94">
-        <v>6.5948364533354926</v>
+        <v>6.0817677097679956</v>
       </c>
       <c r="P94">
-        <v>0.72840441510175502</v>
+        <v>0.71101241445317354</v>
       </c>
       <c r="Q94">
-        <v>0.85085146461232442</v>
+        <v>1.778722393481138</v>
       </c>
       <c r="R94">
-        <v>2.0068650416063751</v>
+        <v>0.89863069107269977</v>
       </c>
       <c r="S94">
-        <v>0.38629392748454261</v>
+        <v>0.42271631648251551</v>
       </c>
     </row>
     <row r="95" spans="1:19" x14ac:dyDescent="0.3">
@@ -6044,34 +6044,34 @@
         <v>24</v>
       </c>
       <c r="J95">
-        <v>-3274.898425748504</v>
+        <v>2047.0823163542659</v>
       </c>
       <c r="K95">
-        <v>4.30343777720904</v>
+        <v>5.893345422222855</v>
       </c>
       <c r="L95">
-        <v>0.79761150754392562</v>
+        <v>0.68202640931702763</v>
       </c>
       <c r="M95">
-        <v>4.8821733839892429</v>
+        <v>6.6812062695642833</v>
       </c>
       <c r="N95">
-        <v>0.50535560064658458</v>
+        <v>0.87049436990181617</v>
       </c>
       <c r="O95">
-        <v>6.588615582115052</v>
+        <v>6.1165546881845163</v>
       </c>
       <c r="P95">
-        <v>0.47352808985943717</v>
+        <v>0.58042533185556133</v>
       </c>
       <c r="Q95">
-        <v>0.58377837356551943</v>
+        <v>1.4712622948757079</v>
       </c>
       <c r="R95">
-        <v>0.93185659562775203</v>
+        <v>0.67241006747350174</v>
       </c>
       <c r="S95">
-        <v>0.46162759974394008</v>
+        <v>0.28932899549495639</v>
       </c>
     </row>
     <row r="96" spans="1:19" x14ac:dyDescent="0.3">
@@ -6103,34 +6103,34 @@
         <v>24</v>
       </c>
       <c r="J96">
-        <v>-3276.7062388454101</v>
+        <v>2070.49032564141</v>
       </c>
       <c r="K96">
-        <v>4.257171388814263</v>
+        <v>5.8067306422247214</v>
       </c>
       <c r="L96">
-        <v>0.90264864440967396</v>
+        <v>0.77922345237655988</v>
       </c>
       <c r="M96">
-        <v>5.5107859163671193</v>
+        <v>7.3689578574896411</v>
       </c>
       <c r="N96">
-        <v>0.46389655283679182</v>
+        <v>0.897503964128191</v>
       </c>
       <c r="O96">
-        <v>6.5878609439238378</v>
+        <v>6.1133834887272824</v>
       </c>
       <c r="P96">
-        <v>0.41150808856899501</v>
+        <v>0.28249026214864431</v>
       </c>
       <c r="Q96">
-        <v>0.39588993739739842</v>
+        <v>1.52351147285594</v>
       </c>
       <c r="R96">
-        <v>0.95128621230055632</v>
+        <v>0.50274369247999073</v>
       </c>
       <c r="S96">
-        <v>0.24327579450382689</v>
+        <v>0.2615621233760107</v>
       </c>
     </row>
     <row r="97" spans="1:19" x14ac:dyDescent="0.3">
@@ -6162,34 +6162,34 @@
         <v>24</v>
       </c>
       <c r="J97">
-        <v>-3279.7499434251049</v>
+        <v>2091.0367914009498</v>
       </c>
       <c r="K97">
-        <v>3.8027257522266238</v>
+        <v>4.5774936802161648</v>
       </c>
       <c r="L97">
-        <v>1.688547001971068</v>
+        <v>3.314641541267326</v>
       </c>
       <c r="M97">
-        <v>5.2491322188645286</v>
+        <v>6.3559490708946216</v>
       </c>
       <c r="N97">
-        <v>1.5068795911441271</v>
+        <v>2.9993952470723149</v>
       </c>
       <c r="O97">
-        <v>6.4687519963226929</v>
+        <v>5.8201549489679278</v>
       </c>
       <c r="P97">
-        <v>0.77727423616757785</v>
+        <v>2.5307057056115849</v>
       </c>
       <c r="Q97">
-        <v>0.90606857520549455</v>
+        <v>4.3839782544736847</v>
       </c>
       <c r="R97">
-        <v>1.8056746669890591</v>
+        <v>2.3862689974906881</v>
       </c>
       <c r="S97">
-        <v>0.97475080011933746</v>
+        <v>2.3821359002457259</v>
       </c>
     </row>
     <row r="98" spans="1:19" x14ac:dyDescent="0.3">
@@ -6221,34 +6221,34 @@
         <v>24</v>
       </c>
       <c r="J98">
-        <v>-3283.672906992756</v>
+        <v>2109.1149513201171</v>
       </c>
       <c r="K98">
-        <v>3.5401672413073921</v>
+        <v>3.986127077195853</v>
       </c>
       <c r="L98">
-        <v>1.460220060933074</v>
+        <v>0.73375605805529909</v>
       </c>
       <c r="M98">
-        <v>4.7828352882857077</v>
+        <v>5.5702670802097236</v>
       </c>
       <c r="N98">
-        <v>1.210308388342441</v>
+        <v>4.2353814161751586</v>
       </c>
       <c r="O98">
-        <v>6.3914722121242944</v>
+        <v>5.5827718440224388</v>
       </c>
       <c r="P98">
-        <v>1.518324683000329</v>
+        <v>4.7805281587488047</v>
       </c>
       <c r="Q98">
-        <v>1.619509870223875</v>
+        <v>6.8522840948457713</v>
       </c>
       <c r="R98">
-        <v>1.3746096298462971</v>
+        <v>1.330521453888188</v>
       </c>
       <c r="S98">
-        <v>0.24876426529300791</v>
+        <v>0.59600926043295688</v>
       </c>
     </row>
     <row r="99" spans="1:19" x14ac:dyDescent="0.3">
@@ -6280,34 +6280,34 @@
         <v>24</v>
       </c>
       <c r="J99">
-        <v>-3288.3071835253731</v>
+        <v>2125.5339481833712</v>
       </c>
       <c r="K99">
-        <v>3.3936540464231921</v>
+        <v>3.825407707243123</v>
       </c>
       <c r="L99">
-        <v>2.238943179401824</v>
+        <v>1.521579406707263</v>
       </c>
       <c r="M99">
-        <v>4.6813032219437503</v>
+        <v>5.6569981756615952</v>
       </c>
       <c r="N99">
-        <v>0.88548179538527083</v>
+        <v>4.1103136222202714</v>
       </c>
       <c r="O99">
-        <v>6.3343121904205093</v>
+        <v>5.4351249346552084</v>
       </c>
       <c r="P99">
-        <v>0.49602396383122582</v>
+        <v>2.0926803071046098</v>
       </c>
       <c r="Q99">
-        <v>0.53674458365081623</v>
+        <v>8.5114471507589808</v>
       </c>
       <c r="R99">
-        <v>2.454646545751046</v>
+        <v>2.178533753693225</v>
       </c>
       <c r="S99">
-        <v>0.26643940785377218</v>
+        <v>0.30489891669836</v>
       </c>
     </row>
     <row r="100" spans="1:19" x14ac:dyDescent="0.3">
@@ -6339,34 +6339,34 @@
         <v>24</v>
       </c>
       <c r="J100">
-        <v>-3293.6281020290339</v>
+        <v>2142.15747878305</v>
       </c>
       <c r="K100">
-        <v>3.27957453902548</v>
+        <v>3.8210433507881221</v>
       </c>
       <c r="L100">
-        <v>1.6823901023035119</v>
+        <v>1.560090972802086</v>
       </c>
       <c r="M100">
-        <v>4.0505502551014656</v>
+        <v>4.9977982909339156</v>
       </c>
       <c r="N100">
-        <v>0.85847367680299136</v>
+        <v>2.066048718787052</v>
       </c>
       <c r="O100">
-        <v>6.2815911362532502</v>
+        <v>5.480956741826847</v>
       </c>
       <c r="P100">
-        <v>0.50894797560051852</v>
+        <v>0.27167239756326228</v>
       </c>
       <c r="Q100">
-        <v>0.54905209660623422</v>
+        <v>8.3069134143342414</v>
       </c>
       <c r="R100">
-        <v>1.8528383586179289</v>
+        <v>2.231268806321129</v>
       </c>
       <c r="S100">
-        <v>0.23055644667083031</v>
+        <v>0.55934219179338895</v>
       </c>
     </row>
     <row r="101" spans="1:19" x14ac:dyDescent="0.3">
@@ -6398,34 +6398,34 @@
         <v>24</v>
       </c>
       <c r="J101">
-        <v>-3299.5217098105691</v>
+        <v>2159.339960104227</v>
       </c>
       <c r="K101">
-        <v>3.2008811379295961</v>
+        <v>3.8334929921720251</v>
       </c>
       <c r="L101">
-        <v>2.397824923228058</v>
+        <v>1.1069901255881129</v>
       </c>
       <c r="M101">
-        <v>4.3988381080409011</v>
+        <v>5.3877077508316678</v>
       </c>
       <c r="N101">
-        <v>0.79625875584369954</v>
+        <v>0.93597337493068999</v>
       </c>
       <c r="O101">
-        <v>6.2414193537564691</v>
+        <v>5.5655421424821148</v>
       </c>
       <c r="P101">
-        <v>0.53050185505049741</v>
+        <v>1.0164765471515731</v>
       </c>
       <c r="Q101">
-        <v>0.5702539495103881</v>
+        <v>7.7479626928366114</v>
       </c>
       <c r="R101">
-        <v>1.0109124045942901</v>
+        <v>1.677554108395386</v>
       </c>
       <c r="S101">
-        <v>0.2171572863326913</v>
+        <v>0.27563703847360049</v>
       </c>
     </row>
     <row r="102" spans="1:19" x14ac:dyDescent="0.3">
@@ -6457,34 +6457,34 @@
         <v>24</v>
       </c>
       <c r="J102">
-        <v>-3305.585779628595</v>
+        <v>2178.6097199489618</v>
       </c>
       <c r="K102">
-        <v>3.1638747822233162</v>
+        <v>4.0576210062498221</v>
       </c>
       <c r="L102">
-        <v>2.2509197789562219</v>
+        <v>0.65299693153756322</v>
       </c>
       <c r="M102">
-        <v>4.1443804603530481</v>
+        <v>5.2145937606188397</v>
       </c>
       <c r="N102">
-        <v>0.51405896660261763</v>
+        <v>0.67783528348450539</v>
       </c>
       <c r="O102">
-        <v>6.2417258400386872</v>
+        <v>5.8026545622753538</v>
       </c>
       <c r="P102">
-        <v>0.2962365789062601</v>
+        <v>1.843583821901879</v>
       </c>
       <c r="Q102">
-        <v>0.25670188637158281</v>
+        <v>5.6606841692772676</v>
       </c>
       <c r="R102">
-        <v>0.71764257987697577</v>
+        <v>0.73936359677750985</v>
       </c>
       <c r="S102">
-        <v>0.2429097430776426</v>
+        <v>1.182006430712746</v>
       </c>
     </row>
     <row r="103" spans="1:19" x14ac:dyDescent="0.3">
@@ -6516,34 +6516,34 @@
         <v>24</v>
       </c>
       <c r="J103">
-        <v>-3311.6486268320341</v>
+        <v>2196.985073320001</v>
       </c>
       <c r="K103">
-        <v>3.1387229653507931</v>
+        <v>3.8613260721375671</v>
       </c>
       <c r="L103">
-        <v>0.59139198533359516</v>
+        <v>0.56404276739799397</v>
       </c>
       <c r="M103">
-        <v>4.1345014097913726</v>
+        <v>5.0697162029741554</v>
       </c>
       <c r="N103">
-        <v>0.48146123595545909</v>
+        <v>0.70808960035534185</v>
       </c>
       <c r="O103">
-        <v>6.2574515097895782</v>
+        <v>5.7362476051904876</v>
       </c>
       <c r="P103">
-        <v>0.25150988107412098</v>
+        <v>0.49567903859840112</v>
       </c>
       <c r="Q103">
-        <v>0.20958155896648401</v>
+        <v>6.5550906429738864</v>
       </c>
       <c r="R103">
-        <v>0.69299278202036152</v>
+        <v>0.97419123451359013</v>
       </c>
       <c r="S103">
-        <v>0.236766685632015</v>
+        <v>1.432306329026775</v>
       </c>
     </row>
     <row r="104" spans="1:19" x14ac:dyDescent="0.3">
@@ -6575,34 +6575,34 @@
         <v>24</v>
       </c>
       <c r="J104">
-        <v>-3317.8464358168758</v>
+        <v>2214.0317568714031</v>
       </c>
       <c r="K104">
-        <v>3.1058438093682379</v>
+        <v>3.7386125681492248</v>
       </c>
       <c r="L104">
-        <v>2.2335557424988881</v>
+        <v>1.1022935989346261</v>
       </c>
       <c r="M104">
-        <v>4.2765941030779642</v>
+        <v>5.2918462973189548</v>
       </c>
       <c r="N104">
-        <v>0.56251371136760719</v>
+        <v>1.6553095381080869</v>
       </c>
       <c r="O104">
-        <v>6.257083582226767</v>
+        <v>5.624572608280122</v>
       </c>
       <c r="P104">
-        <v>0.24135044532296079</v>
+        <v>2.745337879586712</v>
       </c>
       <c r="Q104">
-        <v>0.16507083032341691</v>
+        <v>7.8837604626114519</v>
       </c>
       <c r="R104">
-        <v>1.662552748783477</v>
+        <v>1.7158543774780071</v>
       </c>
       <c r="S104">
-        <v>0.2266957679430999</v>
+        <v>0.5489393676319233</v>
       </c>
     </row>
     <row r="105" spans="1:19" x14ac:dyDescent="0.3">
@@ -6634,31 +6634,31 @@
         <v>24</v>
       </c>
       <c r="K105">
-        <v>3.7236269487776208</v>
+        <v>4.5905330248022578</v>
       </c>
       <c r="L105">
-        <v>1.650616002485279</v>
+        <v>1.1530541726122301</v>
       </c>
       <c r="M105">
-        <v>4.7621779314152164</v>
+        <v>5.9576150870900042</v>
       </c>
       <c r="N105">
-        <v>0.96139703989558001</v>
+        <v>1.841589192869322</v>
       </c>
       <c r="O105">
-        <v>6.4176940499566761</v>
+        <v>5.7873315578883613</v>
       </c>
       <c r="P105">
-        <v>0.817301126246745</v>
+        <v>1.579695625152659</v>
       </c>
       <c r="Q105">
-        <v>0.86885383349392498</v>
+        <v>5.1992338709459469</v>
       </c>
       <c r="R105">
-        <v>1.3688752603829939</v>
+        <v>1.3461978267393699</v>
       </c>
       <c r="S105">
-        <v>0.33385110766960818</v>
+        <v>0.74582100137136476</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finalización capitulo 3 tesis y correcion simulación de tamaños
</commit_message>
<xml_diff>
--- a/codigo_final_organizado/Simulaciones/ARIMA_D/resultados_TEST_DOBLE_MODALIDAD.xlsx
+++ b/codigo_final_organizado/Simulaciones/ARIMA_D/resultados_TEST_DOBLE_MODALIDAD.xlsx
@@ -555,16 +555,16 @@
         <v>2.329352160562849</v>
       </c>
       <c r="L2">
-        <v>0.6250125242161554</v>
+        <v>0.6295551662630674</v>
       </c>
       <c r="M2">
-        <v>2.503322110233595</v>
+        <v>2.488991062256829</v>
       </c>
       <c r="N2">
         <v>0.5760561642423011</v>
       </c>
       <c r="O2">
-        <v>1.759639692274781</v>
+        <v>1.161387200531747</v>
       </c>
       <c r="P2">
         <v>0.5952473505305892</v>
@@ -573,7 +573,7 @@
         <v>0.6051883723260757</v>
       </c>
       <c r="R2">
-        <v>0.9713975067355982</v>
+        <v>0.9891337896979696</v>
       </c>
       <c r="S2">
         <v>0.5763703196297121</v>
@@ -614,16 +614,16 @@
         <v>1.117990376119657</v>
       </c>
       <c r="L3">
-        <v>0.7500587231668514</v>
+        <v>0.762059997183536</v>
       </c>
       <c r="M3">
-        <v>1.356239465275344</v>
+        <v>1.34231345586745</v>
       </c>
       <c r="N3">
         <v>0.6140500706359714</v>
       </c>
       <c r="O3">
-        <v>1.686371333467825</v>
+        <v>0.7354160522409002</v>
       </c>
       <c r="P3">
         <v>0.9518872623865497</v>
@@ -632,7 +632,7 @@
         <v>1.553297537297615</v>
       </c>
       <c r="R3">
-        <v>0.636085284656948</v>
+        <v>0.6333250493404791</v>
       </c>
       <c r="S3">
         <v>0.8511311361243317</v>
@@ -673,16 +673,16 @@
         <v>2.077124112251781</v>
       </c>
       <c r="L4">
-        <v>0.642772488752966</v>
+        <v>0.6415410996542849</v>
       </c>
       <c r="M4">
-        <v>2.231516857239856</v>
+        <v>2.250671527054001</v>
       </c>
       <c r="N4">
         <v>0.5957787302181513</v>
       </c>
       <c r="O4">
-        <v>1.697638352748716</v>
+        <v>1.005343241084632</v>
       </c>
       <c r="P4">
         <v>1.561461927698934</v>
@@ -691,7 +691,7 @@
         <v>0.6699125495309974</v>
       </c>
       <c r="R4">
-        <v>0.659683794758301</v>
+        <v>0.6580503311310667</v>
       </c>
       <c r="S4">
         <v>0.8097134886474673</v>
@@ -732,16 +732,16 @@
         <v>1.456107077862547</v>
       </c>
       <c r="L5">
-        <v>0.5895497294097077</v>
+        <v>0.5971438016366533</v>
       </c>
       <c r="M5">
-        <v>1.606264354625957</v>
+        <v>1.659080130864984</v>
       </c>
       <c r="N5">
         <v>0.5567753748073512</v>
       </c>
       <c r="O5">
-        <v>1.657517909906332</v>
+        <v>0.7579473563946998</v>
       </c>
       <c r="P5">
         <v>0.8876677535344316</v>
@@ -750,7 +750,7 @@
         <v>1.079819281167898</v>
       </c>
       <c r="R5">
-        <v>0.6341832591823116</v>
+        <v>0.6429107513230984</v>
       </c>
       <c r="S5">
         <v>0.6214045184917408</v>
@@ -791,16 +791,16 @@
         <v>1.702348644526452</v>
       </c>
       <c r="L6">
-        <v>1.169149624353454</v>
+        <v>1.165680737284651</v>
       </c>
       <c r="M6">
-        <v>1.912558648115913</v>
+        <v>1.866207643746876</v>
       </c>
       <c r="N6">
         <v>0.5674328540967224</v>
       </c>
       <c r="O6">
-        <v>1.660098633114278</v>
+        <v>0.8356006087478182</v>
       </c>
       <c r="P6">
         <v>0.6868451162821876</v>
@@ -809,7 +809,7 @@
         <v>0.8642650900270513</v>
       </c>
       <c r="R6">
-        <v>0.6063700564678716</v>
+        <v>0.6091317461536611</v>
       </c>
       <c r="S6">
         <v>0.9061833323220045</v>
@@ -850,16 +850,16 @@
         <v>1.674163862907375</v>
       </c>
       <c r="L7">
-        <v>0.7003246129416341</v>
+        <v>0.7141719487127703</v>
       </c>
       <c r="M7">
-        <v>1.82008351883134</v>
+        <v>1.821816705525575</v>
       </c>
       <c r="N7">
         <v>0.5816626812889198</v>
       </c>
       <c r="O7">
-        <v>1.662252047684739</v>
+        <v>0.8310531557752832</v>
       </c>
       <c r="P7">
         <v>0.6222057433780163</v>
@@ -868,7 +868,7 @@
         <v>0.895355952603325</v>
       </c>
       <c r="R7">
-        <v>0.6104024199859275</v>
+        <v>0.6182307933231742</v>
       </c>
       <c r="S7">
         <v>0.7872816563791795</v>
@@ -909,16 +909,16 @@
         <v>2.506239779302529</v>
       </c>
       <c r="L8">
-        <v>0.603903713460239</v>
+        <v>0.6065823781374411</v>
       </c>
       <c r="M8">
-        <v>2.677360062447347</v>
+        <v>2.622670525221102</v>
       </c>
       <c r="N8">
         <v>0.5647551295335711</v>
       </c>
       <c r="O8">
-        <v>1.751808814484567</v>
+        <v>1.246658683585789</v>
       </c>
       <c r="P8">
         <v>0.8767882279816439</v>
@@ -927,7 +927,7 @@
         <v>0.5600324001590659</v>
       </c>
       <c r="R8">
-        <v>0.5946398519907289</v>
+        <v>0.6038074512301116</v>
       </c>
       <c r="S8">
         <v>0.6706522622170192</v>
@@ -968,16 +968,16 @@
         <v>2.838694734058731</v>
       </c>
       <c r="L9">
-        <v>0.6643690866477275</v>
+        <v>0.6653193049522128</v>
       </c>
       <c r="M9">
-        <v>2.955257464843912</v>
+        <v>3.14014073315474</v>
       </c>
       <c r="N9">
         <v>0.5627279974899299</v>
       </c>
       <c r="O9">
-        <v>1.841488713743789</v>
+        <v>1.476190373142271</v>
       </c>
       <c r="P9">
         <v>0.6669820287430237</v>
@@ -986,7 +986,7 @@
         <v>0.6057241363923819</v>
       </c>
       <c r="R9">
-        <v>0.6894604721590011</v>
+        <v>0.6891831374686687</v>
       </c>
       <c r="S9">
         <v>0.5929306216227492</v>
@@ -1027,16 +1027,16 @@
         <v>1.74262588038507</v>
       </c>
       <c r="L10">
-        <v>0.7917261560325749</v>
+        <v>0.8037425550028471</v>
       </c>
       <c r="M10">
-        <v>1.821131828150778</v>
+        <v>1.936559896496115</v>
       </c>
       <c r="N10">
         <v>0.589335088903213</v>
       </c>
       <c r="O10">
-        <v>1.650914327189664</v>
+        <v>0.8455191973668053</v>
       </c>
       <c r="P10">
         <v>0.851368161536773</v>
@@ -1045,7 +1045,7 @@
         <v>0.8176163432933472</v>
       </c>
       <c r="R10">
-        <v>0.7248720717935483</v>
+        <v>0.7342910917720246</v>
       </c>
       <c r="S10">
         <v>0.5899339641195104</v>
@@ -1086,16 +1086,16 @@
         <v>1.354846103453665</v>
       </c>
       <c r="L11">
-        <v>0.6583274329590879</v>
+        <v>0.6660256890377343</v>
       </c>
       <c r="M11">
-        <v>1.453538337315669</v>
+        <v>1.52218024940259</v>
       </c>
       <c r="N11">
         <v>0.5783252930235133</v>
       </c>
       <c r="O11">
-        <v>1.649247418467598</v>
+        <v>0.7418092314241053</v>
       </c>
       <c r="P11">
         <v>0.5766974744046752</v>
@@ -1104,7 +1104,7 @@
         <v>1.138851628389371</v>
       </c>
       <c r="R11">
-        <v>0.6131119906215384</v>
+        <v>0.6176665822516522</v>
       </c>
       <c r="S11">
         <v>0.9849543639772878</v>
@@ -1145,16 +1145,16 @@
         <v>0.6812271877816788</v>
       </c>
       <c r="L12">
-        <v>0.6979697564140056</v>
+        <v>0.7046148624994518</v>
       </c>
       <c r="M12">
-        <v>0.8445908842132359</v>
+        <v>0.8176194782235803</v>
       </c>
       <c r="N12">
         <v>0.6011113031132777</v>
       </c>
       <c r="O12">
-        <v>1.770748627938241</v>
+        <v>1.04635561764207</v>
       </c>
       <c r="P12">
         <v>1.23795449957362</v>
@@ -1163,7 +1163,7 @@
         <v>2.695982549258239</v>
       </c>
       <c r="R12">
-        <v>0.7970272402619447</v>
+        <v>0.7882552209993579</v>
       </c>
       <c r="S12">
         <v>0.6661923996250076</v>
@@ -1204,16 +1204,16 @@
         <v>0.7864032711499824</v>
       </c>
       <c r="L13">
-        <v>0.6087324016048055</v>
+        <v>0.6148073312786212</v>
       </c>
       <c r="M13">
-        <v>0.8164011841417758</v>
+        <v>0.7965000734497908</v>
       </c>
       <c r="N13">
         <v>0.5783593891445493</v>
       </c>
       <c r="O13">
-        <v>1.874080110853181</v>
+        <v>1.591500327353775</v>
       </c>
       <c r="P13">
         <v>0.8411914342269159</v>
@@ -1222,7 +1222,7 @@
         <v>3.815796156270378</v>
       </c>
       <c r="R13">
-        <v>0.5880983419625199</v>
+        <v>0.5988444046595184</v>
       </c>
       <c r="S13">
         <v>0.5608910236851092</v>
@@ -1263,7 +1263,7 @@
         <v>0.5805012599433051</v>
       </c>
       <c r="L14">
-        <v>0.6353487477639628</v>
+        <v>0.6396415684282917</v>
       </c>
       <c r="M14">
         <v>0.5580958722573137</v>
@@ -1272,7 +1272,7 @@
         <v>0.5696021766634581</v>
       </c>
       <c r="O14">
-        <v>0.7551182698457386</v>
+        <v>0.5873564261943489</v>
       </c>
       <c r="P14">
         <v>0.5716741292164806</v>
@@ -1281,7 +1281,7 @@
         <v>0.572094785155306</v>
       </c>
       <c r="R14">
-        <v>0.5730614901275335</v>
+        <v>0.5768053844003823</v>
       </c>
       <c r="S14">
         <v>0.5721415318366755</v>
@@ -1322,7 +1322,7 @@
         <v>0.6054160794703013</v>
       </c>
       <c r="L15">
-        <v>0.6607441456828075</v>
+        <v>0.6801943771672405</v>
       </c>
       <c r="M15">
         <v>0.5788516988977608</v>
@@ -1331,7 +1331,7 @@
         <v>0.6622947600102919</v>
       </c>
       <c r="O15">
-        <v>0.7696397673979957</v>
+        <v>0.6129438092548614</v>
       </c>
       <c r="P15">
         <v>0.5875730071116632</v>
@@ -1340,7 +1340,7 @@
         <v>0.5958981640096126</v>
       </c>
       <c r="R15">
-        <v>0.6979582960723201</v>
+        <v>0.7066306668901658</v>
       </c>
       <c r="S15">
         <v>0.7048627068019401</v>
@@ -1381,7 +1381,7 @@
         <v>0.594714683479767</v>
       </c>
       <c r="L16">
-        <v>0.6335262694899392</v>
+        <v>0.6427717113444953</v>
       </c>
       <c r="M16">
         <v>0.5661918292204633</v>
@@ -1390,7 +1390,7 @@
         <v>0.5948136441526498</v>
       </c>
       <c r="O16">
-        <v>0.7548077770563369</v>
+        <v>0.6001661727642695</v>
       </c>
       <c r="P16">
         <v>0.5842035484766994</v>
@@ -1399,7 +1399,7 @@
         <v>0.584813888976334</v>
       </c>
       <c r="R16">
-        <v>0.6036959921504793</v>
+        <v>0.6088917752205117</v>
       </c>
       <c r="S16">
         <v>0.7522580874785182</v>
@@ -1440,7 +1440,7 @@
         <v>0.5978028336385349</v>
       </c>
       <c r="L17">
-        <v>0.701412757280205</v>
+        <v>0.7031995819025114</v>
       </c>
       <c r="M17">
         <v>0.5706006240037002</v>
@@ -1449,7 +1449,7 @@
         <v>0.5774588057289965</v>
       </c>
       <c r="O17">
-        <v>0.7596346081314396</v>
+        <v>0.6000526626431569</v>
       </c>
       <c r="P17">
         <v>0.6464426243684775</v>
@@ -1458,7 +1458,7 @@
         <v>0.5867012167191404</v>
       </c>
       <c r="R17">
-        <v>0.8342162416397871</v>
+        <v>0.8376228326494306</v>
       </c>
       <c r="S17">
         <v>0.6022558849044196</v>
@@ -1499,7 +1499,7 @@
         <v>0.6154607675689756</v>
       </c>
       <c r="L18">
-        <v>0.6641541626655312</v>
+        <v>0.6685788178700612</v>
       </c>
       <c r="M18">
         <v>0.5795356912910361</v>
@@ -1508,7 +1508,7 @@
         <v>0.572359901978324</v>
       </c>
       <c r="O18">
-        <v>0.7684120287303787</v>
+        <v>0.6240995287962096</v>
       </c>
       <c r="P18">
         <v>0.5700815991707904</v>
@@ -1517,7 +1517,7 @@
         <v>0.604381925301635</v>
       </c>
       <c r="R18">
-        <v>0.6292865140066096</v>
+        <v>0.6369506038996421</v>
       </c>
       <c r="S18">
         <v>0.5802756409849664</v>
@@ -1558,7 +1558,7 @@
         <v>0.5843190066421033</v>
       </c>
       <c r="L19">
-        <v>0.6440774799578556</v>
+        <v>0.6448925334437349</v>
       </c>
       <c r="M19">
         <v>0.5567676456383599</v>
@@ -1567,7 +1567,7 @@
         <v>0.5573596726718332</v>
       </c>
       <c r="O19">
-        <v>0.7550082976630764</v>
+        <v>0.5933770509988034</v>
       </c>
       <c r="P19">
         <v>0.5526512034431753</v>
@@ -1576,7 +1576,7 @@
         <v>0.5772046223267654</v>
       </c>
       <c r="R19">
-        <v>0.6052241316726994</v>
+        <v>0.625866248419109</v>
       </c>
       <c r="S19">
         <v>0.706936791581869</v>
@@ -1617,7 +1617,7 @@
         <v>0.6141700895171466</v>
       </c>
       <c r="L20">
-        <v>0.6892014175282627</v>
+        <v>0.7025536133255801</v>
       </c>
       <c r="M20">
         <v>0.5854417706243705</v>
@@ -1626,7 +1626,7 @@
         <v>0.5790201559863105</v>
       </c>
       <c r="O20">
-        <v>0.7666904478456429</v>
+        <v>0.6191450687626204</v>
       </c>
       <c r="P20">
         <v>0.6192838448150926</v>
@@ -1635,7 +1635,7 @@
         <v>0.6041974609604271</v>
       </c>
       <c r="R20">
-        <v>0.5907084265144853</v>
+        <v>0.5902881754766329</v>
       </c>
       <c r="S20">
         <v>0.5843195130804236</v>
@@ -1676,7 +1676,7 @@
         <v>0.645381834793615</v>
       </c>
       <c r="L21">
-        <v>0.8106067649967913</v>
+        <v>0.8089374535279616</v>
       </c>
       <c r="M21">
         <v>0.6054343726937845</v>
@@ -1685,7 +1685,7 @@
         <v>0.5960473943923774</v>
       </c>
       <c r="O21">
-        <v>0.7730866274829623</v>
+        <v>0.6497568835032318</v>
       </c>
       <c r="P21">
         <v>0.5968086285714208</v>
@@ -1694,7 +1694,7 @@
         <v>0.6316081006900832</v>
       </c>
       <c r="R21">
-        <v>0.6229857032770267</v>
+        <v>0.6373451020236822</v>
       </c>
       <c r="S21">
         <v>0.6043968434973281</v>
@@ -1735,7 +1735,7 @@
         <v>0.5799302811817882</v>
       </c>
       <c r="L22">
-        <v>0.6402422434637739</v>
+        <v>0.6370836829753571</v>
       </c>
       <c r="M22">
         <v>0.5594465306044519</v>
@@ -1744,7 +1744,7 @@
         <v>0.6240662900094331</v>
       </c>
       <c r="O22">
-        <v>0.7590570277838874</v>
+        <v>0.5873116717278462</v>
       </c>
       <c r="P22">
         <v>0.557852731462227</v>
@@ -1753,7 +1753,7 @@
         <v>0.5725880236134514</v>
       </c>
       <c r="R22">
-        <v>0.6978612339245019</v>
+        <v>0.6972609222799506</v>
       </c>
       <c r="S22">
         <v>0.5625674815526233</v>
@@ -1794,7 +1794,7 @@
         <v>0.5830539791996907</v>
       </c>
       <c r="L23">
-        <v>0.603165645307139</v>
+        <v>0.6161661036718882</v>
       </c>
       <c r="M23">
         <v>0.5582499199267044</v>
@@ -1803,7 +1803,7 @@
         <v>0.6011836428796307</v>
       </c>
       <c r="O23">
-        <v>0.7598292406038643</v>
+        <v>0.5880717702042811</v>
       </c>
       <c r="P23">
         <v>0.573245589231001</v>
@@ -1812,7 +1812,7 @@
         <v>0.5746797151261344</v>
       </c>
       <c r="R23">
-        <v>0.7860960024011596</v>
+        <v>0.7866414329029519</v>
       </c>
       <c r="S23">
         <v>0.5827466817501027</v>
@@ -1853,7 +1853,7 @@
         <v>0.5696500087046025</v>
       </c>
       <c r="L24">
-        <v>0.6374358621033671</v>
+        <v>0.6488813813602589</v>
       </c>
       <c r="M24">
         <v>0.5429634668052646</v>
@@ -1862,7 +1862,7 @@
         <v>0.5807645628479093</v>
       </c>
       <c r="O24">
-        <v>0.7558257791431421</v>
+        <v>0.576749447773386</v>
       </c>
       <c r="P24">
         <v>0.5510854632664778</v>
@@ -1871,7 +1871,7 @@
         <v>0.5648418915495145</v>
       </c>
       <c r="R24">
-        <v>0.6051784665433928</v>
+        <v>0.6163433898283603</v>
       </c>
       <c r="S24">
         <v>0.5840254934621194</v>
@@ -1912,7 +1912,7 @@
         <v>0.6109260501187876</v>
       </c>
       <c r="L25">
-        <v>0.6471640127070002</v>
+        <v>0.6546727748781607</v>
       </c>
       <c r="M25">
         <v>0.5778018947349471</v>
@@ -1921,7 +1921,7 @@
         <v>0.5980984291569988</v>
       </c>
       <c r="O25">
-        <v>0.7747805758297045</v>
+        <v>0.6085150645789653</v>
       </c>
       <c r="P25">
         <v>0.5780506220182575</v>
@@ -1930,7 +1930,7 @@
         <v>0.5995412546498207</v>
       </c>
       <c r="R25">
-        <v>0.6970927192462741</v>
+        <v>0.7037101940602868</v>
       </c>
       <c r="S25">
         <v>0.58299541680112</v>
@@ -1971,7 +1971,7 @@
         <v>19.98494915933875</v>
       </c>
       <c r="L26">
-        <v>2.735366526147064</v>
+        <v>2.776989957449815</v>
       </c>
       <c r="M26">
         <v>20.63051348286252</v>
@@ -1980,7 +1980,7 @@
         <v>0.7145171506512795</v>
       </c>
       <c r="O26">
-        <v>12.02839817159663</v>
+        <v>15.6983182757582</v>
       </c>
       <c r="P26">
         <v>0.7591757052928158</v>
@@ -1989,7 +1989,7 @@
         <v>0.7326477863443334</v>
       </c>
       <c r="R26">
-        <v>6.11807653073287</v>
+        <v>6.257129062016025</v>
       </c>
       <c r="S26">
         <v>0.5648428475050683</v>
@@ -2030,7 +2030,7 @@
         <v>19.39546344531029</v>
       </c>
       <c r="L27">
-        <v>2.292681018421286</v>
+        <v>2.429523826938034</v>
       </c>
       <c r="M27">
         <v>19.94083572103992</v>
@@ -2039,7 +2039,7 @@
         <v>1.026616488781003</v>
       </c>
       <c r="O27">
-        <v>11.84830408588927</v>
+        <v>15.24098248248891</v>
       </c>
       <c r="P27">
         <v>0.6181679965137293</v>
@@ -2048,7 +2048,7 @@
         <v>0.6101635910301187</v>
       </c>
       <c r="R27">
-        <v>5.644634070647814</v>
+        <v>5.87532806267454</v>
       </c>
       <c r="S27">
         <v>0.5821438485739769</v>
@@ -2089,7 +2089,7 @@
         <v>21.01859023061818</v>
       </c>
       <c r="L28">
-        <v>4.102999092538871</v>
+        <v>4.18244085923688</v>
       </c>
       <c r="M28">
         <v>21.61835893262667</v>
@@ -2098,7 +2098,7 @@
         <v>0.6565736207593742</v>
       </c>
       <c r="O28">
-        <v>12.555707129256</v>
+        <v>16.74651544089334</v>
       </c>
       <c r="P28">
         <v>1.334711223407604</v>
@@ -2107,7 +2107,7 @@
         <v>1.740976297926027</v>
       </c>
       <c r="R28">
-        <v>7.506788233189297</v>
+        <v>7.695772821112671</v>
       </c>
       <c r="S28">
         <v>0.5735180930561938</v>
@@ -2148,7 +2148,7 @@
         <v>19.4122734388446</v>
       </c>
       <c r="L29">
-        <v>2.795566140662538</v>
+        <v>2.802179417885732</v>
       </c>
       <c r="M29">
         <v>20.0785502387266</v>
@@ -2157,7 +2157,7 @@
         <v>1.316945750179278</v>
       </c>
       <c r="O29">
-        <v>11.92973489027442</v>
+        <v>15.38325497197131</v>
       </c>
       <c r="P29">
         <v>1.006488226005323</v>
@@ -2166,7 +2166,7 @@
         <v>0.7477567784261221</v>
       </c>
       <c r="R29">
-        <v>6.205659675334443</v>
+        <v>6.282537124534026</v>
       </c>
       <c r="S29">
         <v>0.5925876882638579</v>
@@ -2207,7 +2207,7 @@
         <v>18.57338746480737</v>
       </c>
       <c r="L30">
-        <v>2.092980421478124</v>
+        <v>2.212215176736272</v>
       </c>
       <c r="M30">
         <v>19.49224159904928</v>
@@ -2216,7 +2216,7 @@
         <v>1.558884198938063</v>
       </c>
       <c r="O30">
-        <v>11.68246478124728</v>
+        <v>14.72454554679791</v>
       </c>
       <c r="P30">
         <v>0.7474824189950146</v>
@@ -2225,7 +2225,7 @@
         <v>0.5661851479619302</v>
       </c>
       <c r="R30">
-        <v>5.597826821469581</v>
+        <v>5.630574394066367</v>
       </c>
       <c r="S30">
         <v>0.5607745867133788</v>
@@ -2266,7 +2266,7 @@
         <v>19.80222751330581</v>
       </c>
       <c r="L31">
-        <v>3.267273576883375</v>
+        <v>3.574500107094097</v>
       </c>
       <c r="M31">
         <v>21.64012740641807</v>
@@ -2275,7 +2275,7 @@
         <v>0.9056310982794925</v>
       </c>
       <c r="O31">
-        <v>12.1928392080573</v>
+        <v>15.94432510018891</v>
       </c>
       <c r="P31">
         <v>1.123156649862793</v>
@@ -2284,7 +2284,7 @@
         <v>1.248050113789142</v>
       </c>
       <c r="R31">
-        <v>6.94266748078333</v>
+        <v>7.081068063776975</v>
       </c>
       <c r="S31">
         <v>0.585876171613026</v>
@@ -2325,7 +2325,7 @@
         <v>18.66846480278198</v>
       </c>
       <c r="L32">
-        <v>6.10086583999771</v>
+        <v>6.183158549406749</v>
       </c>
       <c r="M32">
         <v>19.78221029207869</v>
@@ -2334,7 +2334,7 @@
         <v>1.326986002348039</v>
       </c>
       <c r="O32">
-        <v>11.81068448683767</v>
+        <v>15.02596207648588</v>
       </c>
       <c r="P32">
         <v>0.7502859726792014</v>
@@ -2343,7 +2343,7 @@
         <v>0.6729010342202766</v>
       </c>
       <c r="R32">
-        <v>6.028642283468943</v>
+        <v>6.105728107943905</v>
       </c>
       <c r="S32">
         <v>0.6080362640740847</v>
@@ -2384,7 +2384,7 @@
         <v>18.81971378322074</v>
       </c>
       <c r="L33">
-        <v>6.507518017849097</v>
+        <v>6.540932862971386</v>
       </c>
       <c r="M33">
         <v>19.07640055463374</v>
@@ -2393,7 +2393,7 @@
         <v>1.135584052849572</v>
       </c>
       <c r="O33">
-        <v>11.92379405094331</v>
+        <v>15.29475957802564</v>
       </c>
       <c r="P33">
         <v>0.5875423990991511</v>
@@ -2402,7 +2402,7 @@
         <v>0.8374491557282465</v>
       </c>
       <c r="R33">
-        <v>6.651227825894411</v>
+        <v>6.456732994877056</v>
       </c>
       <c r="S33">
         <v>0.5749241766057839</v>
@@ -2443,7 +2443,7 @@
         <v>18.50837143804062</v>
       </c>
       <c r="L34">
-        <v>6.112120146395399</v>
+        <v>6.404963682195123</v>
       </c>
       <c r="M34">
         <v>18.65425963209421</v>
@@ -2452,7 +2452,7 @@
         <v>1.231935201905849</v>
       </c>
       <c r="O34">
-        <v>11.86449396682928</v>
+        <v>15.14423191388044</v>
       </c>
       <c r="P34">
         <v>0.5513641195403747</v>
@@ -2461,7 +2461,7 @@
         <v>0.7540976953161301</v>
       </c>
       <c r="R34">
-        <v>6.187533609771708</v>
+        <v>6.32226361912514</v>
       </c>
       <c r="S34">
         <v>0.5538172899562568</v>
@@ -2502,7 +2502,7 @@
         <v>20.73620241053171</v>
       </c>
       <c r="L35">
-        <v>8.644548173887799</v>
+        <v>8.935394261513233</v>
       </c>
       <c r="M35">
         <v>21.14917889780414</v>
@@ -2511,7 +2511,7 @@
         <v>0.6299464141202614</v>
       </c>
       <c r="O35">
-        <v>12.92203115565685</v>
+        <v>17.33084781020669</v>
       </c>
       <c r="P35">
         <v>2.015279919482962</v>
@@ -2520,7 +2520,7 @@
         <v>2.834986565301343</v>
       </c>
       <c r="R35">
-        <v>8.611345395642097</v>
+        <v>8.842535216497778</v>
       </c>
       <c r="S35">
         <v>0.5763230112367974</v>
@@ -2561,7 +2561,7 @@
         <v>18.8736649511854</v>
       </c>
       <c r="L36">
-        <v>9.622737171058009</v>
+        <v>9.552179430982481</v>
       </c>
       <c r="M36">
         <v>20.05656031936848</v>
@@ -2570,7 +2570,7 @@
         <v>1.298325543118778</v>
       </c>
       <c r="O36">
-        <v>12.12106680841681</v>
+        <v>15.73622045776236</v>
       </c>
       <c r="P36">
         <v>1.191354256674</v>
@@ -2579,7 +2579,7 @@
         <v>1.262123262149639</v>
       </c>
       <c r="R36">
-        <v>7.164915019574597</v>
+        <v>7.102279554272643</v>
       </c>
       <c r="S36">
         <v>0.6102822404515501</v>
@@ -2620,7 +2620,7 @@
         <v>17.72043628682542</v>
       </c>
       <c r="L37">
-        <v>8.37068515114702</v>
+        <v>8.478095351731135</v>
       </c>
       <c r="M37">
         <v>18.62373751822582</v>
@@ -2629,7 +2629,7 @@
         <v>1.811337830343618</v>
       </c>
       <c r="O37">
-        <v>11.74164713174096</v>
+        <v>14.78207015381396</v>
       </c>
       <c r="P37">
         <v>1.017428626702239</v>
@@ -2638,7 +2638,7 @@
         <v>0.6665204342046219</v>
       </c>
       <c r="R37">
-        <v>5.848979753656412</v>
+        <v>6.043689490214181</v>
       </c>
       <c r="S37">
         <v>0.5847914393367842</v>
@@ -2679,7 +2679,7 @@
         <v>0.5996829259895005</v>
       </c>
       <c r="L38">
-        <v>0.5839665617251777</v>
+        <v>0.596903979825588</v>
       </c>
       <c r="M38">
         <v>0.6063844273674437</v>
@@ -2688,7 +2688,7 @@
         <v>0.555050145478265</v>
       </c>
       <c r="O38">
-        <v>0.9439199279961407</v>
+        <v>0.7715517152440707</v>
       </c>
       <c r="P38">
         <v>0.5627588544318762</v>
@@ -2697,7 +2697,7 @@
         <v>0.5687742185282195</v>
       </c>
       <c r="R38">
-        <v>0.6166158262488802</v>
+        <v>0.6238974871321992</v>
       </c>
       <c r="S38">
         <v>0.555373524447218</v>
@@ -2738,7 +2738,7 @@
         <v>0.6396029939854777</v>
       </c>
       <c r="L39">
-        <v>0.7040798233058468</v>
+        <v>0.7085804824040374</v>
       </c>
       <c r="M39">
         <v>0.5813181222837525</v>
@@ -2747,7 +2747,7 @@
         <v>0.5786972575077759</v>
       </c>
       <c r="O39">
-        <v>0.8933962652399657</v>
+        <v>0.6375143001121364</v>
       </c>
       <c r="P39">
         <v>0.6837572460664227</v>
@@ -2756,7 +2756,7 @@
         <v>0.7089152157005638</v>
       </c>
       <c r="R39">
-        <v>0.5897721208101659</v>
+        <v>0.5898690086272691</v>
       </c>
       <c r="S39">
         <v>0.5792441002865576</v>
@@ -2797,7 +2797,7 @@
         <v>0.6731290125708083</v>
       </c>
       <c r="L40">
-        <v>0.7900378559393019</v>
+        <v>0.788067565194753</v>
       </c>
       <c r="M40">
         <v>0.6630918110094801</v>
@@ -2806,7 +2806,7 @@
         <v>0.5762542044109658</v>
       </c>
       <c r="O40">
-        <v>0.9852889993554749</v>
+        <v>0.8859909094470114</v>
       </c>
       <c r="P40">
         <v>0.6676295498793714</v>
@@ -2815,7 +2815,7 @@
         <v>0.5754114787575358</v>
       </c>
       <c r="R40">
-        <v>0.8068283151455591</v>
+        <v>0.8143454333397296</v>
       </c>
       <c r="S40">
         <v>0.607964874484995</v>
@@ -2856,7 +2856,7 @@
         <v>0.7254137892434001</v>
       </c>
       <c r="L41">
-        <v>0.6916087283356172</v>
+        <v>0.6942026266210469</v>
       </c>
       <c r="M41">
         <v>0.6196955146059198</v>
@@ -2865,7 +2865,7 @@
         <v>0.559072194109932</v>
       </c>
       <c r="O41">
-        <v>0.8690141199243364</v>
+        <v>0.5735435334481206</v>
       </c>
       <c r="P41">
         <v>0.7720543409176459</v>
@@ -2874,7 +2874,7 @@
         <v>0.8563757973909811</v>
       </c>
       <c r="R41">
-        <v>0.7953827463870636</v>
+        <v>0.7976389485417926</v>
       </c>
       <c r="S41">
         <v>0.5809136342503985</v>
@@ -2915,7 +2915,7 @@
         <v>0.7671873243908454</v>
       </c>
       <c r="L42">
-        <v>0.6603487186076558</v>
+        <v>0.6673421456059601</v>
       </c>
       <c r="M42">
         <v>0.6242764227303704</v>
@@ -2924,7 +2924,7 @@
         <v>0.5644538460092324</v>
       </c>
       <c r="O42">
-        <v>0.8640834726347066</v>
+        <v>0.5734580294852791</v>
       </c>
       <c r="P42">
         <v>0.5945920261291091</v>
@@ -2933,7 +2933,7 @@
         <v>0.9053919842432981</v>
       </c>
       <c r="R42">
-        <v>0.7130514676857933</v>
+        <v>0.7204072078357806</v>
       </c>
       <c r="S42">
         <v>0.5704968289808879</v>
@@ -2974,7 +2974,7 @@
         <v>0.6270841290254098</v>
       </c>
       <c r="L43">
-        <v>0.7779686491125773</v>
+        <v>0.8012695291035882</v>
       </c>
       <c r="M43">
         <v>0.611282620714915</v>
@@ -2983,7 +2983,7 @@
         <v>0.5913743221878596</v>
       </c>
       <c r="O43">
-        <v>0.9350978244138456</v>
+        <v>0.7581517390004693</v>
       </c>
       <c r="P43">
         <v>0.7106656355437193</v>
@@ -2992,7 +2992,7 @@
         <v>0.6158969372523039</v>
       </c>
       <c r="R43">
-        <v>1.019601414029905</v>
+        <v>1.025688705415596</v>
       </c>
       <c r="S43">
         <v>0.5887404864218584</v>
@@ -3033,7 +3033,7 @@
         <v>0.6822201561374404</v>
       </c>
       <c r="L44">
-        <v>0.6613481637837951</v>
+        <v>0.6639470266602575</v>
       </c>
       <c r="M44">
         <v>0.5873194076161933</v>
@@ -3042,7 +3042,7 @@
         <v>0.5567754635449109</v>
       </c>
       <c r="O44">
-        <v>0.8688428243733548</v>
+        <v>0.5820706512480668</v>
       </c>
       <c r="P44">
         <v>0.6148083994914667</v>
@@ -3051,7 +3051,7 @@
         <v>0.8002573618586555</v>
       </c>
       <c r="R44">
-        <v>0.581515577384806</v>
+        <v>0.5816000513730265</v>
       </c>
       <c r="S44">
         <v>0.5737200759917601</v>
@@ -3092,7 +3092,7 @@
         <v>0.615263652655555</v>
       </c>
       <c r="L45">
-        <v>1.118605790731655</v>
+        <v>1.115558164469435</v>
       </c>
       <c r="M45">
         <v>0.556557513730482</v>
@@ -3101,7 +3101,7 @@
         <v>0.5532032885265824</v>
       </c>
       <c r="O45">
-        <v>0.8852966299414861</v>
+        <v>0.62013213825363</v>
       </c>
       <c r="P45">
         <v>0.5542099599130305</v>
@@ -3110,7 +3110,7 @@
         <v>0.6924922942790694</v>
       </c>
       <c r="R45">
-        <v>0.5584176219953075</v>
+        <v>0.5624226032326546</v>
       </c>
       <c r="S45">
         <v>0.5540002077798094</v>
@@ -3151,7 +3151,7 @@
         <v>0.6287748359479493</v>
       </c>
       <c r="L46">
-        <v>0.6149589293328739</v>
+        <v>0.6177789981695073</v>
       </c>
       <c r="M46">
         <v>0.5663510123705223</v>
@@ -3160,7 +3160,7 @@
         <v>0.5565055041259982</v>
       </c>
       <c r="O46">
-        <v>0.8858019023623781</v>
+        <v>0.6125710802710608</v>
       </c>
       <c r="P46">
         <v>0.5577188931132337</v>
@@ -3169,7 +3169,7 @@
         <v>0.721457224817256</v>
       </c>
       <c r="R46">
-        <v>0.591580920625452</v>
+        <v>0.5985162690522775</v>
       </c>
       <c r="S46">
         <v>0.5586409215635567</v>
@@ -3210,7 +3210,7 @@
         <v>0.7187156382140139</v>
       </c>
       <c r="L47">
-        <v>0.7177436784425992</v>
+        <v>0.7118420368861839</v>
       </c>
       <c r="M47">
         <v>0.7287046489228716</v>
@@ -3219,7 +3219,7 @@
         <v>0.5748706520459008</v>
       </c>
       <c r="O47">
-        <v>1.02768762834113</v>
+        <v>0.984249966499268</v>
       </c>
       <c r="P47">
         <v>0.8172539209419111</v>
@@ -3228,7 +3228,7 @@
         <v>0.5800367635178791</v>
       </c>
       <c r="R47">
-        <v>0.5952751260565587</v>
+        <v>0.6042372643901377</v>
       </c>
       <c r="S47">
         <v>0.5827114976120368</v>
@@ -3269,7 +3269,7 @@
         <v>0.7600875064480752</v>
       </c>
       <c r="L48">
-        <v>0.6765647125156196</v>
+        <v>0.6784653597889451</v>
       </c>
       <c r="M48">
         <v>0.613486580796217</v>
@@ -3278,7 +3278,7 @@
         <v>0.5825697457602191</v>
       </c>
       <c r="O48">
-        <v>0.8704875507677329</v>
+        <v>0.5858005805856138</v>
       </c>
       <c r="P48">
         <v>0.9333035787183058</v>
@@ -3287,7 +3287,7 @@
         <v>0.897005985652009</v>
       </c>
       <c r="R48">
-        <v>0.6744979463087856</v>
+        <v>0.6754144632860105</v>
       </c>
       <c r="S48">
         <v>0.5856489888928724</v>
@@ -3328,7 +3328,7 @@
         <v>0.8392581169780149</v>
       </c>
       <c r="L49">
-        <v>0.6021240447732109</v>
+        <v>0.6132471197627841</v>
       </c>
       <c r="M49">
         <v>0.6813836404804574</v>
@@ -3337,7 +3337,7 @@
         <v>0.5707089984095671</v>
       </c>
       <c r="O49">
-        <v>0.8621416860144915</v>
+        <v>0.5796477225813302</v>
       </c>
       <c r="P49">
         <v>0.6262002327952607</v>
@@ -3346,7 +3346,7 @@
         <v>0.9923456014417256</v>
       </c>
       <c r="R49">
-        <v>0.6944921508354928</v>
+        <v>0.6907146639096439</v>
       </c>
       <c r="S49">
         <v>0.5688797679598062</v>
@@ -3387,16 +3387,16 @@
         <v>1171.10576019453</v>
       </c>
       <c r="L50">
-        <v>167.3896584664515</v>
+        <v>166.8469063360648</v>
       </c>
       <c r="M50">
-        <v>1322.091838020998</v>
+        <v>1301.14876570382</v>
       </c>
       <c r="N50">
         <v>589.9616286100908</v>
       </c>
       <c r="O50">
-        <v>372.1402342416891</v>
+        <v>872.9151533943061</v>
       </c>
       <c r="P50">
         <v>34.47996755927177</v>
@@ -3405,7 +3405,7 @@
         <v>34.50806539714995</v>
       </c>
       <c r="R50">
-        <v>315.3397427555565</v>
+        <v>314.1505410468666</v>
       </c>
       <c r="S50">
         <v>16.92048748494794</v>
@@ -3446,16 +3446,16 @@
         <v>1177.843227623663</v>
       </c>
       <c r="L51">
-        <v>183.8668062060017</v>
+        <v>185.8404508101679</v>
       </c>
       <c r="M51">
-        <v>1271.02043139081</v>
+        <v>1314.295541850157</v>
       </c>
       <c r="N51">
         <v>600.6140933696865</v>
       </c>
       <c r="O51">
-        <v>377.2561562748692</v>
+        <v>886.4294466590973</v>
       </c>
       <c r="P51">
         <v>35.8953052876447</v>
@@ -3464,7 +3464,7 @@
         <v>53.50160987125319</v>
       </c>
       <c r="R51">
-        <v>327.8715928923901</v>
+        <v>333.1440855209697</v>
       </c>
       <c r="S51">
         <v>17.37802295733977</v>
@@ -3505,16 +3505,16 @@
         <v>1178.884321733682</v>
       </c>
       <c r="L52">
-        <v>185.0000078800497</v>
+        <v>199.0756375260158</v>
       </c>
       <c r="M52">
-        <v>1256.049650311783</v>
+        <v>1234.802119057399</v>
       </c>
       <c r="N52">
         <v>613.7088602879894</v>
       </c>
       <c r="O52">
-        <v>380.5903274775989</v>
+        <v>895.1248843140278</v>
       </c>
       <c r="P52">
         <v>30.63504650013961</v>
@@ -3523,7 +3523,7 @@
         <v>66.73679658710113</v>
       </c>
       <c r="R52">
-        <v>324.5423646291295</v>
+        <v>346.3792722368178</v>
       </c>
       <c r="S52">
         <v>15.64550973728059</v>
@@ -3564,16 +3564,16 @@
         <v>1184.79750263151</v>
       </c>
       <c r="L53">
-        <v>220.1130487942924</v>
+        <v>217.2903531495712</v>
       </c>
       <c r="M53">
-        <v>1303.329404446826</v>
+        <v>1286.924037015678</v>
       </c>
       <c r="N53">
         <v>630.07227907837</v>
       </c>
       <c r="O53">
-        <v>386.1209181419924</v>
+        <v>908.2008112455633</v>
       </c>
       <c r="P53">
         <v>33.90316165291326</v>
@@ -3582,7 +3582,7 @@
         <v>84.95151221065677</v>
       </c>
       <c r="R53">
-        <v>366.3581528422806</v>
+        <v>364.5939878603736</v>
       </c>
       <c r="S53">
         <v>16.34047135788679</v>
@@ -3623,16 +3623,16 @@
         <v>1194.030023276689</v>
       </c>
       <c r="L54">
-        <v>238.0161486627691</v>
+        <v>238.9485308648716</v>
       </c>
       <c r="M54">
-        <v>1365.342056798595</v>
+        <v>1340.067811867236</v>
       </c>
       <c r="N54">
         <v>651.0762909412637</v>
       </c>
       <c r="O54">
-        <v>393.5773324591518</v>
+        <v>924.3033103931596</v>
       </c>
       <c r="P54">
         <v>38.02519244662786</v>
@@ -3641,7 +3641,7 @@
         <v>106.6096899259572</v>
       </c>
       <c r="R54">
-        <v>385.6410086641094</v>
+        <v>386.2521655756743</v>
       </c>
       <c r="S54">
         <v>17.88182038510013</v>
@@ -3682,16 +3682,16 @@
         <v>1196.215096482058</v>
       </c>
       <c r="L55">
-        <v>258.8286300467686</v>
+        <v>253.4628862171967</v>
       </c>
       <c r="M55">
-        <v>1341.617371469346</v>
+        <v>1327.942760461869</v>
       </c>
       <c r="N55">
         <v>669.117589571109</v>
       </c>
       <c r="O55">
-        <v>398.2152682603729</v>
+        <v>934.3311897947185</v>
       </c>
       <c r="P55">
         <v>32.31594876009364</v>
@@ -3700,7 +3700,7 @@
         <v>121.1240452782824</v>
       </c>
       <c r="R55">
-        <v>414.2403110476156</v>
+        <v>400.7665209279995</v>
       </c>
       <c r="S55">
         <v>16.49965297317861</v>
@@ -3741,16 +3741,16 @@
         <v>1203.50305467134</v>
       </c>
       <c r="L56">
-        <v>277.6797253066389</v>
+        <v>273.2088778473896</v>
       </c>
       <c r="M56">
-        <v>1226.283214173606</v>
+        <v>1204.259831696774</v>
       </c>
       <c r="N56">
         <v>681.1624920409977</v>
       </c>
       <c r="O56">
-        <v>405.7463347223734</v>
+        <v>948.8906167342222</v>
       </c>
       <c r="P56">
         <v>36.21586811983642</v>
@@ -3759,7 +3759,7 @@
         <v>140.8700369084754</v>
       </c>
       <c r="R56">
-        <v>430.5716518899994</v>
+        <v>420.5125125581926</v>
       </c>
       <c r="S56">
         <v>17.45484109298363</v>
@@ -3800,16 +3800,16 @@
         <v>1214.046494985746</v>
       </c>
       <c r="L57">
-        <v>290.6318105966264</v>
+        <v>296.343544319532</v>
       </c>
       <c r="M57">
-        <v>1373.053896022323</v>
+        <v>1383.974796361251</v>
       </c>
       <c r="N57">
         <v>697.6158992305635</v>
       </c>
       <c r="O57">
-        <v>415.7267304780551</v>
+        <v>966.5210942536822</v>
       </c>
       <c r="P57">
         <v>40.53474882627835</v>
@@ -3818,7 +3818,7 @@
         <v>164.0047033806179</v>
       </c>
       <c r="R57">
-        <v>437.391128392201</v>
+        <v>443.6471790303351</v>
       </c>
       <c r="S57">
         <v>19.07965614956348</v>
@@ -3859,16 +3859,16 @@
         <v>1223.77590743068</v>
       </c>
       <c r="L58">
-        <v>324.2260686732005</v>
+        <v>318.6877185271023</v>
       </c>
       <c r="M58">
-        <v>1234.959554406737</v>
+        <v>1237.24395722864</v>
       </c>
       <c r="N58">
         <v>718.5404573760344</v>
       </c>
       <c r="O58">
-        <v>425.9595281162495</v>
+        <v>983.5587324605177</v>
       </c>
       <c r="P58">
         <v>41.41967976161417</v>
@@ -3877,7 +3877,7 @@
         <v>186.3488775881881</v>
       </c>
       <c r="R58">
-        <v>469.0124808517558</v>
+        <v>465.9913532379058</v>
       </c>
       <c r="S58">
         <v>19.96786862465314</v>
@@ -3918,16 +3918,16 @@
         <v>1231.642883752134</v>
       </c>
       <c r="L59">
-        <v>335.9418287046361</v>
+        <v>339.1602249514683</v>
       </c>
       <c r="M59">
-        <v>1346.20403253084</v>
+        <v>1372.255007452439</v>
       </c>
       <c r="N59">
         <v>740.9007484616374</v>
       </c>
       <c r="O59">
-        <v>435.5409031681446</v>
+        <v>999.1084770053631</v>
       </c>
       <c r="P59">
         <v>40.38570587835434</v>
@@ -3936,7 +3936,7 @@
         <v>206.8213840125538</v>
       </c>
       <c r="R59">
-        <v>483.4750409697597</v>
+        <v>486.4638596622717</v>
       </c>
       <c r="S59">
         <v>19.94113730394288</v>
@@ -3977,16 +3977,16 @@
         <v>1239.94619255536</v>
       </c>
       <c r="L60">
-        <v>351.9703901351027</v>
+        <v>360.1306400249867</v>
       </c>
       <c r="M60">
-        <v>1355.48283472791</v>
+        <v>1361.23160246261</v>
       </c>
       <c r="N60">
         <v>754.8390468867054</v>
       </c>
       <c r="O60">
-        <v>445.8782277235514</v>
+        <v>1015.056946388514</v>
       </c>
       <c r="P60">
         <v>40.84192142278264</v>
@@ -3995,7 +3995,7 @@
         <v>227.7917990860723</v>
       </c>
       <c r="R60">
-        <v>497.0062797187522</v>
+        <v>507.4342747357903</v>
       </c>
       <c r="S60">
         <v>20.19574418296876</v>
@@ -4036,16 +4036,16 @@
         <v>1246.281048175741</v>
       </c>
       <c r="L61">
-        <v>378.7033369247682</v>
+        <v>379.1311724989172</v>
       </c>
       <c r="M61">
-        <v>1386.098706295822</v>
+        <v>1382.269780625788</v>
       </c>
       <c r="N61">
         <v>777.5142826946914</v>
       </c>
       <c r="O61">
-        <v>455.3170943165321</v>
+        <v>1029.330599874736</v>
       </c>
       <c r="P61">
         <v>39.03123254588987</v>
@@ -4054,7 +4054,7 @@
         <v>246.7923315600029</v>
       </c>
       <c r="R61">
-        <v>529.9466239443022</v>
+        <v>526.4348072097209</v>
       </c>
       <c r="S61">
         <v>19.41882387611805</v>
@@ -4095,7 +4095,7 @@
         <v>16.78214195519561</v>
       </c>
       <c r="L62">
-        <v>17.10844341368163</v>
+        <v>17.11444714087145</v>
       </c>
       <c r="M62">
         <v>16.57167457951122</v>
@@ -4104,7 +4104,7 @@
         <v>17.01474333157247</v>
       </c>
       <c r="O62">
-        <v>16.59968265933713</v>
+        <v>18.62643435655872</v>
       </c>
       <c r="P62">
         <v>16.91081658693724</v>
@@ -4113,7 +4113,7 @@
         <v>16.91094069717593</v>
       </c>
       <c r="R62">
-        <v>16.31641149322834</v>
+        <v>16.34208639342132</v>
       </c>
       <c r="S62">
         <v>17.04190088985236</v>
@@ -4154,7 +4154,7 @@
         <v>17.66217311063426</v>
       </c>
       <c r="L63">
-        <v>17.9594717279659</v>
+        <v>17.95032270020019</v>
       </c>
       <c r="M63">
         <v>17.38864692156954</v>
@@ -4163,7 +4163,7 @@
         <v>17.54225196006774</v>
       </c>
       <c r="O63">
-        <v>17.49154473954744</v>
+        <v>19.50784405631421</v>
       </c>
       <c r="P63">
         <v>17.91523193998572</v>
@@ -4172,7 +4172,7 @@
         <v>17.7899689529105</v>
       </c>
       <c r="R63">
-        <v>17.18421650889873</v>
+        <v>17.22111464915588</v>
       </c>
       <c r="S63">
         <v>17.63620695721325</v>
@@ -4213,7 +4213,7 @@
         <v>14.37738093726306</v>
       </c>
       <c r="L64">
-        <v>15.22082556796042</v>
+        <v>15.22873573159836</v>
       </c>
       <c r="M64">
         <v>13.98899370593799</v>
@@ -4222,7 +4222,7 @@
         <v>15.53028934816708</v>
       </c>
       <c r="O64">
-        <v>14.23359132258601</v>
+        <v>16.23507282466099</v>
       </c>
       <c r="P64">
         <v>14.26192083415031</v>
@@ -4231,7 +4231,7 @@
         <v>14.50411619251059</v>
       </c>
       <c r="R64">
-        <v>15.16510467702575</v>
+        <v>15.16106958586137</v>
       </c>
       <c r="S64">
         <v>15.73525621465426</v>
@@ -4272,7 +4272,7 @@
         <v>15.51777415889313</v>
       </c>
       <c r="L65">
-        <v>16.29520606540039</v>
+        <v>16.32621472480399</v>
       </c>
       <c r="M65">
         <v>15.20179796358365</v>
@@ -4281,7 +4281,7 @@
         <v>16.55013526868055</v>
       </c>
       <c r="O65">
-        <v>15.39264134147369</v>
+        <v>17.38136935744545</v>
       </c>
       <c r="P65">
         <v>16.93512408033495</v>
@@ -4290,7 +4290,7 @@
         <v>15.64130236955413</v>
       </c>
       <c r="R65">
-        <v>15.86386803244016</v>
+        <v>15.95544990047812</v>
       </c>
       <c r="S65">
         <v>16.49420485333006</v>
@@ -4331,7 +4331,7 @@
         <v>18.60611474396546</v>
       </c>
       <c r="L66">
-        <v>18.07441640871646</v>
+        <v>18.07764368400185</v>
       </c>
       <c r="M66">
         <v>18.11065651424346</v>
@@ -4340,7 +4340,7 @@
         <v>18.23180940213139</v>
       </c>
       <c r="O66">
-        <v>18.47820650883883</v>
+        <v>20.46466148671558</v>
       </c>
       <c r="P66">
         <v>19.57543429402306</v>
@@ -4349,7 +4349,7 @@
         <v>18.72671802722682</v>
       </c>
       <c r="R66">
-        <v>18.14694268967363</v>
+        <v>18.15786372347221</v>
       </c>
       <c r="S66">
         <v>18.02470351605817</v>
@@ -4390,7 +4390,7 @@
         <v>15.82569572628208</v>
       </c>
       <c r="L67">
-        <v>16.78545731372881</v>
+        <v>16.74570787850423</v>
       </c>
       <c r="M67">
         <v>15.54555772360919</v>
@@ -4399,7 +4399,7 @@
         <v>16.14863717393424</v>
       </c>
       <c r="O67">
-        <v>15.70966017311991</v>
+        <v>17.68982006652963</v>
       </c>
       <c r="P67">
         <v>15.21929564999648</v>
@@ -4408,7 +4408,7 @@
         <v>15.94537613543688</v>
       </c>
       <c r="R67">
-        <v>16.38078492376447</v>
+        <v>16.38882664487654</v>
       </c>
       <c r="S67">
         <v>16.55114372334094</v>
@@ -4449,7 +4449,7 @@
         <v>17.48046250434433</v>
       </c>
       <c r="L68">
-        <v>16.76564303628307</v>
+        <v>16.77378340993065</v>
       </c>
       <c r="M68">
         <v>17.21960324174313</v>
@@ -4458,7 +4458,7 @@
         <v>17.46708117581513</v>
       </c>
       <c r="O68">
-        <v>17.3628184278072</v>
+        <v>19.34128665165061</v>
       </c>
       <c r="P68">
         <v>18.19506782124708</v>
@@ -4467,7 +4467,7 @@
         <v>17.59720140972066</v>
       </c>
       <c r="R68">
-        <v>17.0576324276178</v>
+        <v>17.04742440699155</v>
       </c>
       <c r="S68">
         <v>17.51592272852103</v>
@@ -4508,7 +4508,7 @@
         <v>20.89677381691637</v>
       </c>
       <c r="L69">
-        <v>19.87600935282494</v>
+        <v>19.87250953880798</v>
       </c>
       <c r="M69">
         <v>20.48281371434826</v>
@@ -4517,7 +4517,7 @@
         <v>19.36370436467577</v>
       </c>
       <c r="O69">
-        <v>20.752333646624</v>
+        <v>22.74157721096281</v>
       </c>
       <c r="P69">
         <v>20.92378259664401</v>
@@ -4526,7 +4526,7 @@
         <v>21.01149893579414</v>
       </c>
       <c r="R69">
-        <v>19.99479562786787</v>
+        <v>19.97877947482138</v>
       </c>
       <c r="S69">
         <v>19.1892160920417</v>
@@ -4567,7 +4567,7 @@
         <v>22.58192855485389</v>
       </c>
       <c r="L70">
-        <v>20.62276882639396</v>
+        <v>20.69333149879936</v>
       </c>
       <c r="M70">
         <v>22.19391314637613</v>
@@ -4576,7 +4576,7 @@
         <v>19.91439229759671</v>
       </c>
       <c r="O70">
-        <v>22.40035034109253</v>
+        <v>24.40565755363546</v>
       </c>
       <c r="P70">
         <v>20.93498068902393</v>
@@ -4585,7 +4585,7 @@
         <v>22.69839305608578</v>
       </c>
       <c r="R70">
-        <v>20.43534410598976</v>
+        <v>20.50677204393287</v>
       </c>
       <c r="S70">
         <v>20.08814526994307</v>
@@ -4626,7 +4626,7 @@
         <v>22.50082565791799</v>
       </c>
       <c r="L71">
-        <v>20.62303205301522</v>
+        <v>20.53834656182002</v>
       </c>
       <c r="M71">
         <v>22.29651611840302</v>
@@ -4635,7 +4635,7 @@
         <v>19.63048471919883</v>
       </c>
       <c r="O71">
-        <v>22.27114833138014</v>
+        <v>24.30298221765347</v>
       </c>
       <c r="P71">
         <v>19.98208725708054</v>
@@ -4644,7 +4644,7 @@
         <v>22.62203284444839</v>
       </c>
       <c r="R71">
-        <v>20.22136294744974</v>
+        <v>20.18557502504421</v>
       </c>
       <c r="S71">
         <v>20.13319938702826</v>
@@ -4685,7 +4685,7 @@
         <v>22.72505463027017</v>
       </c>
       <c r="L72">
-        <v>21.02680021678103</v>
+        <v>21.01784550953149</v>
       </c>
       <c r="M72">
         <v>22.11539003751576</v>
@@ -4694,7 +4694,7 @@
         <v>20.00386206968625</v>
       </c>
       <c r="O72">
-        <v>22.44058565718547</v>
+        <v>24.50379455563737</v>
       </c>
       <c r="P72">
         <v>20.28545937973662</v>
@@ -4703,7 +4703,7 @@
         <v>22.85120372819503</v>
       </c>
       <c r="R72">
-        <v>20.77868923866174</v>
+        <v>20.76986370664235</v>
       </c>
       <c r="S72">
         <v>20.25453134051679</v>
@@ -4744,7 +4744,7 @@
         <v>21.66445086606808</v>
       </c>
       <c r="L73">
-        <v>19.65876491132473</v>
+        <v>19.73010123198004</v>
       </c>
       <c r="M73">
         <v>21.20192730309451</v>
@@ -4753,7 +4753,7 @@
         <v>19.25110477596052</v>
       </c>
       <c r="O73">
-        <v>21.3402882756142</v>
+        <v>23.42732695204434</v>
       </c>
       <c r="P73">
         <v>19.10621621407265</v>
@@ -4762,7 +4762,7 @@
         <v>21.7975216454677</v>
       </c>
       <c r="R73">
-        <v>20.89113165611587</v>
+        <v>20.90621226122064</v>
       </c>
       <c r="S73">
         <v>19.65751692973848</v>
@@ -4803,7 +4803,7 @@
         <v>180.6281371436667</v>
       </c>
       <c r="L74">
-        <v>35.53275618552673</v>
+        <v>36.66774904176933</v>
       </c>
       <c r="M74">
         <v>214.2740816027381</v>
@@ -4812,7 +4812,7 @@
         <v>54.62718331184978</v>
       </c>
       <c r="O74">
-        <v>43.75842842773066</v>
+        <v>33.60455890782424</v>
       </c>
       <c r="P74">
         <v>11.38406051123655</v>
@@ -4821,7 +4821,7 @@
         <v>11.15347656235814</v>
       </c>
       <c r="R74">
-        <v>28.36865696870442</v>
+        <v>28.35110436016512</v>
       </c>
       <c r="S74">
         <v>5.341967926962412</v>
@@ -4862,7 +4862,7 @@
         <v>184.6663026400083</v>
       </c>
       <c r="L75">
-        <v>44.33689088237994</v>
+        <v>42.45243430219544</v>
       </c>
       <c r="M75">
         <v>212.983907754279</v>
@@ -4871,7 +4871,7 @@
         <v>58.08727593322796</v>
       </c>
       <c r="O75">
-        <v>43.68185915603725</v>
+        <v>36.4935220999081</v>
       </c>
       <c r="P75">
         <v>11.12327841547765</v>
@@ -4880,7 +4880,7 @@
         <v>16.93816182278425</v>
       </c>
       <c r="R75">
-        <v>34.90692113530788</v>
+        <v>34.13578962059122</v>
       </c>
       <c r="S75">
         <v>5.425818431775537</v>
@@ -4921,7 +4921,7 @@
         <v>188.4982011369401</v>
       </c>
       <c r="L76">
-        <v>47.45423789146906</v>
+        <v>48.05675046634047</v>
       </c>
       <c r="M76">
         <v>223.1402902032866</v>
@@ -4930,7 +4930,7 @@
         <v>61.32340177895592</v>
       </c>
       <c r="O76">
-        <v>43.65909207143855</v>
+        <v>39.42187928112722</v>
       </c>
       <c r="P76">
         <v>11.04829381036523</v>
@@ -4939,7 +4939,7 @@
         <v>22.54247798692925</v>
       </c>
       <c r="R76">
-        <v>39.69488909220252</v>
+        <v>39.74010578473622</v>
       </c>
       <c r="S76">
         <v>5.537122816455598</v>
@@ -4980,7 +4980,7 @@
         <v>192.867499673145</v>
       </c>
       <c r="L77">
-        <v>54.59873635771568</v>
+        <v>54.22947093300276</v>
       </c>
       <c r="M77">
         <v>219.0749158814599</v>
@@ -4989,7 +4989,7 @@
         <v>61.02575910437928</v>
       </c>
       <c r="O77">
-        <v>43.719871384089</v>
+        <v>42.81601601160556</v>
       </c>
       <c r="P77">
         <v>11.61018385473535</v>
@@ -4998,7 +4998,7 @@
         <v>28.71519845359149</v>
       </c>
       <c r="R77">
-        <v>45.92969139051718</v>
+        <v>45.91282625139843</v>
       </c>
       <c r="S77">
         <v>5.625843642381598</v>
@@ -5039,7 +5039,7 @@
         <v>195.6971794204459</v>
       </c>
       <c r="L78">
-        <v>57.49566884679567</v>
+        <v>58.89752586876752</v>
       </c>
       <c r="M78">
         <v>226.1188108256238</v>
@@ -5048,7 +5048,7 @@
         <v>64.73068841049812</v>
       </c>
       <c r="O78">
-        <v>43.76985451890889</v>
+        <v>45.16162811194564</v>
       </c>
       <c r="P78">
         <v>10.24617253780025</v>
@@ -5057,7 +5057,7 @@
         <v>33.38325338935621</v>
       </c>
       <c r="R78">
-        <v>49.98892895158436</v>
+        <v>50.58088118716318</v>
       </c>
       <c r="S78">
         <v>5.268072562714314</v>
@@ -5098,7 +5098,7 @@
         <v>198.9745921950694</v>
       </c>
       <c r="L79">
-        <v>64.79534104149768</v>
+        <v>64.05018324344607</v>
       </c>
       <c r="M79">
         <v>214.2183668225738</v>
@@ -5107,7 +5107,7 @@
         <v>66.04863062083999</v>
       </c>
       <c r="O79">
-        <v>43.89784420549884</v>
+        <v>47.88038001536757</v>
       </c>
       <c r="P79">
         <v>10.38022725425499</v>
@@ -5116,7 +5116,7 @@
         <v>38.53591076403475</v>
       </c>
       <c r="R79">
-        <v>55.94093907116291</v>
+        <v>55.73353856184168</v>
       </c>
       <c r="S79">
         <v>5.095713946336543</v>
@@ -5157,7 +5157,7 @@
         <v>201.8338181300993</v>
       </c>
       <c r="L80">
-        <v>67.89217381177637</v>
+        <v>68.82216006459075</v>
       </c>
       <c r="M80">
         <v>222.8074713093995</v>
@@ -5166,7 +5166,7 @@
         <v>68.07082205429411</v>
       </c>
       <c r="O80">
-        <v>44.03359468270968</v>
+        <v>50.30015406807834</v>
       </c>
       <c r="P80">
         <v>9.868372106284056</v>
@@ -5175,7 +5175,7 @@
         <v>43.30788758517942</v>
       </c>
       <c r="R80">
-        <v>59.99880149235413</v>
+        <v>60.50551538298636</v>
       </c>
       <c r="S80">
         <v>4.960261611113662</v>
@@ -5216,7 +5216,7 @@
         <v>204.6279883196755</v>
       </c>
       <c r="L81">
-        <v>72.27878170433824</v>
+        <v>73.56599201480442</v>
       </c>
       <c r="M81">
         <v>225.3846550875173</v>
@@ -5225,7 +5225,7 @@
         <v>67.96979145682549</v>
       </c>
       <c r="O81">
-        <v>44.19268984767571</v>
+        <v>52.68394698308816</v>
       </c>
       <c r="P81">
         <v>9.692928053565659</v>
@@ -5234,7 +5234,7 @@
         <v>48.05171953539303</v>
       </c>
       <c r="R81">
-        <v>64.37706820342183</v>
+        <v>65.24934733319998</v>
       </c>
       <c r="S81">
         <v>4.785184360552173</v>
@@ -5275,7 +5275,7 @@
         <v>209.4345695187794</v>
       </c>
       <c r="L82">
-        <v>77.7737328886371</v>
+        <v>80.35788284302227</v>
       </c>
       <c r="M82">
         <v>233.1405168676925</v>
@@ -5284,7 +5284,7 @@
         <v>71.80689505383711</v>
       </c>
       <c r="O82">
-        <v>44.75957071282154</v>
+        <v>56.81900895114972</v>
       </c>
       <c r="P82">
         <v>11.56529278760643</v>
@@ -5293,7 +5293,7 @@
         <v>54.8436103636109</v>
       </c>
       <c r="R82">
-        <v>71.03232144629101</v>
+        <v>72.04123816141787</v>
       </c>
       <c r="S82">
         <v>5.316546890558328</v>
@@ -5334,7 +5334,7 @@
         <v>216.6680698101138</v>
       </c>
       <c r="L83">
-        <v>88.92003220024098</v>
+        <v>89.61238501550673</v>
       </c>
       <c r="M83">
         <v>248.0263386627053</v>
@@ -5343,7 +5343,7 @@
         <v>77.39959557975475</v>
       </c>
       <c r="O83">
-        <v>46.0875648692861</v>
+        <v>63.29624412094641</v>
       </c>
       <c r="P83">
         <v>14.5414571680573</v>
@@ -5352,7 +5352,7 @@
         <v>64.09811253609539</v>
       </c>
       <c r="R83">
-        <v>80.62377479718928</v>
+        <v>81.29574033390234</v>
       </c>
       <c r="S83">
         <v>6.59250773818743</v>
@@ -5393,7 +5393,7 @@
         <v>223.279208473255</v>
       </c>
       <c r="L84">
-        <v>98.10352345170193</v>
+        <v>98.28324183671543</v>
       </c>
       <c r="M84">
         <v>236.4371665224166</v>
@@ -5402,7 +5402,7 @@
         <v>83.47704367844891</v>
       </c>
       <c r="O84">
-        <v>47.621844503488</v>
+        <v>69.39425217208866</v>
       </c>
       <c r="P84">
         <v>15.19557489243575</v>
@@ -5411,7 +5411,7 @@
         <v>72.76896935730416</v>
       </c>
       <c r="R84">
-        <v>89.7155019147658</v>
+        <v>89.9665971551111</v>
       </c>
       <c r="S84">
         <v>7.199353666196877</v>
@@ -5452,7 +5452,7 @@
         <v>231.7440209148139</v>
       </c>
       <c r="L85">
-        <v>106.2408757834081</v>
+        <v>108.851216305349</v>
       </c>
       <c r="M85">
         <v>256.973849473574</v>
@@ -5461,7 +5461,7 @@
         <v>89.57435635460517</v>
       </c>
       <c r="O85">
-        <v>50.10952157915923</v>
+        <v>77.37324861344946</v>
       </c>
       <c r="P85">
         <v>17.76338919503952</v>
@@ -5470,7 +5470,7 @@
         <v>83.33694382593774</v>
       </c>
       <c r="R85">
-        <v>100.1027098560539</v>
+        <v>100.5345716237447</v>
       </c>
       <c r="S85">
         <v>8.387298458071591</v>
@@ -5511,7 +5511,7 @@
         <v>4.713460384036707</v>
       </c>
       <c r="L86">
-        <v>3.123664802503818</v>
+        <v>3.167164779604897</v>
       </c>
       <c r="M86">
         <v>4.599462333003186</v>
@@ -5520,7 +5520,7 @@
         <v>5.341464245308501</v>
       </c>
       <c r="O86">
-        <v>4.314672864520659</v>
+        <v>2.322467782620476</v>
       </c>
       <c r="P86">
         <v>5.512823080561064</v>
@@ -5529,7 +5529,7 @@
         <v>5.502289484456631</v>
       </c>
       <c r="R86">
-        <v>3.045191741264441</v>
+        <v>3.069380910745354</v>
       </c>
       <c r="S86">
         <v>5.177112879683605</v>
@@ -5570,7 +5570,7 @@
         <v>4.790972075001171</v>
       </c>
       <c r="L87">
-        <v>2.948382223389602</v>
+        <v>3.000358720696724</v>
       </c>
       <c r="M87">
         <v>4.486544631941098</v>
@@ -5579,7 +5579,7 @@
         <v>5.407494217925759</v>
       </c>
       <c r="O87">
-        <v>4.297807270057266</v>
+        <v>2.309763171371638</v>
       </c>
       <c r="P87">
         <v>5.132757906081364</v>
@@ -5588,7 +5588,7 @@
         <v>5.611842685623573</v>
       </c>
       <c r="R87">
-        <v>3.329430476847712</v>
+        <v>3.191697151881465</v>
       </c>
       <c r="S87">
         <v>5.940958372408251</v>
@@ -5629,7 +5629,7 @@
         <v>4.686717333381376</v>
       </c>
       <c r="L88">
-        <v>3.032930778607022</v>
+        <v>2.937399676134602</v>
       </c>
       <c r="M88">
         <v>4.771223613176</v>
@@ -5638,7 +5638,7 @@
         <v>5.386055095205766</v>
       </c>
       <c r="O88">
-        <v>4.284626085711174</v>
+        <v>2.265090973894816</v>
       </c>
       <c r="P88">
         <v>5.050303613759088</v>
@@ -5647,7 +5647,7 @@
         <v>5.481596018398434</v>
       </c>
       <c r="R88">
-        <v>1.82169192170732</v>
+        <v>1.848063405946064</v>
       </c>
       <c r="S88">
         <v>5.314771099902661</v>
@@ -5688,7 +5688,7 @@
         <v>4.948447087562418</v>
       </c>
       <c r="L89">
-        <v>3.343547626621078</v>
+        <v>3.324467108805568</v>
       </c>
       <c r="M89">
         <v>4.397363181004817</v>
@@ -5697,7 +5697,7 @@
         <v>5.619215542150225</v>
       </c>
       <c r="O89">
-        <v>4.283917408797487</v>
+        <v>2.298781350766299</v>
       </c>
       <c r="P89">
         <v>5.496227551620405</v>
@@ -5706,7 +5706,7 @@
         <v>5.825632033386229</v>
       </c>
       <c r="R89">
-        <v>2.013095618018083</v>
+        <v>2.122402398478987</v>
       </c>
       <c r="S89">
         <v>6.010570319787956</v>
@@ -5747,7 +5747,7 @@
         <v>4.241872061665477</v>
       </c>
       <c r="L90">
-        <v>2.27987540072447</v>
+        <v>2.331686924613471</v>
       </c>
       <c r="M90">
         <v>4.508108909754121</v>
@@ -5756,7 +5756,7 @@
         <v>5.183787438996109</v>
       </c>
       <c r="O90">
-        <v>4.278634952897497</v>
+        <v>2.161625219333701</v>
       </c>
       <c r="P90">
         <v>4.396302537071656</v>
@@ -5765,7 +5765,7 @@
         <v>4.915473681759972</v>
       </c>
       <c r="R90">
-        <v>1.438527168488165</v>
+        <v>1.444037816475493</v>
       </c>
       <c r="S90">
         <v>5.183406168979106</v>
@@ -5806,7 +5806,7 @@
         <v>4.075850219306989</v>
       </c>
       <c r="L91">
-        <v>2.307089773966116</v>
+        <v>2.343706387371544</v>
       </c>
       <c r="M91">
         <v>4.355641264054554</v>
@@ -5815,7 +5815,7 @@
         <v>5.130227360185765</v>
       </c>
       <c r="O91">
-        <v>4.288180278802593</v>
+        <v>2.139777664767813</v>
       </c>
       <c r="P91">
         <v>4.728177846295027</v>
@@ -5824,7 +5824,7 @@
         <v>4.699624369249633</v>
       </c>
       <c r="R91">
-        <v>1.296489383690219</v>
+        <v>1.308117223029361</v>
       </c>
       <c r="S91">
         <v>5.204956223067518</v>
@@ -5865,7 +5865,7 @@
         <v>3.703710079375747</v>
       </c>
       <c r="L92">
-        <v>1.933478137225402</v>
+        <v>1.962616253146183</v>
       </c>
       <c r="M92">
         <v>3.910618696480379</v>
@@ -5874,7 +5874,7 @@
         <v>4.773528384681438</v>
       </c>
       <c r="O92">
-        <v>4.311963473171212</v>
+        <v>2.120422408931472</v>
       </c>
       <c r="P92">
         <v>4.303464191550757</v>
@@ -5883,7 +5883,7 @@
         <v>4.172915745182592</v>
       </c>
       <c r="R92">
-        <v>1.021431464778483</v>
+        <v>1.009060269592577</v>
       </c>
       <c r="S92">
         <v>4.769722236101714</v>
@@ -5924,7 +5924,7 @@
         <v>3.576614160817996</v>
       </c>
       <c r="L93">
-        <v>2.205201691667216</v>
+        <v>2.261764663484909</v>
       </c>
       <c r="M93">
         <v>3.992682325044561</v>
@@ -5933,7 +5933,7 @@
         <v>4.741314000173661</v>
       </c>
       <c r="O93">
-        <v>4.327780646551504</v>
+        <v>2.123018243510516</v>
       </c>
       <c r="P93">
         <v>4.356318299528287</v>
@@ -5942,7 +5942,7 @@
         <v>3.991374279559115</v>
       </c>
       <c r="R93">
-        <v>3.259719318934025</v>
+        <v>3.18082801845869</v>
       </c>
       <c r="S93">
         <v>4.465389495723371</v>
@@ -5983,7 +5983,7 @@
         <v>4.50806844364122</v>
       </c>
       <c r="L94">
-        <v>2.020389282855091</v>
+        <v>2.124123318683707</v>
       </c>
       <c r="M94">
         <v>4.548944309391396</v>
@@ -5992,7 +5992,7 @@
         <v>5.385993707478743</v>
       </c>
       <c r="O94">
-        <v>4.300342440249622</v>
+        <v>2.172096912411476</v>
       </c>
       <c r="P94">
         <v>5.808613069222283</v>
@@ -6001,7 +6001,7 @@
         <v>5.316506664540172</v>
       </c>
       <c r="R94">
-        <v>2.279813721627711</v>
+        <v>2.311460527802423</v>
       </c>
       <c r="S94">
         <v>4.965222037935574</v>
@@ -6042,7 +6042,7 @@
         <v>6.768470862002949</v>
       </c>
       <c r="L95">
-        <v>2.096551023793951</v>
+        <v>2.205846956909175</v>
       </c>
       <c r="M95">
         <v>5.591894100467138</v>
@@ -6051,7 +6051,7 @@
         <v>6.678956673984143</v>
       </c>
       <c r="O95">
-        <v>4.428529328499617</v>
+        <v>2.701836124136054</v>
       </c>
       <c r="P95">
         <v>7.647391917453333</v>
@@ -6060,7 +6060,7 @@
         <v>7.953207261357237</v>
       </c>
       <c r="R95">
-        <v>1.065652357244822</v>
+        <v>1.115695686732081</v>
       </c>
       <c r="S95">
         <v>6.259075186003367</v>
@@ -6101,7 +6101,7 @@
         <v>7.990533932814115</v>
       </c>
       <c r="L96">
-        <v>2.528311886034185</v>
+        <v>2.563900542223836</v>
       </c>
       <c r="M96">
         <v>6.271150635486489</v>
@@ -6110,7 +6110,7 @@
         <v>7.237734398692501</v>
       </c>
       <c r="O96">
-        <v>4.636252310453265</v>
+        <v>3.140547281017766</v>
       </c>
       <c r="P96">
         <v>7.518744328662224</v>
@@ -6119,7 +6119,7 @@
         <v>9.244774997475208</v>
       </c>
       <c r="R96">
-        <v>0.976463808556753</v>
+        <v>1.006992196645092</v>
       </c>
       <c r="S96">
         <v>7.128925257706974</v>
@@ -6160,7 +6160,7 @@
         <v>10.09254552043759</v>
       </c>
       <c r="L97">
-        <v>3.766964901694023</v>
+        <v>3.774482296828511</v>
       </c>
       <c r="M97">
         <v>7.111985998385481</v>
@@ -6169,7 +6169,7 @@
         <v>8.327733987657934</v>
       </c>
       <c r="O97">
-        <v>5.379501086532826</v>
+        <v>4.148003154359824</v>
       </c>
       <c r="P97">
         <v>9.049470867720945</v>
@@ -6178,7 +6178,7 @@
         <v>11.38871768359558</v>
       </c>
       <c r="R97">
-        <v>1.644972759289026</v>
+        <v>1.750893485491843</v>
       </c>
       <c r="S97">
         <v>7.816092893736995</v>

</xml_diff>